<commit_message>
fixed #198 FlixelRL-198 武器パラメータの調整
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -235,43 +235,43 @@
     <t>Weapon</t>
   </si>
   <si>
-    <t>こん棒</t>
+    <t>竹刀</t>
   </si>
   <si>
     <t>WEAPON2</t>
   </si>
   <si>
-    <t>金の剣</t>
+    <t>木刀</t>
   </si>
   <si>
     <t>WEAPON3</t>
   </si>
   <si>
-    <t>銅の剣</t>
+    <t>ダガー</t>
   </si>
   <si>
     <t>WEAPON4</t>
   </si>
   <si>
-    <t>鉄の斧</t>
+    <t>レイピア</t>
   </si>
   <si>
     <t>WEAPON5</t>
   </si>
   <si>
-    <t>ドラゴンキラー</t>
+    <t>三日月刀</t>
   </si>
   <si>
     <t>WEAPON6</t>
   </si>
   <si>
-    <t>はぐれメタルの剣</t>
+    <t>妖刀ムラマサ</t>
   </si>
   <si>
     <t>WEAPON7</t>
   </si>
   <si>
-    <t>正義のソロバン</t>
+    <t>ライトセーバー</t>
   </si>
   <si>
     <t>WEAPON8</t>
@@ -322,43 +322,43 @@
     <t>Armor</t>
   </si>
   <si>
-    <t>皮のよろい</t>
+    <t>ローブ</t>
   </si>
   <si>
     <t>ARMOR2</t>
   </si>
   <si>
-    <t>青銅のよろい</t>
+    <t>毛皮の鎧</t>
   </si>
   <si>
     <t>ARMOR3</t>
   </si>
   <si>
-    <t>うろこのよろい</t>
+    <t>鎖かたびら</t>
   </si>
   <si>
     <t>ARMOR4</t>
   </si>
   <si>
-    <t>みかがみのよろい</t>
+    <t>エルフの鎧</t>
   </si>
   <si>
     <t>ARMOR5</t>
   </si>
   <si>
-    <t>鋼鉄のよろい</t>
+    <t>鋼鉄の鎧</t>
   </si>
   <si>
     <t>ARMOR6</t>
   </si>
   <si>
-    <t>ドラゴンアーマー</t>
+    <t>シルバーアーマー</t>
   </si>
   <si>
     <t>ARMOR7</t>
   </si>
   <si>
-    <t>はぐれメタルの鎧</t>
+    <t>プラチナメイル</t>
   </si>
   <si>
     <t>ARMOR8</t>
@@ -2808,7 +2808,7 @@
         <v>73</v>
       </c>
       <c r="D3" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -2827,7 +2827,7 @@
         <v>75</v>
       </c>
       <c r="D4" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2846,7 +2846,7 @@
         <v>77</v>
       </c>
       <c r="D5" s="4">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2865,7 +2865,7 @@
         <v>79</v>
       </c>
       <c r="D6" s="4">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2884,7 +2884,7 @@
         <v>81</v>
       </c>
       <c r="D7" s="4">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -2903,7 +2903,7 @@
         <v>83</v>
       </c>
       <c r="D8" s="4">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -2922,7 +2922,7 @@
         <v>85</v>
       </c>
       <c r="D9" s="4">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -3210,7 +3210,7 @@
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -3294,7 +3294,7 @@
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>

</xml_diff>

<commit_message>
fixed #258 FlixelRL-258 最大HPを上昇する薬
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="329">
   <si>
     <t>id</t>
   </si>
@@ -28,15 +28,6 @@
     <t>hp</t>
   </si>
   <si>
-    <t>hp2</t>
-  </si>
-  <si>
-    <t>mp</t>
-  </si>
-  <si>
-    <t>mp2</t>
-  </si>
-  <si>
     <t>food</t>
   </si>
   <si>
@@ -55,6 +46,9 @@
     <t>extra</t>
   </si>
   <si>
+    <t>extval</t>
+  </si>
+  <si>
     <t>detail</t>
   </si>
   <si>
@@ -287,6 +281,111 @@
   </si>
   <si>
     <t>飲むとHPが160回復します</t>
+  </si>
+  <si>
+    <t>PORTION17</t>
+  </si>
+  <si>
+    <t>命の薬</t>
+  </si>
+  <si>
+    <t>hpmax</t>
+  </si>
+  <si>
+    <t>最大HPが上昇します</t>
+  </si>
+  <si>
+    <t>PORTION18</t>
+  </si>
+  <si>
+    <t>薬18</t>
+  </si>
+  <si>
+    <t>飲むとHPが1回復します</t>
+  </si>
+  <si>
+    <t>PORTION19</t>
+  </si>
+  <si>
+    <t>薬19</t>
+  </si>
+  <si>
+    <t>PORTION20</t>
+  </si>
+  <si>
+    <t>薬20</t>
+  </si>
+  <si>
+    <t>PORTION21</t>
+  </si>
+  <si>
+    <t>薬21</t>
+  </si>
+  <si>
+    <t>PORTION22</t>
+  </si>
+  <si>
+    <t>薬22</t>
+  </si>
+  <si>
+    <t>PORTION23</t>
+  </si>
+  <si>
+    <t>薬23</t>
+  </si>
+  <si>
+    <t>PORTION24</t>
+  </si>
+  <si>
+    <t>薬24</t>
+  </si>
+  <si>
+    <t>PORTION25</t>
+  </si>
+  <si>
+    <t>薬25</t>
+  </si>
+  <si>
+    <t>PORTION26</t>
+  </si>
+  <si>
+    <t>薬26</t>
+  </si>
+  <si>
+    <t>PORTION27</t>
+  </si>
+  <si>
+    <t>薬27</t>
+  </si>
+  <si>
+    <t>PORTION28</t>
+  </si>
+  <si>
+    <t>薬28</t>
+  </si>
+  <si>
+    <t>PORTION29</t>
+  </si>
+  <si>
+    <t>薬29</t>
+  </si>
+  <si>
+    <t>PORTION30</t>
+  </si>
+  <si>
+    <t>薬30</t>
+  </si>
+  <si>
+    <t>PORTION31</t>
+  </si>
+  <si>
+    <t>薬31</t>
+  </si>
+  <si>
+    <t>PORTION32</t>
+  </si>
+  <si>
+    <t>薬32</t>
   </si>
   <si>
     <t>SCROLL1</t>
@@ -2431,7 +2530,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2441,17 +2540,15 @@
     <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="1" customWidth="1"/>
-    <col min="5" max="5" width="3.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="2.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="3.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.75" style="1" customWidth="1"/>
     <col min="8" max="8" width="4.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="4.75" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.75" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.875" style="1" customWidth="1"/>
     <col min="11" max="11" width="4.75" style="1" customWidth="1"/>
-    <col min="12" max="12" width="5.75" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.75" style="1" customWidth="1"/>
-    <col min="14" max="14" width="31.2812" style="1" customWidth="1"/>
-    <col min="15" max="256" width="9" style="1" customWidth="1"/>
+    <col min="12" max="12" width="31.2812" style="1" customWidth="1"/>
+    <col min="13" max="256" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -2491,1502 +2588,1448 @@
       <c r="L1" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s" s="2">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L2" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="M2" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="N2" t="s" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="D3" s="5"/>
+      <c r="E3" s="4">
+        <v>50</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
+      <c r="L3" t="s" s="4">
         <v>17</v>
-      </c>
-      <c r="C3" t="s" s="4">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4">
-        <v>50</v>
-      </c>
-      <c r="I3" s="5">
-        <v>2</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" t="s" s="4">
-        <v>19</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4">
+        <v>100</v>
+      </c>
+      <c r="F4" s="5">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" t="s" s="4">
         <v>20</v>
-      </c>
-      <c r="B4" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s" s="4">
-        <v>21</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4">
-        <v>100</v>
-      </c>
-      <c r="I4" s="5">
-        <v>4</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" t="s" s="4">
-        <v>22</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5">
+        <v>25</v>
+      </c>
+      <c r="F5" s="5">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" t="s" s="4">
         <v>23</v>
-      </c>
-      <c r="B5" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s" s="4">
-        <v>24</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5">
-        <v>25</v>
-      </c>
-      <c r="I5" s="5">
-        <v>8</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" t="s" s="4">
-        <v>25</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>25</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5">
+        <v>25</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6"/>
+      <c r="L6" t="s" s="4">
         <v>26</v>
-      </c>
-      <c r="B6" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s" s="4">
-        <v>27</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5">
-        <v>25</v>
-      </c>
-      <c r="I6" s="5">
-        <v>2</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" t="s" s="4">
-        <v>28</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>2</v>
+      </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="5">
-        <v>1</v>
-      </c>
-      <c r="I7" s="5">
-        <v>2</v>
-      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" t="s" s="4">
-        <v>30</v>
+      <c r="K7" s="6"/>
+      <c r="L7" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2</v>
+      </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="5">
-        <v>1</v>
-      </c>
-      <c r="I8" s="5">
-        <v>2</v>
-      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" t="s" s="4">
-        <v>30</v>
+      <c r="K8" s="6"/>
+      <c r="L8" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>2</v>
+      </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="5">
-        <v>1</v>
-      </c>
-      <c r="I9" s="5">
-        <v>2</v>
-      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" t="s" s="4">
-        <v>30</v>
+      <c r="K9" s="6"/>
+      <c r="L9" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>2</v>
+      </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="5">
-        <v>1</v>
-      </c>
-      <c r="I10" s="5">
-        <v>2</v>
-      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" t="s" s="4">
-        <v>30</v>
+      <c r="K10" s="6"/>
+      <c r="L10" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2</v>
+      </c>
       <c r="G11" s="5"/>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-      <c r="I11" s="5">
-        <v>2</v>
-      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" t="s" s="4">
-        <v>30</v>
+      <c r="K11" s="6"/>
+      <c r="L11" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2</v>
+      </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="5">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5">
-        <v>2</v>
-      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" t="s" s="4">
-        <v>30</v>
+      <c r="K12" s="6"/>
+      <c r="L12" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2</v>
+      </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="5">
-        <v>1</v>
-      </c>
-      <c r="I13" s="5">
-        <v>2</v>
-      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" t="s" s="4">
-        <v>30</v>
+      <c r="K13" s="6"/>
+      <c r="L13" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
+        <v>2</v>
+      </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="5">
-        <v>1</v>
-      </c>
-      <c r="I14" s="5">
-        <v>2</v>
-      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" t="s" s="4">
-        <v>30</v>
+      <c r="K14" s="6"/>
+      <c r="L14" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2</v>
+      </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="5">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5">
-        <v>2</v>
-      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" t="s" s="4">
-        <v>30</v>
+      <c r="K15" s="6"/>
+      <c r="L15" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5">
+        <v>2</v>
+      </c>
       <c r="G16" s="5"/>
-      <c r="H16" s="5">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5">
-        <v>2</v>
-      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" t="s" s="4">
-        <v>30</v>
+      <c r="K16" s="6"/>
+      <c r="L16" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5">
+        <v>2</v>
+      </c>
       <c r="G17" s="5"/>
-      <c r="H17" s="5">
-        <v>1</v>
-      </c>
-      <c r="I17" s="5">
-        <v>2</v>
-      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" t="s" s="4">
-        <v>30</v>
+      <c r="K17" s="6"/>
+      <c r="L17" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <v>2</v>
+      </c>
       <c r="G18" s="5"/>
-      <c r="H18" s="5">
-        <v>1</v>
-      </c>
-      <c r="I18" s="5">
-        <v>2</v>
-      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" t="s" s="4">
-        <v>30</v>
+      <c r="K18" s="6"/>
+      <c r="L18" t="s" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s" s="4">
         <v>42</v>
-      </c>
-      <c r="B19" t="s" s="4">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s" s="4">
-        <v>44</v>
       </c>
       <c r="D19" s="4">
         <v>10</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="5">
+        <v>10</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5">
-        <v>10</v>
-      </c>
+      <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" t="s" s="4">
-        <v>45</v>
+      <c r="K19" s="6"/>
+      <c r="L19" t="s" s="4">
+        <v>43</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D20" s="4">
         <v>20</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="5">
+        <v>10</v>
+      </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="5">
-        <v>10</v>
-      </c>
+      <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" t="s" s="4">
-        <v>48</v>
+      <c r="K20" s="6"/>
+      <c r="L20" t="s" s="4">
+        <v>46</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D21" s="4">
         <v>30</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="5">
+        <v>10</v>
+      </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="5">
-        <v>10</v>
-      </c>
+      <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" t="s" s="4">
-        <v>51</v>
+      <c r="K21" s="6"/>
+      <c r="L21" t="s" s="4">
+        <v>49</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D22" s="4">
         <v>40</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="5">
+        <v>10</v>
+      </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="5">
-        <v>10</v>
-      </c>
+      <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" t="s" s="4">
-        <v>54</v>
+      <c r="K22" s="6"/>
+      <c r="L22" t="s" s="4">
+        <v>52</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D23" s="4">
         <v>50</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="5">
+        <v>10</v>
+      </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="5">
-        <v>10</v>
-      </c>
+      <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" t="s" s="4">
-        <v>57</v>
+      <c r="K23" s="6"/>
+      <c r="L23" t="s" s="4">
+        <v>55</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s" s="4">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D24" s="4">
         <v>60</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="5">
+        <v>10</v>
+      </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="5">
-        <v>10</v>
-      </c>
+      <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" t="s" s="4">
-        <v>60</v>
+      <c r="K24" s="6"/>
+      <c r="L24" t="s" s="4">
+        <v>58</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s" s="4">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D25" s="4">
         <v>70</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="5">
+        <v>10</v>
+      </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="5">
-        <v>10</v>
-      </c>
+      <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" t="s" s="4">
-        <v>63</v>
+      <c r="K25" s="6"/>
+      <c r="L25" t="s" s="4">
+        <v>61</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D26" s="4">
         <v>80</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="5">
+        <v>10</v>
+      </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="5">
-        <v>10</v>
-      </c>
+      <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" t="s" s="4">
-        <v>66</v>
+      <c r="K26" s="6"/>
+      <c r="L26" t="s" s="4">
+        <v>64</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D27" s="4">
         <v>90</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="5">
+        <v>10</v>
+      </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="5">
-        <v>10</v>
-      </c>
+      <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" t="s" s="4">
-        <v>69</v>
+      <c r="K27" s="6"/>
+      <c r="L27" t="s" s="4">
+        <v>67</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D28" s="4">
         <v>100</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="5">
+        <v>10</v>
+      </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="5">
-        <v>10</v>
-      </c>
+      <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" t="s" s="4">
-        <v>72</v>
+      <c r="K28" s="6"/>
+      <c r="L28" t="s" s="4">
+        <v>70</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D29" s="4">
         <v>110</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="E29" s="5">
+        <v>10</v>
+      </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="5">
-        <v>10</v>
-      </c>
+      <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" t="s" s="4">
-        <v>75</v>
+      <c r="K29" s="6"/>
+      <c r="L29" t="s" s="4">
+        <v>73</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s" s="4">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D30" s="4">
         <v>120</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5">
+        <v>10</v>
+      </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="5">
-        <v>10</v>
-      </c>
+      <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" t="s" s="4">
-        <v>78</v>
+      <c r="K30" s="6"/>
+      <c r="L30" t="s" s="4">
+        <v>76</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D31" s="4">
         <v>130</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5">
+        <v>10</v>
+      </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="5">
-        <v>10</v>
-      </c>
+      <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" t="s" s="4">
-        <v>81</v>
+      <c r="K31" s="6"/>
+      <c r="L31" t="s" s="4">
+        <v>79</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D32" s="4">
         <v>140</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="5">
+        <v>10</v>
+      </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="5">
-        <v>10</v>
-      </c>
+      <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" t="s" s="4">
-        <v>84</v>
+      <c r="K32" s="6"/>
+      <c r="L32" t="s" s="4">
+        <v>82</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D33" s="4">
         <v>150</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5">
+        <v>10</v>
+      </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
-      <c r="H33" s="5">
-        <v>10</v>
-      </c>
+      <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" t="s" s="4">
-        <v>87</v>
+      <c r="K33" s="6"/>
+      <c r="L33" t="s" s="4">
+        <v>85</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D34" s="4">
         <v>160</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="5">
+        <v>10</v>
+      </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
-      <c r="H34" s="5">
-        <v>10</v>
-      </c>
+      <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" t="s" s="4">
-        <v>90</v>
+      <c r="K34" s="6"/>
+      <c r="L34" t="s" s="4">
+        <v>88</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
+        <v>89</v>
+      </c>
+      <c r="B35" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="C35" t="s" s="4">
+        <v>90</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="5">
+        <v>10</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" t="s" s="4">
         <v>91</v>
       </c>
-      <c r="B35" t="s" s="4">
+      <c r="K35" s="5">
+        <v>3</v>
+      </c>
+      <c r="L35" t="s" s="4">
         <v>92</v>
-      </c>
-      <c r="C35" t="s" s="4">
-        <v>93</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5">
-        <v>10</v>
-      </c>
-      <c r="J35" t="s" s="4">
-        <v>94</v>
-      </c>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" t="s" s="4">
-        <v>95</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>97</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5">
+        <v>10</v>
+      </c>
       <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
+      <c r="G36" s="6"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="5">
-        <v>30</v>
-      </c>
-      <c r="J36" t="s" s="4">
-        <v>94</v>
-      </c>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" t="s" s="4">
-        <v>98</v>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="6"/>
+      <c r="L36" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>100</v>
-      </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+      <c r="E37" s="5">
+        <v>10</v>
+      </c>
       <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="6"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="5">
-        <v>100</v>
-      </c>
-      <c r="J37" t="s" s="4">
-        <v>94</v>
-      </c>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" t="s" s="4">
-        <v>101</v>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="6"/>
+      <c r="L37" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>103</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5">
+        <v>10</v>
+      </c>
       <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="G38" s="6"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" t="s" s="4">
-        <v>104</v>
+      <c r="J38" s="5"/>
+      <c r="K38" s="6"/>
+      <c r="L38" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>106</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
+      </c>
+      <c r="E39" s="5">
+        <v>10</v>
+      </c>
       <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="G39" s="6"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" t="s" s="4">
-        <v>104</v>
+      <c r="J39" s="5"/>
+      <c r="K39" s="6"/>
+      <c r="L39" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>108</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+      <c r="E40" s="5">
+        <v>10</v>
+      </c>
       <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
+      <c r="G40" s="6"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" t="s" s="4">
-        <v>104</v>
+      <c r="J40" s="5"/>
+      <c r="K40" s="6"/>
+      <c r="L40" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>110</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1</v>
+      </c>
+      <c r="E41" s="5">
+        <v>10</v>
+      </c>
       <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
+      <c r="G41" s="6"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" t="s" s="4">
-        <v>104</v>
+      <c r="K41" s="6"/>
+      <c r="L41" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>112</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="5"/>
+        <v>107</v>
+      </c>
+      <c r="D42" s="4">
+        <v>1</v>
+      </c>
+      <c r="E42" s="5">
+        <v>10</v>
+      </c>
       <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="G42" s="6"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" t="s" s="4">
-        <v>104</v>
+      <c r="K42" s="6"/>
+      <c r="L42" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>114</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="5"/>
+        <v>109</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1</v>
+      </c>
+      <c r="E43" s="5">
+        <v>10</v>
+      </c>
       <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="G43" s="6"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" t="s" s="4">
-        <v>104</v>
+      <c r="K43" s="6"/>
+      <c r="L43" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>116</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="5"/>
+        <v>111</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="5">
+        <v>10</v>
+      </c>
       <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="G44" s="6"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" t="s" s="4">
-        <v>104</v>
+      <c r="K44" s="6"/>
+      <c r="L44" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>118</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="5"/>
+        <v>113</v>
+      </c>
+      <c r="D45" s="4">
+        <v>1</v>
+      </c>
+      <c r="E45" s="5">
+        <v>10</v>
+      </c>
       <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="G45" s="6"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" t="s" s="4">
-        <v>104</v>
+      <c r="K45" s="6"/>
+      <c r="L45" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>120</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="5"/>
+        <v>115</v>
+      </c>
+      <c r="D46" s="4">
+        <v>1</v>
+      </c>
+      <c r="E46" s="5">
+        <v>10</v>
+      </c>
       <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="G46" s="6"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" t="s" s="4">
-        <v>104</v>
+      <c r="K46" s="6"/>
+      <c r="L46" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>122</v>
-      </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="5"/>
+        <v>117</v>
+      </c>
+      <c r="D47" s="4">
+        <v>1</v>
+      </c>
+      <c r="E47" s="5">
+        <v>10</v>
+      </c>
       <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="G47" s="6"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" t="s" s="4">
-        <v>104</v>
+      <c r="K47" s="6"/>
+      <c r="L47" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>124</v>
-      </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="5"/>
+        <v>119</v>
+      </c>
+      <c r="D48" s="4">
+        <v>1</v>
+      </c>
+      <c r="E48" s="5">
+        <v>10</v>
+      </c>
       <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="G48" s="6"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
-      <c r="N48" t="s" s="4">
-        <v>104</v>
+      <c r="K48" s="6"/>
+      <c r="L48" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>126</v>
-      </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="5"/>
+        <v>121</v>
+      </c>
+      <c r="D49" s="4">
+        <v>1</v>
+      </c>
+      <c r="E49" s="5">
+        <v>10</v>
+      </c>
       <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="G49" s="6"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" t="s" s="4">
-        <v>104</v>
+      <c r="K49" s="6"/>
+      <c r="L49" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>128</v>
-      </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="5"/>
+        <v>123</v>
+      </c>
+      <c r="D50" s="4">
+        <v>1</v>
+      </c>
+      <c r="E50" s="5">
+        <v>10</v>
+      </c>
       <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="6"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" t="s" s="4">
-        <v>104</v>
+      <c r="K50" s="6"/>
+      <c r="L50" t="s" s="4">
+        <v>95</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+      <c r="F51" s="5">
+        <v>10</v>
+      </c>
+      <c r="G51" t="s" s="4">
+        <v>127</v>
+      </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" t="s" s="4">
-        <v>132</v>
+      <c r="K51" s="6"/>
+      <c r="L51" t="s" s="4">
+        <v>128</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B52" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C52" t="s" s="4">
         <v>130</v>
-      </c>
-      <c r="C52" t="s" s="4">
-        <v>134</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="5">
+        <v>30</v>
+      </c>
+      <c r="G52" t="s" s="4">
+        <v>127</v>
+      </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" t="s" s="4">
-        <v>132</v>
+      <c r="K52" s="6"/>
+      <c r="L52" t="s" s="4">
+        <v>131</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
+      <c r="F53" s="5">
+        <v>100</v>
+      </c>
+      <c r="G53" t="s" s="4">
+        <v>127</v>
+      </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" t="s" s="4">
-        <v>132</v>
+      <c r="K53" s="6"/>
+      <c r="L53" t="s" s="4">
+        <v>134</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="G54" s="6"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" t="s" s="4">
-        <v>132</v>
+      <c r="K54" s="6"/>
+      <c r="L54" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
+        <v>138</v>
+      </c>
+      <c r="B55" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C55" t="s" s="4">
         <v>139</v>
-      </c>
-      <c r="B55" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C55" t="s" s="4">
-        <v>140</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
+      <c r="G55" s="6"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" t="s" s="4">
-        <v>132</v>
+      <c r="K55" s="6"/>
+      <c r="L55" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
+        <v>140</v>
+      </c>
+      <c r="B56" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C56" t="s" s="4">
         <v>141</v>
-      </c>
-      <c r="B56" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C56" t="s" s="4">
-        <v>142</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
+      <c r="G56" s="6"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
-      <c r="N56" t="s" s="4">
-        <v>132</v>
+      <c r="K56" s="6"/>
+      <c r="L56" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
+        <v>142</v>
+      </c>
+      <c r="B57" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C57" t="s" s="4">
         <v>143</v>
-      </c>
-      <c r="B57" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C57" t="s" s="4">
-        <v>144</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="5"/>
@@ -3995,22 +4038,20 @@
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
-      <c r="N57" t="s" s="4">
-        <v>132</v>
+      <c r="K57" s="6"/>
+      <c r="L57" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
+        <v>144</v>
+      </c>
+      <c r="B58" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C58" t="s" s="4">
         <v>145</v>
-      </c>
-      <c r="B58" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C58" t="s" s="4">
-        <v>146</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="5"/>
@@ -4019,22 +4060,20 @@
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="N58" t="s" s="4">
-        <v>132</v>
+      <c r="K58" s="6"/>
+      <c r="L58" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
+        <v>146</v>
+      </c>
+      <c r="B59" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C59" t="s" s="4">
         <v>147</v>
-      </c>
-      <c r="B59" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C59" t="s" s="4">
-        <v>148</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="5"/>
@@ -4043,22 +4082,20 @@
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-      <c r="M59" s="5"/>
-      <c r="N59" t="s" s="4">
-        <v>132</v>
+      <c r="K59" s="6"/>
+      <c r="L59" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
+        <v>148</v>
+      </c>
+      <c r="B60" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C60" t="s" s="4">
         <v>149</v>
-      </c>
-      <c r="B60" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C60" t="s" s="4">
-        <v>150</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
@@ -4067,22 +4104,20 @@
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
-      <c r="M60" s="5"/>
-      <c r="N60" t="s" s="4">
-        <v>132</v>
+      <c r="K60" s="6"/>
+      <c r="L60" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
+        <v>150</v>
+      </c>
+      <c r="B61" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C61" t="s" s="4">
         <v>151</v>
-      </c>
-      <c r="B61" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C61" t="s" s="4">
-        <v>152</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5"/>
@@ -4091,22 +4126,20 @@
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-      <c r="M61" s="5"/>
-      <c r="N61" t="s" s="4">
-        <v>132</v>
+      <c r="K61" s="6"/>
+      <c r="L61" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
+        <v>152</v>
+      </c>
+      <c r="B62" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C62" t="s" s="4">
         <v>153</v>
-      </c>
-      <c r="B62" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C62" t="s" s="4">
-        <v>154</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="5"/>
@@ -4115,22 +4148,20 @@
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-      <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
-      <c r="N62" t="s" s="4">
-        <v>132</v>
+      <c r="K62" s="6"/>
+      <c r="L62" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" t="s" s="3">
+        <v>154</v>
+      </c>
+      <c r="B63" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C63" t="s" s="4">
         <v>155</v>
-      </c>
-      <c r="B63" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C63" t="s" s="4">
-        <v>156</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="5"/>
@@ -4139,22 +4170,20 @@
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
-      <c r="N63" t="s" s="4">
-        <v>132</v>
+      <c r="K63" s="6"/>
+      <c r="L63" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
       <c r="A64" t="s" s="3">
+        <v>156</v>
+      </c>
+      <c r="B64" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C64" t="s" s="4">
         <v>157</v>
-      </c>
-      <c r="B64" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C64" t="s" s="4">
-        <v>158</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="5"/>
@@ -4163,22 +4192,20 @@
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" t="s" s="4">
-        <v>132</v>
+      <c r="K64" s="6"/>
+      <c r="L64" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" t="s" s="3">
+        <v>158</v>
+      </c>
+      <c r="B65" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C65" t="s" s="4">
         <v>159</v>
-      </c>
-      <c r="B65" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C65" t="s" s="4">
-        <v>160</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="5"/>
@@ -4187,22 +4214,20 @@
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
-      <c r="M65" s="5"/>
-      <c r="N65" t="s" s="4">
-        <v>132</v>
+      <c r="K65" s="6"/>
+      <c r="L65" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" t="s" s="3">
+        <v>160</v>
+      </c>
+      <c r="B66" t="s" s="4">
+        <v>125</v>
+      </c>
+      <c r="C66" t="s" s="4">
         <v>161</v>
-      </c>
-      <c r="B66" t="s" s="4">
-        <v>130</v>
-      </c>
-      <c r="C66" t="s" s="4">
-        <v>162</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="5"/>
@@ -4211,76 +4236,418 @@
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5"/>
-      <c r="M66" s="5"/>
-      <c r="N66" t="s" s="4">
-        <v>132</v>
+      <c r="K66" s="6"/>
+      <c r="L66" t="s" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
-      <c r="A67" s="7"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="8"/>
-      <c r="K67" s="8"/>
-      <c r="L67" s="8"/>
-      <c r="M67" s="9"/>
-      <c r="N67" s="10"/>
+      <c r="A67" t="s" s="3">
+        <v>162</v>
+      </c>
+      <c r="B67" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C67" t="s" s="4">
+        <v>164</v>
+      </c>
+      <c r="D67" s="6"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="6"/>
+      <c r="L67" t="s" s="4">
+        <v>165</v>
+      </c>
     </row>
     <row r="68" ht="20" customHeight="1">
-      <c r="A68" s="11"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="12"/>
-      <c r="J68" s="12"/>
-      <c r="K68" s="12"/>
-      <c r="L68" s="12"/>
-      <c r="M68" s="13"/>
-      <c r="N68" s="14"/>
+      <c r="A68" t="s" s="3">
+        <v>166</v>
+      </c>
+      <c r="B68" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C68" t="s" s="4">
+        <v>167</v>
+      </c>
+      <c r="D68" s="6"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="6"/>
+      <c r="L68" t="s" s="4">
+        <v>165</v>
+      </c>
     </row>
     <row r="69" ht="20" customHeight="1">
-      <c r="A69" s="11"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="12"/>
-      <c r="I69" s="12"/>
-      <c r="J69" s="12"/>
-      <c r="K69" s="12"/>
-      <c r="L69" s="12"/>
-      <c r="M69" s="13"/>
-      <c r="N69" s="14"/>
+      <c r="A69" t="s" s="3">
+        <v>168</v>
+      </c>
+      <c r="B69" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C69" t="s" s="4">
+        <v>169</v>
+      </c>
+      <c r="D69" s="6"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="6"/>
+      <c r="L69" t="s" s="4">
+        <v>165</v>
+      </c>
     </row>
     <row r="70" ht="20" customHeight="1">
-      <c r="A70" s="15"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="16"/>
-      <c r="G70" s="16"/>
-      <c r="H70" s="16"/>
-      <c r="I70" s="16"/>
-      <c r="J70" s="16"/>
-      <c r="K70" s="16"/>
-      <c r="L70" s="16"/>
-      <c r="M70" s="17"/>
-      <c r="N70" s="18"/>
+      <c r="A70" t="s" s="3">
+        <v>170</v>
+      </c>
+      <c r="B70" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C70" t="s" s="4">
+        <v>171</v>
+      </c>
+      <c r="D70" s="6"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="6"/>
+      <c r="L70" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="71" ht="20" customHeight="1">
+      <c r="A71" t="s" s="3">
+        <v>172</v>
+      </c>
+      <c r="B71" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C71" t="s" s="4">
+        <v>173</v>
+      </c>
+      <c r="D71" s="6"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="6"/>
+      <c r="L71" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="72" ht="20" customHeight="1">
+      <c r="A72" t="s" s="3">
+        <v>174</v>
+      </c>
+      <c r="B72" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C72" t="s" s="4">
+        <v>175</v>
+      </c>
+      <c r="D72" s="6"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="6"/>
+      <c r="L72" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" ht="20" customHeight="1">
+      <c r="A73" t="s" s="3">
+        <v>176</v>
+      </c>
+      <c r="B73" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C73" t="s" s="4">
+        <v>177</v>
+      </c>
+      <c r="D73" s="6"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="6"/>
+      <c r="L73" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="74" ht="20" customHeight="1">
+      <c r="A74" t="s" s="3">
+        <v>178</v>
+      </c>
+      <c r="B74" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C74" t="s" s="4">
+        <v>179</v>
+      </c>
+      <c r="D74" s="6"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="6"/>
+      <c r="L74" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" ht="20" customHeight="1">
+      <c r="A75" t="s" s="3">
+        <v>180</v>
+      </c>
+      <c r="B75" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C75" t="s" s="4">
+        <v>181</v>
+      </c>
+      <c r="D75" s="6"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="6"/>
+      <c r="L75" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="76" ht="20" customHeight="1">
+      <c r="A76" t="s" s="3">
+        <v>182</v>
+      </c>
+      <c r="B76" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C76" t="s" s="4">
+        <v>183</v>
+      </c>
+      <c r="D76" s="6"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="6"/>
+      <c r="L76" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="77" ht="20" customHeight="1">
+      <c r="A77" t="s" s="3">
+        <v>184</v>
+      </c>
+      <c r="B77" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C77" t="s" s="4">
+        <v>185</v>
+      </c>
+      <c r="D77" s="6"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="6"/>
+      <c r="L77" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="78" ht="20" customHeight="1">
+      <c r="A78" t="s" s="3">
+        <v>186</v>
+      </c>
+      <c r="B78" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C78" t="s" s="4">
+        <v>187</v>
+      </c>
+      <c r="D78" s="6"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="6"/>
+      <c r="L78" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" ht="20" customHeight="1">
+      <c r="A79" t="s" s="3">
+        <v>188</v>
+      </c>
+      <c r="B79" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C79" t="s" s="4">
+        <v>189</v>
+      </c>
+      <c r="D79" s="6"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="6"/>
+      <c r="L79" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="80" ht="20" customHeight="1">
+      <c r="A80" t="s" s="3">
+        <v>190</v>
+      </c>
+      <c r="B80" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C80" t="s" s="4">
+        <v>191</v>
+      </c>
+      <c r="D80" s="6"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="6"/>
+      <c r="L80" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="81" ht="20" customHeight="1">
+      <c r="A81" t="s" s="3">
+        <v>192</v>
+      </c>
+      <c r="B81" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C81" t="s" s="4">
+        <v>193</v>
+      </c>
+      <c r="D81" s="6"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="6"/>
+      <c r="L81" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="82" ht="20" customHeight="1">
+      <c r="A82" t="s" s="3">
+        <v>194</v>
+      </c>
+      <c r="B82" t="s" s="4">
+        <v>163</v>
+      </c>
+      <c r="C82" t="s" s="4">
+        <v>195</v>
+      </c>
+      <c r="D82" s="6"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="6"/>
+      <c r="L82" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="83" ht="20" customHeight="1">
+      <c r="A83" s="7"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="8"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="9"/>
+      <c r="K83" s="10"/>
+      <c r="L83" s="10"/>
+    </row>
+    <row r="84" ht="20" customHeight="1">
+      <c r="A84" s="11"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+    </row>
+    <row r="85" ht="20" customHeight="1">
+      <c r="A85" s="11"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
+    </row>
+    <row r="86" ht="20" customHeight="1">
+      <c r="A86" s="15"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="16"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="16"/>
+      <c r="I86" s="16"/>
+      <c r="J86" s="17"/>
+      <c r="K86" s="18"/>
+      <c r="L86" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4326,68 +4693,68 @@
         <v>2</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>166</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>168</v>
+        <v>201</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -4398,18 +4765,18 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s" s="4">
-        <v>171</v>
+        <v>204</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -4420,18 +4787,18 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s" s="4">
-        <v>173</v>
+        <v>206</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -4442,18 +4809,18 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>175</v>
+        <v>208</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
@@ -4464,18 +4831,18 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>177</v>
+        <v>210</v>
       </c>
       <c r="D7" s="4">
         <v>10</v>
@@ -4486,18 +4853,18 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>178</v>
+        <v>211</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="D8" s="4">
         <v>20</v>
@@ -4508,18 +4875,18 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="D9" s="4">
         <v>25</v>
@@ -4530,18 +4897,18 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>182</v>
+        <v>215</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>183</v>
+        <v>216</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -4552,18 +4919,18 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>184</v>
+        <v>217</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>185</v>
+        <v>218</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -4574,18 +4941,18 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>186</v>
+        <v>219</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>187</v>
+        <v>220</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -4596,18 +4963,18 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>189</v>
+        <v>222</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -4618,18 +4985,18 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>190</v>
+        <v>223</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>191</v>
+        <v>224</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -4640,18 +5007,18 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C15" t="s" s="4">
-        <v>193</v>
+        <v>226</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -4662,18 +5029,18 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>194</v>
+        <v>227</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>195</v>
+        <v>228</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -4684,18 +5051,18 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>196</v>
+        <v>229</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C17" t="s" s="4">
-        <v>197</v>
+        <v>230</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -4706,18 +5073,18 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>198</v>
+        <v>231</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -4728,18 +5095,18 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
+        <v>233</v>
+      </c>
+      <c r="B19" t="s" s="4">
         <v>200</v>
       </c>
-      <c r="B19" t="s" s="4">
-        <v>167</v>
-      </c>
       <c r="C19" t="s" s="4">
-        <v>201</v>
+        <v>234</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -4750,18 +5117,18 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>202</v>
+        <v>235</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>203</v>
+        <v>236</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -4772,18 +5139,18 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>204</v>
+        <v>237</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>205</v>
+        <v>238</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -4794,18 +5161,18 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>206</v>
+        <v>239</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>207</v>
+        <v>240</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -4816,18 +5183,18 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" t="s" s="4">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>208</v>
+        <v>241</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>210</v>
+        <v>243</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
@@ -4840,18 +5207,18 @@
         <v>1</v>
       </c>
       <c r="J23" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>212</v>
+        <v>245</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C24" t="s" s="4">
-        <v>213</v>
+        <v>246</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
@@ -4864,18 +5231,18 @@
         <v>1</v>
       </c>
       <c r="J24" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>214</v>
+        <v>247</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C25" t="s" s="4">
-        <v>215</v>
+        <v>248</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
@@ -4888,18 +5255,18 @@
         <v>1</v>
       </c>
       <c r="J25" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>216</v>
+        <v>249</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>217</v>
+        <v>250</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
@@ -4912,18 +5279,18 @@
         <v>1</v>
       </c>
       <c r="J26" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>219</v>
+        <v>252</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4">
@@ -4936,18 +5303,18 @@
         <v>1</v>
       </c>
       <c r="J27" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>220</v>
+        <v>253</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>221</v>
+        <v>254</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4">
@@ -4960,18 +5327,18 @@
         <v>1</v>
       </c>
       <c r="J28" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>222</v>
+        <v>255</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>223</v>
+        <v>256</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4">
@@ -4984,18 +5351,18 @@
         <v>1</v>
       </c>
       <c r="J29" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C30" t="s" s="4">
-        <v>225</v>
+        <v>258</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4">
@@ -5008,18 +5375,18 @@
         <v>1</v>
       </c>
       <c r="J30" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>226</v>
+        <v>259</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>227</v>
+        <v>260</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4">
@@ -5032,18 +5399,18 @@
         <v>1</v>
       </c>
       <c r="J31" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>228</v>
+        <v>261</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>229</v>
+        <v>262</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4">
@@ -5056,18 +5423,18 @@
         <v>1</v>
       </c>
       <c r="J32" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>230</v>
+        <v>263</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>231</v>
+        <v>264</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4">
@@ -5080,18 +5447,18 @@
         <v>1</v>
       </c>
       <c r="J33" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>233</v>
+        <v>266</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4">
@@ -5104,18 +5471,18 @@
         <v>1</v>
       </c>
       <c r="J34" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>234</v>
+        <v>267</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>235</v>
+        <v>268</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4">
@@ -5128,18 +5495,18 @@
         <v>1</v>
       </c>
       <c r="J35" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>236</v>
+        <v>269</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>237</v>
+        <v>270</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4">
@@ -5152,18 +5519,18 @@
         <v>1</v>
       </c>
       <c r="J36" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>238</v>
+        <v>271</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>239</v>
+        <v>272</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4">
@@ -5176,18 +5543,18 @@
         <v>1</v>
       </c>
       <c r="J37" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>240</v>
+        <v>273</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>241</v>
+        <v>274</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4">
@@ -5200,18 +5567,18 @@
         <v>1</v>
       </c>
       <c r="J38" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
+        <v>275</v>
+      </c>
+      <c r="B39" t="s" s="4">
         <v>242</v>
       </c>
-      <c r="B39" t="s" s="4">
-        <v>209</v>
-      </c>
       <c r="C39" t="s" s="4">
-        <v>243</v>
+        <v>276</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4">
@@ -5224,18 +5591,18 @@
         <v>1</v>
       </c>
       <c r="J39" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>244</v>
+        <v>277</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>245</v>
+        <v>278</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4">
@@ -5248,18 +5615,18 @@
         <v>1</v>
       </c>
       <c r="J40" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>246</v>
+        <v>279</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>247</v>
+        <v>280</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4">
@@ -5272,18 +5639,18 @@
         <v>1</v>
       </c>
       <c r="J41" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>248</v>
+        <v>281</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>249</v>
+        <v>282</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4">
@@ -5296,18 +5663,18 @@
         <v>1</v>
       </c>
       <c r="J42" t="s" s="4">
-        <v>211</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>250</v>
+        <v>283</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>252</v>
+        <v>285</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4">
@@ -5318,18 +5685,18 @@
       <c r="H43" s="5"/>
       <c r="I43" s="6"/>
       <c r="J43" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>254</v>
+        <v>287</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>255</v>
+        <v>288</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4">
@@ -5340,18 +5707,18 @@
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
       <c r="J44" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>256</v>
+        <v>289</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>257</v>
+        <v>290</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4">
@@ -5362,18 +5729,18 @@
       <c r="H45" s="5"/>
       <c r="I45" s="6"/>
       <c r="J45" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>258</v>
+        <v>291</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>259</v>
+        <v>292</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4">
@@ -5384,18 +5751,18 @@
       <c r="H46" s="5"/>
       <c r="I46" s="6"/>
       <c r="J46" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>260</v>
+        <v>293</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>261</v>
+        <v>294</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4">
@@ -5406,18 +5773,18 @@
       <c r="H47" s="5"/>
       <c r="I47" s="6"/>
       <c r="J47" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>262</v>
+        <v>295</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>263</v>
+        <v>296</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -5428,18 +5795,18 @@
       <c r="H48" s="5"/>
       <c r="I48" s="6"/>
       <c r="J48" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>264</v>
+        <v>297</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>265</v>
+        <v>298</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -5450,18 +5817,18 @@
       <c r="H49" s="5"/>
       <c r="I49" s="6"/>
       <c r="J49" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>266</v>
+        <v>299</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>267</v>
+        <v>300</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -5472,18 +5839,18 @@
       <c r="H50" s="5"/>
       <c r="I50" s="6"/>
       <c r="J50" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>268</v>
+        <v>301</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>269</v>
+        <v>302</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -5494,18 +5861,18 @@
       <c r="H51" s="5"/>
       <c r="I51" s="6"/>
       <c r="J51" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>270</v>
+        <v>303</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>271</v>
+        <v>304</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -5516,18 +5883,18 @@
       <c r="H52" s="5"/>
       <c r="I52" s="6"/>
       <c r="J52" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>272</v>
+        <v>305</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>273</v>
+        <v>306</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -5538,18 +5905,18 @@
       <c r="H53" s="5"/>
       <c r="I53" s="6"/>
       <c r="J53" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>274</v>
+        <v>307</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>275</v>
+        <v>308</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -5560,18 +5927,18 @@
       <c r="H54" s="5"/>
       <c r="I54" s="6"/>
       <c r="J54" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>276</v>
+        <v>309</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>277</v>
+        <v>310</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -5582,18 +5949,18 @@
       <c r="H55" s="5"/>
       <c r="I55" s="6"/>
       <c r="J55" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>278</v>
+        <v>311</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>279</v>
+        <v>312</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -5604,18 +5971,18 @@
       <c r="H56" s="5"/>
       <c r="I56" s="6"/>
       <c r="J56" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -5626,18 +5993,18 @@
       <c r="H57" s="5"/>
       <c r="I57" s="6"/>
       <c r="J57" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>282</v>
+        <v>315</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>283</v>
+        <v>316</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -5648,18 +6015,18 @@
       <c r="H58" s="5"/>
       <c r="I58" s="6"/>
       <c r="J58" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
+        <v>317</v>
+      </c>
+      <c r="B59" t="s" s="4">
         <v>284</v>
       </c>
-      <c r="B59" t="s" s="4">
-        <v>251</v>
-      </c>
       <c r="C59" t="s" s="4">
-        <v>285</v>
+        <v>318</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -5670,18 +6037,18 @@
       <c r="H59" s="5"/>
       <c r="I59" s="6"/>
       <c r="J59" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>286</v>
+        <v>319</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>287</v>
+        <v>320</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -5692,18 +6059,18 @@
       <c r="H60" s="5"/>
       <c r="I60" s="6"/>
       <c r="J60" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>288</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>289</v>
+        <v>322</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -5714,18 +6081,18 @@
       <c r="H61" s="5"/>
       <c r="I61" s="6"/>
       <c r="J61" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>290</v>
+        <v>323</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>291</v>
+        <v>324</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -5736,7 +6103,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="6"/>
       <c r="J62" t="s" s="4">
-        <v>253</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -5772,33 +6139,33 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>292</v>
+        <v>325</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>293</v>
+        <v>326</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>294</v>
+        <v>327</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>295</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
@@ -5812,7 +6179,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>166</v>
+        <v>199</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -5829,7 +6196,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="E4" s="4">
         <v>30</v>
@@ -5846,7 +6213,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s" s="4">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
@@ -5863,7 +6230,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s" s="4">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="E6" s="4">
         <v>10</v>
@@ -5880,7 +6247,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
@@ -5897,7 +6264,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>178</v>
+        <v>211</v>
       </c>
       <c r="E8" s="4">
         <v>2</v>
@@ -5914,7 +6281,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -5931,7 +6298,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>208</v>
+        <v>241</v>
       </c>
       <c r="E10" s="4">
         <v>50</v>
@@ -5948,7 +6315,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s" s="4">
-        <v>212</v>
+        <v>245</v>
       </c>
       <c r="E11" s="4">
         <v>30</v>
@@ -5965,7 +6332,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>214</v>
+        <v>247</v>
       </c>
       <c r="E12" s="4">
         <v>20</v>
@@ -5982,7 +6349,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>216</v>
+        <v>249</v>
       </c>
       <c r="E13" s="4">
         <v>10</v>
@@ -5999,7 +6366,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s" s="4">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
@@ -6016,7 +6383,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="4">
-        <v>220</v>
+        <v>253</v>
       </c>
       <c r="E15" s="4">
         <v>2</v>
@@ -6033,7 +6400,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s" s="4">
-        <v>222</v>
+        <v>255</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -6050,7 +6417,7 @@
         <v>10</v>
       </c>
       <c r="D17" t="s" s="4">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E17" s="4">
         <v>200</v>
@@ -6067,7 +6434,7 @@
         <v>10</v>
       </c>
       <c r="D18" t="s" s="4">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E18" s="4">
         <v>50</v>
@@ -6084,7 +6451,7 @@
         <v>10</v>
       </c>
       <c r="D19" t="s" s="4">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E19" s="4">
         <v>20</v>
@@ -6101,7 +6468,7 @@
         <v>10</v>
       </c>
       <c r="D20" t="s" s="4">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E20" s="4">
         <v>20</v>
@@ -6118,7 +6485,7 @@
         <v>10</v>
       </c>
       <c r="D21" t="s" s="4">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E21" s="4">
         <v>500</v>
@@ -6135,7 +6502,7 @@
         <v>10</v>
       </c>
       <c r="D22" t="s" s="4">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E22" s="4">
         <v>400</v>
@@ -6152,7 +6519,7 @@
         <v>10</v>
       </c>
       <c r="D23" t="s" s="4">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E23" s="4">
         <v>300</v>
@@ -6169,7 +6536,7 @@
         <v>10</v>
       </c>
       <c r="D24" t="s" s="4">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E24" s="4">
         <v>100</v>
@@ -6186,7 +6553,7 @@
         <v>10</v>
       </c>
       <c r="D25" t="s" s="4">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E25" s="4">
         <v>50</v>
@@ -6203,7 +6570,7 @@
         <v>10</v>
       </c>
       <c r="D26" t="s" s="4">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E26" s="4">
         <v>25</v>

</xml_diff>

<commit_message>
fixed #280 FlixelRL-280 力の薬
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="331">
   <si>
     <t>id</t>
   </si>
@@ -307,16 +307,19 @@
     <t>PORTION19</t>
   </si>
   <si>
-    <t>薬19</t>
+    <t>力の薬</t>
+  </si>
+  <si>
+    <t>力が上昇します</t>
+  </si>
+  <si>
+    <t>PORTION20</t>
+  </si>
+  <si>
+    <t>薬20</t>
   </si>
   <si>
     <t>飲むとHPが1回復します</t>
-  </si>
-  <si>
-    <t>PORTION20</t>
-  </si>
-  <si>
-    <t>薬20</t>
   </si>
   <si>
     <t>PORTION21</t>
@@ -3528,9 +3531,7 @@
       <c r="C37" t="s" s="4">
         <v>97</v>
       </c>
-      <c r="D37" s="4">
-        <v>1</v>
-      </c>
+      <c r="D37" s="6"/>
       <c r="E37" s="5">
         <v>10</v>
       </c>
@@ -3538,8 +3539,12 @@
       <c r="G37" s="6"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="6"/>
+      <c r="J37" t="s" s="4">
+        <v>13</v>
+      </c>
+      <c r="K37" s="5">
+        <v>1</v>
+      </c>
       <c r="L37" t="s" s="4">
         <v>98</v>
       </c>
@@ -3567,18 +3572,18 @@
       <c r="J38" s="5"/>
       <c r="K38" s="6"/>
       <c r="L38" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B39" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D39" s="4">
         <v>1</v>
@@ -3593,18 +3598,18 @@
       <c r="J39" s="5"/>
       <c r="K39" s="6"/>
       <c r="L39" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B40" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D40" s="4">
         <v>1</v>
@@ -3619,18 +3624,18 @@
       <c r="J40" s="5"/>
       <c r="K40" s="6"/>
       <c r="L40" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D41" s="4">
         <v>1</v>
@@ -3645,18 +3650,18 @@
       <c r="J41" s="5"/>
       <c r="K41" s="6"/>
       <c r="L41" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D42" s="4">
         <v>1</v>
@@ -3671,18 +3676,18 @@
       <c r="J42" s="5"/>
       <c r="K42" s="6"/>
       <c r="L42" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B43" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D43" s="4">
         <v>1</v>
@@ -3697,18 +3702,18 @@
       <c r="J43" s="5"/>
       <c r="K43" s="6"/>
       <c r="L43" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B44" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D44" s="4">
         <v>1</v>
@@ -3723,18 +3728,18 @@
       <c r="J44" s="5"/>
       <c r="K44" s="6"/>
       <c r="L44" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B45" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D45" s="4">
         <v>1</v>
@@ -3749,18 +3754,18 @@
       <c r="J45" s="5"/>
       <c r="K45" s="6"/>
       <c r="L45" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
@@ -3775,18 +3780,18 @@
       <c r="J46" s="5"/>
       <c r="K46" s="6"/>
       <c r="L46" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B47" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -3801,18 +3806,18 @@
       <c r="J47" s="5"/>
       <c r="K47" s="6"/>
       <c r="L47" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
@@ -3827,18 +3832,18 @@
       <c r="J48" s="5"/>
       <c r="K48" s="6"/>
       <c r="L48" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -3853,18 +3858,18 @@
       <c r="J49" s="5"/>
       <c r="K49" s="6"/>
       <c r="L49" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
@@ -3879,18 +3884,18 @@
       <c r="J50" s="5"/>
       <c r="K50" s="6"/>
       <c r="L50" t="s" s="4">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5"/>
@@ -3898,25 +3903,25 @@
         <v>10</v>
       </c>
       <c r="G51" t="s" s="4">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="6"/>
       <c r="L51" t="s" s="4">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="5"/>
@@ -3924,25 +3929,25 @@
         <v>30</v>
       </c>
       <c r="G52" t="s" s="4">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="6"/>
       <c r="L52" t="s" s="4">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5"/>
@@ -3950,25 +3955,25 @@
         <v>100</v>
       </c>
       <c r="G53" t="s" s="4">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="6"/>
       <c r="L53" t="s" s="4">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
@@ -3979,18 +3984,18 @@
       <c r="J54" s="5"/>
       <c r="K54" s="6"/>
       <c r="L54" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="5"/>
@@ -4001,18 +4006,18 @@
       <c r="J55" s="5"/>
       <c r="K55" s="6"/>
       <c r="L55" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="5"/>
@@ -4023,18 +4028,18 @@
       <c r="J56" s="5"/>
       <c r="K56" s="6"/>
       <c r="L56" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="5"/>
@@ -4045,18 +4050,18 @@
       <c r="J57" s="5"/>
       <c r="K57" s="6"/>
       <c r="L57" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="5"/>
@@ -4067,18 +4072,18 @@
       <c r="J58" s="5"/>
       <c r="K58" s="6"/>
       <c r="L58" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="5"/>
@@ -4089,18 +4094,18 @@
       <c r="J59" s="5"/>
       <c r="K59" s="6"/>
       <c r="L59" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
@@ -4111,18 +4116,18 @@
       <c r="J60" s="5"/>
       <c r="K60" s="6"/>
       <c r="L60" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5"/>
@@ -4133,18 +4138,18 @@
       <c r="J61" s="5"/>
       <c r="K61" s="6"/>
       <c r="L61" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="5"/>
@@ -4155,18 +4160,18 @@
       <c r="J62" s="5"/>
       <c r="K62" s="6"/>
       <c r="L62" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" t="s" s="3">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C63" t="s" s="4">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="5"/>
@@ -4177,18 +4182,18 @@
       <c r="J63" s="5"/>
       <c r="K63" s="6"/>
       <c r="L63" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
       <c r="A64" t="s" s="3">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C64" t="s" s="4">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="5"/>
@@ -4199,18 +4204,18 @@
       <c r="J64" s="5"/>
       <c r="K64" s="6"/>
       <c r="L64" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" t="s" s="3">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C65" t="s" s="4">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="5"/>
@@ -4221,18 +4226,18 @@
       <c r="J65" s="5"/>
       <c r="K65" s="6"/>
       <c r="L65" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" t="s" s="3">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C66" t="s" s="4">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="5"/>
@@ -4243,18 +4248,18 @@
       <c r="J66" s="5"/>
       <c r="K66" s="6"/>
       <c r="L66" t="s" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
       <c r="A67" t="s" s="3">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B67" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C67" t="s" s="4">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="5"/>
@@ -4265,18 +4270,18 @@
       <c r="J67" s="5"/>
       <c r="K67" s="6"/>
       <c r="L67" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" ht="20" customHeight="1">
       <c r="A68" t="s" s="3">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B68" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C68" t="s" s="4">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="5"/>
@@ -4287,18 +4292,18 @@
       <c r="J68" s="5"/>
       <c r="K68" s="6"/>
       <c r="L68" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
       <c r="A69" t="s" s="3">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B69" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C69" t="s" s="4">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="5"/>
@@ -4309,18 +4314,18 @@
       <c r="J69" s="5"/>
       <c r="K69" s="6"/>
       <c r="L69" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
       <c r="A70" t="s" s="3">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B70" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C70" t="s" s="4">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="5"/>
@@ -4331,18 +4336,18 @@
       <c r="J70" s="5"/>
       <c r="K70" s="6"/>
       <c r="L70" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
       <c r="A71" t="s" s="3">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C71" t="s" s="4">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="5"/>
@@ -4353,18 +4358,18 @@
       <c r="J71" s="5"/>
       <c r="K71" s="6"/>
       <c r="L71" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" ht="20" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C72" t="s" s="4">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="5"/>
@@ -4375,18 +4380,18 @@
       <c r="J72" s="5"/>
       <c r="K72" s="6"/>
       <c r="L72" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" t="s" s="3">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B73" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C73" t="s" s="4">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="5"/>
@@ -4397,18 +4402,18 @@
       <c r="J73" s="5"/>
       <c r="K73" s="6"/>
       <c r="L73" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" ht="20" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B74" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C74" t="s" s="4">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="5"/>
@@ -4419,18 +4424,18 @@
       <c r="J74" s="5"/>
       <c r="K74" s="6"/>
       <c r="L74" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="75" ht="20" customHeight="1">
       <c r="A75" t="s" s="3">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B75" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C75" t="s" s="4">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="5"/>
@@ -4441,18 +4446,18 @@
       <c r="J75" s="5"/>
       <c r="K75" s="6"/>
       <c r="L75" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C76" t="s" s="4">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -4463,18 +4468,18 @@
       <c r="J76" s="5"/>
       <c r="K76" s="6"/>
       <c r="L76" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" t="s" s="3">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B77" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C77" t="s" s="4">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="5"/>
@@ -4485,18 +4490,18 @@
       <c r="J77" s="5"/>
       <c r="K77" s="6"/>
       <c r="L77" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B78" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C78" t="s" s="4">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="5"/>
@@ -4507,18 +4512,18 @@
       <c r="J78" s="5"/>
       <c r="K78" s="6"/>
       <c r="L78" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" t="s" s="3">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C79" t="s" s="4">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="5"/>
@@ -4529,18 +4534,18 @@
       <c r="J79" s="5"/>
       <c r="K79" s="6"/>
       <c r="L79" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B80" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C80" t="s" s="4">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="5"/>
@@ -4551,18 +4556,18 @@
       <c r="J80" s="5"/>
       <c r="K80" s="6"/>
       <c r="L80" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" t="s" s="3">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B81" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C81" t="s" s="4">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="5"/>
@@ -4573,18 +4578,18 @@
       <c r="J81" s="5"/>
       <c r="K81" s="6"/>
       <c r="L81" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B82" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C82" t="s" s="4">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="5"/>
@@ -4595,7 +4600,7 @@
       <c r="J82" s="5"/>
       <c r="K82" s="6"/>
       <c r="L82" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
@@ -4701,16 +4706,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G1" t="s" s="2">
         <v>9</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>4</v>
@@ -4753,13 +4758,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -4770,18 +4775,18 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s" s="4">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -4792,18 +4797,18 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C5" t="s" s="4">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -4814,18 +4819,18 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
@@ -4836,18 +4841,18 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D7" s="4">
         <v>10</v>
@@ -4858,18 +4863,18 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D8" s="4">
         <v>20</v>
@@ -4880,18 +4885,18 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D9" s="4">
         <v>25</v>
@@ -4902,18 +4907,18 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -4924,18 +4929,18 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -4946,18 +4951,18 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -4968,18 +4973,18 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -4990,18 +4995,18 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -5012,18 +5017,18 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C15" t="s" s="4">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -5034,18 +5039,18 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -5056,18 +5061,18 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C17" t="s" s="4">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -5078,18 +5083,18 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -5100,18 +5105,18 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -5122,18 +5127,18 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -5144,18 +5149,18 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -5166,18 +5171,18 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -5188,18 +5193,18 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" t="s" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
@@ -5212,18 +5217,18 @@
         <v>1</v>
       </c>
       <c r="J23" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C24" t="s" s="4">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
@@ -5236,18 +5241,18 @@
         <v>1</v>
       </c>
       <c r="J24" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C25" t="s" s="4">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
@@ -5260,18 +5265,18 @@
         <v>1</v>
       </c>
       <c r="J25" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
@@ -5284,18 +5289,18 @@
         <v>1</v>
       </c>
       <c r="J26" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4">
@@ -5308,18 +5313,18 @@
         <v>1</v>
       </c>
       <c r="J27" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4">
@@ -5332,18 +5337,18 @@
         <v>1</v>
       </c>
       <c r="J28" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4">
@@ -5356,18 +5361,18 @@
         <v>1</v>
       </c>
       <c r="J29" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C30" t="s" s="4">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4">
@@ -5380,18 +5385,18 @@
         <v>1</v>
       </c>
       <c r="J30" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4">
@@ -5404,18 +5409,18 @@
         <v>1</v>
       </c>
       <c r="J31" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4">
@@ -5428,18 +5433,18 @@
         <v>1</v>
       </c>
       <c r="J32" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4">
@@ -5452,18 +5457,18 @@
         <v>1</v>
       </c>
       <c r="J33" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4">
@@ -5476,18 +5481,18 @@
         <v>1</v>
       </c>
       <c r="J34" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4">
@@ -5500,18 +5505,18 @@
         <v>1</v>
       </c>
       <c r="J35" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4">
@@ -5524,18 +5529,18 @@
         <v>1</v>
       </c>
       <c r="J36" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4">
@@ -5548,18 +5553,18 @@
         <v>1</v>
       </c>
       <c r="J37" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4">
@@ -5572,18 +5577,18 @@
         <v>1</v>
       </c>
       <c r="J38" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4">
@@ -5596,18 +5601,18 @@
         <v>1</v>
       </c>
       <c r="J39" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4">
@@ -5620,18 +5625,18 @@
         <v>1</v>
       </c>
       <c r="J40" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4">
@@ -5644,18 +5649,18 @@
         <v>1</v>
       </c>
       <c r="J41" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4">
@@ -5668,18 +5673,18 @@
         <v>1</v>
       </c>
       <c r="J42" t="s" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4">
@@ -5690,18 +5695,18 @@
       <c r="H43" s="5"/>
       <c r="I43" s="6"/>
       <c r="J43" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4">
@@ -5712,18 +5717,18 @@
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
       <c r="J44" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4">
@@ -5734,18 +5739,18 @@
       <c r="H45" s="5"/>
       <c r="I45" s="6"/>
       <c r="J45" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4">
@@ -5756,18 +5761,18 @@
       <c r="H46" s="5"/>
       <c r="I46" s="6"/>
       <c r="J46" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4">
@@ -5778,18 +5783,18 @@
       <c r="H47" s="5"/>
       <c r="I47" s="6"/>
       <c r="J47" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -5800,18 +5805,18 @@
       <c r="H48" s="5"/>
       <c r="I48" s="6"/>
       <c r="J48" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -5822,18 +5827,18 @@
       <c r="H49" s="5"/>
       <c r="I49" s="6"/>
       <c r="J49" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -5844,18 +5849,18 @@
       <c r="H50" s="5"/>
       <c r="I50" s="6"/>
       <c r="J50" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -5866,18 +5871,18 @@
       <c r="H51" s="5"/>
       <c r="I51" s="6"/>
       <c r="J51" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -5888,18 +5893,18 @@
       <c r="H52" s="5"/>
       <c r="I52" s="6"/>
       <c r="J52" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -5910,18 +5915,18 @@
       <c r="H53" s="5"/>
       <c r="I53" s="6"/>
       <c r="J53" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -5932,18 +5937,18 @@
       <c r="H54" s="5"/>
       <c r="I54" s="6"/>
       <c r="J54" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -5954,18 +5959,18 @@
       <c r="H55" s="5"/>
       <c r="I55" s="6"/>
       <c r="J55" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -5976,18 +5981,18 @@
       <c r="H56" s="5"/>
       <c r="I56" s="6"/>
       <c r="J56" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -5998,18 +6003,18 @@
       <c r="H57" s="5"/>
       <c r="I57" s="6"/>
       <c r="J57" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -6020,18 +6025,18 @@
       <c r="H58" s="5"/>
       <c r="I58" s="6"/>
       <c r="J58" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -6042,18 +6047,18 @@
       <c r="H59" s="5"/>
       <c r="I59" s="6"/>
       <c r="J59" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -6064,18 +6069,18 @@
       <c r="H60" s="5"/>
       <c r="I60" s="6"/>
       <c r="J60" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -6086,18 +6091,18 @@
       <c r="H61" s="5"/>
       <c r="I61" s="6"/>
       <c r="J61" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -6108,7 +6113,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="6"/>
       <c r="J62" t="s" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -6125,7 +6130,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -6144,16 +6149,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -6184,7 +6189,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -6201,7 +6206,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E4" s="4">
         <v>30</v>
@@ -6218,7 +6223,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s" s="4">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
@@ -6235,7 +6240,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s" s="4">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E6" s="4">
         <v>10</v>
@@ -6252,7 +6257,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
@@ -6269,7 +6274,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E8" s="4">
         <v>2</v>
@@ -6286,7 +6291,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -6303,7 +6308,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E10" s="4">
         <v>50</v>
@@ -6320,7 +6325,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s" s="4">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E11" s="4">
         <v>30</v>
@@ -6337,7 +6342,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E12" s="4">
         <v>20</v>
@@ -6354,7 +6359,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E13" s="4">
         <v>10</v>
@@ -6371,7 +6376,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s" s="4">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
@@ -6388,7 +6393,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="4">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E15" s="4">
         <v>2</v>
@@ -6405,7 +6410,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s" s="4">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -6612,6 +6617,23 @@
         <v>93</v>
       </c>
       <c r="E28" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" ht="20" customHeight="1">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s" s="4">
+        <v>96</v>
+      </c>
+      <c r="E29" s="4">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed #284 FlixelRL-284 毒薬
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="333">
   <si>
     <t>id</t>
   </si>
@@ -316,16 +316,22 @@
     <t>PORTION20</t>
   </si>
   <si>
-    <t>薬20</t>
+    <t>毒薬</t>
+  </si>
+  <si>
+    <t>poison</t>
+  </si>
+  <si>
+    <t>猛毒の薬。飲んではいけません</t>
+  </si>
+  <si>
+    <t>PORTION21</t>
+  </si>
+  <si>
+    <t>薬21</t>
   </si>
   <si>
     <t>飲むとHPが1回復します</t>
-  </si>
-  <si>
-    <t>PORTION21</t>
-  </si>
-  <si>
-    <t>薬21</t>
   </si>
   <si>
     <t>PORTION22</t>
@@ -3559,9 +3565,7 @@
       <c r="C38" t="s" s="4">
         <v>100</v>
       </c>
-      <c r="D38" s="4">
-        <v>1</v>
-      </c>
+      <c r="D38" s="6"/>
       <c r="E38" s="5">
         <v>10</v>
       </c>
@@ -3569,21 +3573,23 @@
       <c r="G38" s="6"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
+      <c r="J38" t="s" s="4">
+        <v>101</v>
+      </c>
       <c r="K38" s="6"/>
       <c r="L38" t="s" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D39" s="4">
         <v>1</v>
@@ -3598,18 +3604,18 @@
       <c r="J39" s="5"/>
       <c r="K39" s="6"/>
       <c r="L39" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B40" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D40" s="4">
         <v>1</v>
@@ -3624,18 +3630,18 @@
       <c r="J40" s="5"/>
       <c r="K40" s="6"/>
       <c r="L40" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B41" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D41" s="4">
         <v>1</v>
@@ -3650,18 +3656,18 @@
       <c r="J41" s="5"/>
       <c r="K41" s="6"/>
       <c r="L41" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B42" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D42" s="4">
         <v>1</v>
@@ -3676,18 +3682,18 @@
       <c r="J42" s="5"/>
       <c r="K42" s="6"/>
       <c r="L42" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B43" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D43" s="4">
         <v>1</v>
@@ -3702,18 +3708,18 @@
       <c r="J43" s="5"/>
       <c r="K43" s="6"/>
       <c r="L43" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B44" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D44" s="4">
         <v>1</v>
@@ -3728,18 +3734,18 @@
       <c r="J44" s="5"/>
       <c r="K44" s="6"/>
       <c r="L44" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B45" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D45" s="4">
         <v>1</v>
@@ -3754,18 +3760,18 @@
       <c r="J45" s="5"/>
       <c r="K45" s="6"/>
       <c r="L45" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
@@ -3780,18 +3786,18 @@
       <c r="J46" s="5"/>
       <c r="K46" s="6"/>
       <c r="L46" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B47" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -3806,18 +3812,18 @@
       <c r="J47" s="5"/>
       <c r="K47" s="6"/>
       <c r="L47" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
@@ -3832,18 +3838,18 @@
       <c r="J48" s="5"/>
       <c r="K48" s="6"/>
       <c r="L48" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B49" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -3858,18 +3864,18 @@
       <c r="J49" s="5"/>
       <c r="K49" s="6"/>
       <c r="L49" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>41</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
@@ -3884,18 +3890,18 @@
       <c r="J50" s="5"/>
       <c r="K50" s="6"/>
       <c r="L50" t="s" s="4">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5"/>
@@ -3903,25 +3909,25 @@
         <v>10</v>
       </c>
       <c r="G51" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="6"/>
       <c r="L51" t="s" s="4">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="5"/>
@@ -3929,25 +3935,25 @@
         <v>30</v>
       </c>
       <c r="G52" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="6"/>
       <c r="L52" t="s" s="4">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5"/>
@@ -3955,25 +3961,25 @@
         <v>100</v>
       </c>
       <c r="G53" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="6"/>
       <c r="L53" t="s" s="4">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
@@ -3984,18 +3990,18 @@
       <c r="J54" s="5"/>
       <c r="K54" s="6"/>
       <c r="L54" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="5"/>
@@ -4006,18 +4012,18 @@
       <c r="J55" s="5"/>
       <c r="K55" s="6"/>
       <c r="L55" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="5"/>
@@ -4028,18 +4034,18 @@
       <c r="J56" s="5"/>
       <c r="K56" s="6"/>
       <c r="L56" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="5"/>
@@ -4050,18 +4056,18 @@
       <c r="J57" s="5"/>
       <c r="K57" s="6"/>
       <c r="L57" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="5"/>
@@ -4072,18 +4078,18 @@
       <c r="J58" s="5"/>
       <c r="K58" s="6"/>
       <c r="L58" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="5"/>
@@ -4094,18 +4100,18 @@
       <c r="J59" s="5"/>
       <c r="K59" s="6"/>
       <c r="L59" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
@@ -4116,18 +4122,18 @@
       <c r="J60" s="5"/>
       <c r="K60" s="6"/>
       <c r="L60" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5"/>
@@ -4138,18 +4144,18 @@
       <c r="J61" s="5"/>
       <c r="K61" s="6"/>
       <c r="L61" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="5"/>
@@ -4160,18 +4166,18 @@
       <c r="J62" s="5"/>
       <c r="K62" s="6"/>
       <c r="L62" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" t="s" s="3">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C63" t="s" s="4">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="5"/>
@@ -4182,18 +4188,18 @@
       <c r="J63" s="5"/>
       <c r="K63" s="6"/>
       <c r="L63" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
       <c r="A64" t="s" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C64" t="s" s="4">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="5"/>
@@ -4204,18 +4210,18 @@
       <c r="J64" s="5"/>
       <c r="K64" s="6"/>
       <c r="L64" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" t="s" s="3">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C65" t="s" s="4">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="5"/>
@@ -4226,18 +4232,18 @@
       <c r="J65" s="5"/>
       <c r="K65" s="6"/>
       <c r="L65" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" t="s" s="3">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C66" t="s" s="4">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="5"/>
@@ -4248,18 +4254,18 @@
       <c r="J66" s="5"/>
       <c r="K66" s="6"/>
       <c r="L66" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
       <c r="A67" t="s" s="3">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B67" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C67" t="s" s="4">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="5"/>
@@ -4270,18 +4276,18 @@
       <c r="J67" s="5"/>
       <c r="K67" s="6"/>
       <c r="L67" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" ht="20" customHeight="1">
       <c r="A68" t="s" s="3">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B68" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C68" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="5"/>
@@ -4292,18 +4298,18 @@
       <c r="J68" s="5"/>
       <c r="K68" s="6"/>
       <c r="L68" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
       <c r="A69" t="s" s="3">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B69" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C69" t="s" s="4">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="5"/>
@@ -4314,18 +4320,18 @@
       <c r="J69" s="5"/>
       <c r="K69" s="6"/>
       <c r="L69" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
       <c r="A70" t="s" s="3">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B70" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C70" t="s" s="4">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="5"/>
@@ -4336,18 +4342,18 @@
       <c r="J70" s="5"/>
       <c r="K70" s="6"/>
       <c r="L70" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
       <c r="A71" t="s" s="3">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C71" t="s" s="4">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="5"/>
@@ -4358,18 +4364,18 @@
       <c r="J71" s="5"/>
       <c r="K71" s="6"/>
       <c r="L71" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" ht="20" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C72" t="s" s="4">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="5"/>
@@ -4380,18 +4386,18 @@
       <c r="J72" s="5"/>
       <c r="K72" s="6"/>
       <c r="L72" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" t="s" s="3">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B73" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C73" t="s" s="4">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="5"/>
@@ -4402,18 +4408,18 @@
       <c r="J73" s="5"/>
       <c r="K73" s="6"/>
       <c r="L73" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" ht="20" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B74" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C74" t="s" s="4">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="5"/>
@@ -4424,18 +4430,18 @@
       <c r="J74" s="5"/>
       <c r="K74" s="6"/>
       <c r="L74" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="75" ht="20" customHeight="1">
       <c r="A75" t="s" s="3">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B75" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C75" t="s" s="4">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="5"/>
@@ -4446,18 +4452,18 @@
       <c r="J75" s="5"/>
       <c r="K75" s="6"/>
       <c r="L75" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C76" t="s" s="4">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -4468,18 +4474,18 @@
       <c r="J76" s="5"/>
       <c r="K76" s="6"/>
       <c r="L76" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" t="s" s="3">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B77" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C77" t="s" s="4">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="5"/>
@@ -4490,18 +4496,18 @@
       <c r="J77" s="5"/>
       <c r="K77" s="6"/>
       <c r="L77" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B78" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C78" t="s" s="4">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="5"/>
@@ -4512,18 +4518,18 @@
       <c r="J78" s="5"/>
       <c r="K78" s="6"/>
       <c r="L78" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" t="s" s="3">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C79" t="s" s="4">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="5"/>
@@ -4534,18 +4540,18 @@
       <c r="J79" s="5"/>
       <c r="K79" s="6"/>
       <c r="L79" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B80" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C80" t="s" s="4">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="5"/>
@@ -4556,18 +4562,18 @@
       <c r="J80" s="5"/>
       <c r="K80" s="6"/>
       <c r="L80" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" t="s" s="3">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B81" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C81" t="s" s="4">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="5"/>
@@ -4578,18 +4584,18 @@
       <c r="J81" s="5"/>
       <c r="K81" s="6"/>
       <c r="L81" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B82" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C82" t="s" s="4">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="5"/>
@@ -4600,7 +4606,7 @@
       <c r="J82" s="5"/>
       <c r="K82" s="6"/>
       <c r="L82" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
@@ -4706,16 +4712,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G1" t="s" s="2">
         <v>9</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>4</v>
@@ -4758,13 +4764,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -4775,18 +4781,18 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -4797,18 +4803,18 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s" s="4">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -4819,18 +4825,18 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
@@ -4841,18 +4847,18 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D7" s="4">
         <v>10</v>
@@ -4863,18 +4869,18 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D8" s="4">
         <v>20</v>
@@ -4885,18 +4891,18 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D9" s="4">
         <v>25</v>
@@ -4907,18 +4913,18 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -4929,18 +4935,18 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -4951,18 +4957,18 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -4973,18 +4979,18 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -4995,18 +5001,18 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -5017,18 +5023,18 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C15" t="s" s="4">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -5039,18 +5045,18 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -5061,18 +5067,18 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C17" t="s" s="4">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -5083,18 +5089,18 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -5105,18 +5111,18 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -5127,18 +5133,18 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -5149,18 +5155,18 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -5171,18 +5177,18 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -5193,18 +5199,18 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
@@ -5217,18 +5223,18 @@
         <v>1</v>
       </c>
       <c r="J23" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C24" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
@@ -5241,18 +5247,18 @@
         <v>1</v>
       </c>
       <c r="J24" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C25" t="s" s="4">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
@@ -5265,18 +5271,18 @@
         <v>1</v>
       </c>
       <c r="J25" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
@@ -5289,18 +5295,18 @@
         <v>1</v>
       </c>
       <c r="J26" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4">
@@ -5313,18 +5319,18 @@
         <v>1</v>
       </c>
       <c r="J27" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4">
@@ -5337,18 +5343,18 @@
         <v>1</v>
       </c>
       <c r="J28" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4">
@@ -5361,18 +5367,18 @@
         <v>1</v>
       </c>
       <c r="J29" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C30" t="s" s="4">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4">
@@ -5385,18 +5391,18 @@
         <v>1</v>
       </c>
       <c r="J30" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4">
@@ -5409,18 +5415,18 @@
         <v>1</v>
       </c>
       <c r="J31" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4">
@@ -5433,18 +5439,18 @@
         <v>1</v>
       </c>
       <c r="J32" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4">
@@ -5457,18 +5463,18 @@
         <v>1</v>
       </c>
       <c r="J33" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4">
@@ -5481,18 +5487,18 @@
         <v>1</v>
       </c>
       <c r="J34" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4">
@@ -5505,18 +5511,18 @@
         <v>1</v>
       </c>
       <c r="J35" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4">
@@ -5529,18 +5535,18 @@
         <v>1</v>
       </c>
       <c r="J36" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4">
@@ -5553,18 +5559,18 @@
         <v>1</v>
       </c>
       <c r="J37" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4">
@@ -5577,18 +5583,18 @@
         <v>1</v>
       </c>
       <c r="J38" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4">
@@ -5601,18 +5607,18 @@
         <v>1</v>
       </c>
       <c r="J39" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4">
@@ -5625,18 +5631,18 @@
         <v>1</v>
       </c>
       <c r="J40" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4">
@@ -5649,18 +5655,18 @@
         <v>1</v>
       </c>
       <c r="J41" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4">
@@ -5673,18 +5679,18 @@
         <v>1</v>
       </c>
       <c r="J42" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4">
@@ -5695,18 +5701,18 @@
       <c r="H43" s="5"/>
       <c r="I43" s="6"/>
       <c r="J43" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4">
@@ -5717,18 +5723,18 @@
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
       <c r="J44" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4">
@@ -5739,18 +5745,18 @@
       <c r="H45" s="5"/>
       <c r="I45" s="6"/>
       <c r="J45" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4">
@@ -5761,18 +5767,18 @@
       <c r="H46" s="5"/>
       <c r="I46" s="6"/>
       <c r="J46" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4">
@@ -5783,18 +5789,18 @@
       <c r="H47" s="5"/>
       <c r="I47" s="6"/>
       <c r="J47" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -5805,18 +5811,18 @@
       <c r="H48" s="5"/>
       <c r="I48" s="6"/>
       <c r="J48" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -5827,18 +5833,18 @@
       <c r="H49" s="5"/>
       <c r="I49" s="6"/>
       <c r="J49" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -5849,18 +5855,18 @@
       <c r="H50" s="5"/>
       <c r="I50" s="6"/>
       <c r="J50" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -5871,18 +5877,18 @@
       <c r="H51" s="5"/>
       <c r="I51" s="6"/>
       <c r="J51" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -5893,18 +5899,18 @@
       <c r="H52" s="5"/>
       <c r="I52" s="6"/>
       <c r="J52" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -5915,18 +5921,18 @@
       <c r="H53" s="5"/>
       <c r="I53" s="6"/>
       <c r="J53" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -5937,18 +5943,18 @@
       <c r="H54" s="5"/>
       <c r="I54" s="6"/>
       <c r="J54" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -5959,18 +5965,18 @@
       <c r="H55" s="5"/>
       <c r="I55" s="6"/>
       <c r="J55" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -5981,18 +5987,18 @@
       <c r="H56" s="5"/>
       <c r="I56" s="6"/>
       <c r="J56" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -6003,18 +6009,18 @@
       <c r="H57" s="5"/>
       <c r="I57" s="6"/>
       <c r="J57" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -6025,18 +6031,18 @@
       <c r="H58" s="5"/>
       <c r="I58" s="6"/>
       <c r="J58" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -6047,18 +6053,18 @@
       <c r="H59" s="5"/>
       <c r="I59" s="6"/>
       <c r="J59" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -6069,18 +6075,18 @@
       <c r="H60" s="5"/>
       <c r="I60" s="6"/>
       <c r="J60" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -6091,18 +6097,18 @@
       <c r="H61" s="5"/>
       <c r="I61" s="6"/>
       <c r="J61" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -6113,7 +6119,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="6"/>
       <c r="J62" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -6130,7 +6136,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -6149,16 +6155,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -6189,7 +6195,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -6206,7 +6212,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E4" s="4">
         <v>30</v>
@@ -6223,7 +6229,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s" s="4">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
@@ -6240,7 +6246,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s" s="4">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E6" s="4">
         <v>10</v>
@@ -6257,7 +6263,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
@@ -6274,7 +6280,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E8" s="4">
         <v>2</v>
@@ -6291,7 +6297,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -6308,7 +6314,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E10" s="4">
         <v>50</v>
@@ -6325,7 +6331,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s" s="4">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E11" s="4">
         <v>30</v>
@@ -6342,7 +6348,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E12" s="4">
         <v>20</v>
@@ -6359,7 +6365,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E13" s="4">
         <v>10</v>
@@ -6376,7 +6382,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s" s="4">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
@@ -6393,7 +6399,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="4">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E15" s="4">
         <v>2</v>
@@ -6410,7 +6416,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s" s="4">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -6635,6 +6641,23 @@
       </c>
       <c r="E29" s="4">
         <v>50</v>
+      </c>
+    </row>
+    <row r="30" ht="20" customHeight="1">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s" s="4">
+        <v>99</v>
+      </c>
+      <c r="E30" s="4">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #286 FlixelRL-286 眠りの薬
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="335">
   <si>
     <t>id</t>
   </si>
@@ -328,16 +328,22 @@
     <t>PORTION21</t>
   </si>
   <si>
-    <t>薬21</t>
+    <t>眠り薬</t>
+  </si>
+  <si>
+    <t>sleep</t>
+  </si>
+  <si>
+    <t>飲むと眠くなる薬</t>
+  </si>
+  <si>
+    <t>PORTION22</t>
+  </si>
+  <si>
+    <t>薬22</t>
   </si>
   <si>
     <t>飲むとHPが1回復します</t>
-  </si>
-  <si>
-    <t>PORTION22</t>
-  </si>
-  <si>
-    <t>薬22</t>
   </si>
   <si>
     <t>PORTION23</t>
@@ -3593,9 +3599,7 @@
       <c r="C39" t="s" s="4">
         <v>104</v>
       </c>
-      <c r="D39" s="4">
-        <v>1</v>
-      </c>
+      <c r="D39" s="6"/>
       <c r="E39" s="5">
         <v>10</v>
       </c>
@@ -3603,21 +3607,23 @@
       <c r="G39" s="6"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
+      <c r="J39" t="s" s="4">
+        <v>105</v>
+      </c>
       <c r="K39" s="6"/>
       <c r="L39" t="s" s="4">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D40" s="4">
         <v>1</v>
@@ -3632,18 +3638,18 @@
       <c r="J40" s="5"/>
       <c r="K40" s="6"/>
       <c r="L40" t="s" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B41" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D41" s="4">
         <v>1</v>
@@ -3658,18 +3664,18 @@
       <c r="J41" s="5"/>
       <c r="K41" s="6"/>
       <c r="L41" t="s" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D42" s="4">
         <v>1</v>
@@ -3684,18 +3690,18 @@
       <c r="J42" s="5"/>
       <c r="K42" s="6"/>
       <c r="L42" t="s" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B43" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D43" s="4">
         <v>1</v>
@@ -3710,18 +3716,18 @@
       <c r="J43" s="5"/>
       <c r="K43" s="6"/>
       <c r="L43" t="s" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D44" s="4">
         <v>1</v>
@@ -3736,18 +3742,18 @@
       <c r="J44" s="5"/>
       <c r="K44" s="6"/>
       <c r="L44" t="s" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B45" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D45" s="4">
         <v>1</v>
@@ -3762,18 +3768,18 @@
       <c r="J45" s="5"/>
       <c r="K45" s="6"/>
       <c r="L45" t="s" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B46" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
@@ -3788,18 +3794,18 @@
       <c r="J46" s="5"/>
       <c r="K46" s="6"/>
       <c r="L46" t="s" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B47" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -3814,18 +3820,18 @@
       <c r="J47" s="5"/>
       <c r="K47" s="6"/>
       <c r="L47" t="s" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
@@ -3840,18 +3846,18 @@
       <c r="J48" s="5"/>
       <c r="K48" s="6"/>
       <c r="L48" t="s" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B49" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -3866,18 +3872,18 @@
       <c r="J49" s="5"/>
       <c r="K49" s="6"/>
       <c r="L49" t="s" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
@@ -3892,18 +3898,18 @@
       <c r="J50" s="5"/>
       <c r="K50" s="6"/>
       <c r="L50" t="s" s="4">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5"/>
@@ -3911,25 +3917,25 @@
         <v>10</v>
       </c>
       <c r="G51" t="s" s="4">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="6"/>
       <c r="L51" t="s" s="4">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="5"/>
@@ -3937,25 +3943,25 @@
         <v>30</v>
       </c>
       <c r="G52" t="s" s="4">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="6"/>
       <c r="L52" t="s" s="4">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5"/>
@@ -3963,25 +3969,25 @@
         <v>100</v>
       </c>
       <c r="G53" t="s" s="4">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="6"/>
       <c r="L53" t="s" s="4">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
@@ -3992,18 +3998,18 @@
       <c r="J54" s="5"/>
       <c r="K54" s="6"/>
       <c r="L54" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="5"/>
@@ -4014,18 +4020,18 @@
       <c r="J55" s="5"/>
       <c r="K55" s="6"/>
       <c r="L55" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="5"/>
@@ -4036,18 +4042,18 @@
       <c r="J56" s="5"/>
       <c r="K56" s="6"/>
       <c r="L56" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="5"/>
@@ -4058,18 +4064,18 @@
       <c r="J57" s="5"/>
       <c r="K57" s="6"/>
       <c r="L57" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="5"/>
@@ -4080,18 +4086,18 @@
       <c r="J58" s="5"/>
       <c r="K58" s="6"/>
       <c r="L58" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="5"/>
@@ -4102,18 +4108,18 @@
       <c r="J59" s="5"/>
       <c r="K59" s="6"/>
       <c r="L59" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
@@ -4124,18 +4130,18 @@
       <c r="J60" s="5"/>
       <c r="K60" s="6"/>
       <c r="L60" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5"/>
@@ -4146,18 +4152,18 @@
       <c r="J61" s="5"/>
       <c r="K61" s="6"/>
       <c r="L61" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="5"/>
@@ -4168,18 +4174,18 @@
       <c r="J62" s="5"/>
       <c r="K62" s="6"/>
       <c r="L62" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" t="s" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C63" t="s" s="4">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="5"/>
@@ -4190,18 +4196,18 @@
       <c r="J63" s="5"/>
       <c r="K63" s="6"/>
       <c r="L63" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
       <c r="A64" t="s" s="3">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C64" t="s" s="4">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="5"/>
@@ -4212,18 +4218,18 @@
       <c r="J64" s="5"/>
       <c r="K64" s="6"/>
       <c r="L64" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" t="s" s="3">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C65" t="s" s="4">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="5"/>
@@ -4234,18 +4240,18 @@
       <c r="J65" s="5"/>
       <c r="K65" s="6"/>
       <c r="L65" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" t="s" s="3">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C66" t="s" s="4">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="5"/>
@@ -4256,18 +4262,18 @@
       <c r="J66" s="5"/>
       <c r="K66" s="6"/>
       <c r="L66" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
       <c r="A67" t="s" s="3">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B67" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C67" t="s" s="4">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="5"/>
@@ -4278,18 +4284,18 @@
       <c r="J67" s="5"/>
       <c r="K67" s="6"/>
       <c r="L67" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" ht="20" customHeight="1">
       <c r="A68" t="s" s="3">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B68" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C68" t="s" s="4">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="5"/>
@@ -4300,18 +4306,18 @@
       <c r="J68" s="5"/>
       <c r="K68" s="6"/>
       <c r="L68" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
       <c r="A69" t="s" s="3">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B69" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C69" t="s" s="4">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="5"/>
@@ -4322,18 +4328,18 @@
       <c r="J69" s="5"/>
       <c r="K69" s="6"/>
       <c r="L69" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
       <c r="A70" t="s" s="3">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B70" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C70" t="s" s="4">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="5"/>
@@ -4344,18 +4350,18 @@
       <c r="J70" s="5"/>
       <c r="K70" s="6"/>
       <c r="L70" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
       <c r="A71" t="s" s="3">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C71" t="s" s="4">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="5"/>
@@ -4366,18 +4372,18 @@
       <c r="J71" s="5"/>
       <c r="K71" s="6"/>
       <c r="L71" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="72" ht="20" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C72" t="s" s="4">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="5"/>
@@ -4388,18 +4394,18 @@
       <c r="J72" s="5"/>
       <c r="K72" s="6"/>
       <c r="L72" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" t="s" s="3">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B73" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C73" t="s" s="4">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="5"/>
@@ -4410,18 +4416,18 @@
       <c r="J73" s="5"/>
       <c r="K73" s="6"/>
       <c r="L73" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" ht="20" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B74" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C74" t="s" s="4">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="5"/>
@@ -4432,18 +4438,18 @@
       <c r="J74" s="5"/>
       <c r="K74" s="6"/>
       <c r="L74" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="75" ht="20" customHeight="1">
       <c r="A75" t="s" s="3">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B75" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C75" t="s" s="4">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="5"/>
@@ -4454,18 +4460,18 @@
       <c r="J75" s="5"/>
       <c r="K75" s="6"/>
       <c r="L75" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C76" t="s" s="4">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -4476,18 +4482,18 @@
       <c r="J76" s="5"/>
       <c r="K76" s="6"/>
       <c r="L76" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" t="s" s="3">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B77" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C77" t="s" s="4">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="5"/>
@@ -4498,18 +4504,18 @@
       <c r="J77" s="5"/>
       <c r="K77" s="6"/>
       <c r="L77" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B78" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C78" t="s" s="4">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="5"/>
@@ -4520,18 +4526,18 @@
       <c r="J78" s="5"/>
       <c r="K78" s="6"/>
       <c r="L78" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" t="s" s="3">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C79" t="s" s="4">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="5"/>
@@ -4542,18 +4548,18 @@
       <c r="J79" s="5"/>
       <c r="K79" s="6"/>
       <c r="L79" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B80" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C80" t="s" s="4">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="5"/>
@@ -4564,18 +4570,18 @@
       <c r="J80" s="5"/>
       <c r="K80" s="6"/>
       <c r="L80" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" t="s" s="3">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B81" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C81" t="s" s="4">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="5"/>
@@ -4586,18 +4592,18 @@
       <c r="J81" s="5"/>
       <c r="K81" s="6"/>
       <c r="L81" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B82" t="s" s="4">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C82" t="s" s="4">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="5"/>
@@ -4608,7 +4614,7 @@
       <c r="J82" s="5"/>
       <c r="K82" s="6"/>
       <c r="L82" t="s" s="4">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
@@ -4714,16 +4720,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G1" t="s" s="2">
         <v>9</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>4</v>
@@ -4766,13 +4772,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -4783,18 +4789,18 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C4" t="s" s="4">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -4805,18 +4811,18 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s" s="4">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -4827,18 +4833,18 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
@@ -4849,18 +4855,18 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D7" s="4">
         <v>10</v>
@@ -4871,18 +4877,18 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D8" s="4">
         <v>20</v>
@@ -4893,18 +4899,18 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D9" s="4">
         <v>25</v>
@@ -4915,18 +4921,18 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -4937,18 +4943,18 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -4959,18 +4965,18 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -4981,18 +4987,18 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -5003,18 +5009,18 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -5025,18 +5031,18 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C15" t="s" s="4">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -5047,18 +5053,18 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -5069,18 +5075,18 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C17" t="s" s="4">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -5091,18 +5097,18 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -5113,18 +5119,18 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -5135,18 +5141,18 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -5157,18 +5163,18 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -5179,18 +5185,18 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -5201,18 +5207,18 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" t="s" s="4">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
@@ -5225,18 +5231,18 @@
         <v>1</v>
       </c>
       <c r="J23" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C24" t="s" s="4">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
@@ -5249,18 +5255,18 @@
         <v>1</v>
       </c>
       <c r="J24" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C25" t="s" s="4">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
@@ -5273,18 +5279,18 @@
         <v>1</v>
       </c>
       <c r="J25" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
@@ -5297,18 +5303,18 @@
         <v>1</v>
       </c>
       <c r="J26" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4">
@@ -5321,18 +5327,18 @@
         <v>1</v>
       </c>
       <c r="J27" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4">
@@ -5345,18 +5351,18 @@
         <v>1</v>
       </c>
       <c r="J28" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4">
@@ -5369,18 +5375,18 @@
         <v>1</v>
       </c>
       <c r="J29" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C30" t="s" s="4">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4">
@@ -5393,18 +5399,18 @@
         <v>1</v>
       </c>
       <c r="J30" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4">
@@ -5417,18 +5423,18 @@
         <v>1</v>
       </c>
       <c r="J31" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4">
@@ -5441,18 +5447,18 @@
         <v>1</v>
       </c>
       <c r="J32" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4">
@@ -5465,18 +5471,18 @@
         <v>1</v>
       </c>
       <c r="J33" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4">
@@ -5489,18 +5495,18 @@
         <v>1</v>
       </c>
       <c r="J34" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4">
@@ -5513,18 +5519,18 @@
         <v>1</v>
       </c>
       <c r="J35" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4">
@@ -5537,18 +5543,18 @@
         <v>1</v>
       </c>
       <c r="J36" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4">
@@ -5561,18 +5567,18 @@
         <v>1</v>
       </c>
       <c r="J37" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4">
@@ -5585,18 +5591,18 @@
         <v>1</v>
       </c>
       <c r="J38" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4">
@@ -5609,18 +5615,18 @@
         <v>1</v>
       </c>
       <c r="J39" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4">
@@ -5633,18 +5639,18 @@
         <v>1</v>
       </c>
       <c r="J40" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4">
@@ -5657,18 +5663,18 @@
         <v>1</v>
       </c>
       <c r="J41" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4">
@@ -5681,18 +5687,18 @@
         <v>1</v>
       </c>
       <c r="J42" t="s" s="4">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4">
@@ -5703,18 +5709,18 @@
       <c r="H43" s="5"/>
       <c r="I43" s="6"/>
       <c r="J43" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4">
@@ -5725,18 +5731,18 @@
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
       <c r="J44" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4">
@@ -5747,18 +5753,18 @@
       <c r="H45" s="5"/>
       <c r="I45" s="6"/>
       <c r="J45" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4">
@@ -5769,18 +5775,18 @@
       <c r="H46" s="5"/>
       <c r="I46" s="6"/>
       <c r="J46" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4">
@@ -5791,18 +5797,18 @@
       <c r="H47" s="5"/>
       <c r="I47" s="6"/>
       <c r="J47" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -5813,18 +5819,18 @@
       <c r="H48" s="5"/>
       <c r="I48" s="6"/>
       <c r="J48" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -5835,18 +5841,18 @@
       <c r="H49" s="5"/>
       <c r="I49" s="6"/>
       <c r="J49" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -5857,18 +5863,18 @@
       <c r="H50" s="5"/>
       <c r="I50" s="6"/>
       <c r="J50" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -5879,18 +5885,18 @@
       <c r="H51" s="5"/>
       <c r="I51" s="6"/>
       <c r="J51" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -5901,18 +5907,18 @@
       <c r="H52" s="5"/>
       <c r="I52" s="6"/>
       <c r="J52" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -5923,18 +5929,18 @@
       <c r="H53" s="5"/>
       <c r="I53" s="6"/>
       <c r="J53" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -5945,18 +5951,18 @@
       <c r="H54" s="5"/>
       <c r="I54" s="6"/>
       <c r="J54" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -5967,18 +5973,18 @@
       <c r="H55" s="5"/>
       <c r="I55" s="6"/>
       <c r="J55" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -5989,18 +5995,18 @@
       <c r="H56" s="5"/>
       <c r="I56" s="6"/>
       <c r="J56" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -6011,18 +6017,18 @@
       <c r="H57" s="5"/>
       <c r="I57" s="6"/>
       <c r="J57" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -6033,18 +6039,18 @@
       <c r="H58" s="5"/>
       <c r="I58" s="6"/>
       <c r="J58" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -6055,18 +6061,18 @@
       <c r="H59" s="5"/>
       <c r="I59" s="6"/>
       <c r="J59" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -6077,18 +6083,18 @@
       <c r="H60" s="5"/>
       <c r="I60" s="6"/>
       <c r="J60" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -6099,18 +6105,18 @@
       <c r="H61" s="5"/>
       <c r="I61" s="6"/>
       <c r="J61" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -6121,7 +6127,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="6"/>
       <c r="J62" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -6138,7 +6144,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -6157,16 +6163,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -6197,7 +6203,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -6214,7 +6220,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E4" s="4">
         <v>30</v>
@@ -6231,7 +6237,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s" s="4">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
@@ -6248,7 +6254,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s" s="4">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E6" s="4">
         <v>10</v>
@@ -6265,7 +6271,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
@@ -6282,7 +6288,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E8" s="4">
         <v>2</v>
@@ -6299,7 +6305,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -6316,7 +6322,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E10" s="4">
         <v>50</v>
@@ -6333,7 +6339,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s" s="4">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E11" s="4">
         <v>30</v>
@@ -6350,7 +6356,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E12" s="4">
         <v>20</v>
@@ -6367,7 +6373,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E13" s="4">
         <v>10</v>
@@ -6384,7 +6390,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s" s="4">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
@@ -6401,7 +6407,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="4">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E15" s="4">
         <v>2</v>
@@ -6418,7 +6424,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s" s="4">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -6659,6 +6665,23 @@
         <v>100</v>
       </c>
       <c r="E30" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" ht="20" customHeight="1">
+      <c r="A31" s="3">
+        <v>29</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s" s="4">
+        <v>103</v>
+      </c>
+      <c r="E31" s="4">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed #287 FlixelRL-287 しびれ薬
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="343">
   <si>
     <t>id</t>
   </si>
@@ -340,34 +340,58 @@
     <t>PORTION22</t>
   </si>
   <si>
-    <t>薬22</t>
+    <t>しびれ薬</t>
+  </si>
+  <si>
+    <t>paralysis</t>
+  </si>
+  <si>
+    <t>しびれて動けなくなります</t>
+  </si>
+  <si>
+    <t>PORTION23</t>
+  </si>
+  <si>
+    <t>混乱の薬</t>
+  </si>
+  <si>
+    <t>confusion</t>
+  </si>
+  <si>
+    <t>混乱する薬</t>
+  </si>
+  <si>
+    <t>PORTION24</t>
+  </si>
+  <si>
+    <t>怒りの薬</t>
+  </si>
+  <si>
+    <t>anger</t>
+  </si>
+  <si>
+    <t>怒り状態になります</t>
+  </si>
+  <si>
+    <t>PORTION25</t>
+  </si>
+  <si>
+    <t>元気になる薬</t>
+  </si>
+  <si>
+    <t>powerful</t>
+  </si>
+  <si>
+    <t>元気状態になります</t>
+  </si>
+  <si>
+    <t>PORTION26</t>
+  </si>
+  <si>
+    <t>薬26</t>
   </si>
   <si>
     <t>飲むとHPが1回復します</t>
-  </si>
-  <si>
-    <t>PORTION23</t>
-  </si>
-  <si>
-    <t>薬23</t>
-  </si>
-  <si>
-    <t>PORTION24</t>
-  </si>
-  <si>
-    <t>薬24</t>
-  </si>
-  <si>
-    <t>PORTION25</t>
-  </si>
-  <si>
-    <t>薬25</t>
-  </si>
-  <si>
-    <t>PORTION26</t>
-  </si>
-  <si>
-    <t>薬26</t>
   </si>
   <si>
     <t>PORTION27</t>
@@ -2563,7 +2587,7 @@
     <col min="7" max="7" width="4.75" style="1" customWidth="1"/>
     <col min="8" max="8" width="4.75" style="1" customWidth="1"/>
     <col min="9" max="9" width="5.75" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.75" style="1" customWidth="1"/>
     <col min="11" max="11" width="4.75" style="1" customWidth="1"/>
     <col min="12" max="12" width="31.2812" style="1" customWidth="1"/>
     <col min="13" max="256" width="9" style="1" customWidth="1"/>
@@ -3625,9 +3649,7 @@
       <c r="C40" t="s" s="4">
         <v>108</v>
       </c>
-      <c r="D40" s="4">
-        <v>1</v>
-      </c>
+      <c r="D40" s="6"/>
       <c r="E40" s="5">
         <v>10</v>
       </c>
@@ -3635,25 +3657,25 @@
       <c r="G40" s="6"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
+      <c r="J40" t="s" s="4">
+        <v>109</v>
+      </c>
       <c r="K40" s="6"/>
       <c r="L40" t="s" s="4">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>111</v>
-      </c>
-      <c r="D41" s="4">
-        <v>1</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="D41" s="6"/>
       <c r="E41" s="5">
         <v>10</v>
       </c>
@@ -3661,25 +3683,25 @@
       <c r="G41" s="6"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
+      <c r="J41" t="s" s="4">
+        <v>113</v>
+      </c>
       <c r="K41" s="6"/>
       <c r="L41" t="s" s="4">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>113</v>
-      </c>
-      <c r="D42" s="4">
-        <v>1</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D42" s="6"/>
       <c r="E42" s="5">
         <v>10</v>
       </c>
@@ -3687,25 +3709,25 @@
       <c r="G42" s="6"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
+      <c r="J42" t="s" s="4">
+        <v>117</v>
+      </c>
       <c r="K42" s="6"/>
       <c r="L42" t="s" s="4">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B43" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>115</v>
-      </c>
-      <c r="D43" s="4">
-        <v>1</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D43" s="6"/>
       <c r="E43" s="5">
         <v>10</v>
       </c>
@@ -3713,21 +3735,23 @@
       <c r="G43" s="6"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
+      <c r="J43" t="s" s="4">
+        <v>121</v>
+      </c>
       <c r="K43" s="6"/>
       <c r="L43" t="s" s="4">
-        <v>109</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B44" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D44" s="4">
         <v>1</v>
@@ -3742,18 +3766,18 @@
       <c r="J44" s="5"/>
       <c r="K44" s="6"/>
       <c r="L44" t="s" s="4">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D45" s="4">
         <v>1</v>
@@ -3768,18 +3792,18 @@
       <c r="J45" s="5"/>
       <c r="K45" s="6"/>
       <c r="L45" t="s" s="4">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B46" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
@@ -3794,18 +3818,18 @@
       <c r="J46" s="5"/>
       <c r="K46" s="6"/>
       <c r="L46" t="s" s="4">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B47" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -3820,18 +3844,18 @@
       <c r="J47" s="5"/>
       <c r="K47" s="6"/>
       <c r="L47" t="s" s="4">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
@@ -3846,18 +3870,18 @@
       <c r="J48" s="5"/>
       <c r="K48" s="6"/>
       <c r="L48" t="s" s="4">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B49" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -3872,18 +3896,18 @@
       <c r="J49" s="5"/>
       <c r="K49" s="6"/>
       <c r="L49" t="s" s="4">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>42</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
@@ -3898,18 +3922,18 @@
       <c r="J50" s="5"/>
       <c r="K50" s="6"/>
       <c r="L50" t="s" s="4">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5"/>
@@ -3917,25 +3941,25 @@
         <v>10</v>
       </c>
       <c r="G51" t="s" s="4">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="6"/>
       <c r="L51" t="s" s="4">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="5"/>
@@ -3943,25 +3967,25 @@
         <v>30</v>
       </c>
       <c r="G52" t="s" s="4">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="6"/>
       <c r="L52" t="s" s="4">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5"/>
@@ -3969,25 +3993,25 @@
         <v>100</v>
       </c>
       <c r="G53" t="s" s="4">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="6"/>
       <c r="L53" t="s" s="4">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
@@ -3998,18 +4022,18 @@
       <c r="J54" s="5"/>
       <c r="K54" s="6"/>
       <c r="L54" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="5"/>
@@ -4020,18 +4044,18 @@
       <c r="J55" s="5"/>
       <c r="K55" s="6"/>
       <c r="L55" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="5"/>
@@ -4042,18 +4066,18 @@
       <c r="J56" s="5"/>
       <c r="K56" s="6"/>
       <c r="L56" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="5"/>
@@ -4064,18 +4088,18 @@
       <c r="J57" s="5"/>
       <c r="K57" s="6"/>
       <c r="L57" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="5"/>
@@ -4086,18 +4110,18 @@
       <c r="J58" s="5"/>
       <c r="K58" s="6"/>
       <c r="L58" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="5"/>
@@ -4108,18 +4132,18 @@
       <c r="J59" s="5"/>
       <c r="K59" s="6"/>
       <c r="L59" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
@@ -4130,18 +4154,18 @@
       <c r="J60" s="5"/>
       <c r="K60" s="6"/>
       <c r="L60" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5"/>
@@ -4152,18 +4176,18 @@
       <c r="J61" s="5"/>
       <c r="K61" s="6"/>
       <c r="L61" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="5"/>
@@ -4174,18 +4198,18 @@
       <c r="J62" s="5"/>
       <c r="K62" s="6"/>
       <c r="L62" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" t="s" s="3">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C63" t="s" s="4">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="5"/>
@@ -4196,18 +4220,18 @@
       <c r="J63" s="5"/>
       <c r="K63" s="6"/>
       <c r="L63" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
       <c r="A64" t="s" s="3">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C64" t="s" s="4">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="5"/>
@@ -4218,18 +4242,18 @@
       <c r="J64" s="5"/>
       <c r="K64" s="6"/>
       <c r="L64" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" t="s" s="3">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C65" t="s" s="4">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="5"/>
@@ -4240,18 +4264,18 @@
       <c r="J65" s="5"/>
       <c r="K65" s="6"/>
       <c r="L65" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" t="s" s="3">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C66" t="s" s="4">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="5"/>
@@ -4262,18 +4286,18 @@
       <c r="J66" s="5"/>
       <c r="K66" s="6"/>
       <c r="L66" t="s" s="4">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
       <c r="A67" t="s" s="3">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B67" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C67" t="s" s="4">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="5"/>
@@ -4284,18 +4308,18 @@
       <c r="J67" s="5"/>
       <c r="K67" s="6"/>
       <c r="L67" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" ht="20" customHeight="1">
       <c r="A68" t="s" s="3">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B68" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C68" t="s" s="4">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="5"/>
@@ -4306,18 +4330,18 @@
       <c r="J68" s="5"/>
       <c r="K68" s="6"/>
       <c r="L68" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
       <c r="A69" t="s" s="3">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B69" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C69" t="s" s="4">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="5"/>
@@ -4328,18 +4352,18 @@
       <c r="J69" s="5"/>
       <c r="K69" s="6"/>
       <c r="L69" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
       <c r="A70" t="s" s="3">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B70" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C70" t="s" s="4">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="5"/>
@@ -4350,18 +4374,18 @@
       <c r="J70" s="5"/>
       <c r="K70" s="6"/>
       <c r="L70" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
       <c r="A71" t="s" s="3">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C71" t="s" s="4">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="5"/>
@@ -4372,18 +4396,18 @@
       <c r="J71" s="5"/>
       <c r="K71" s="6"/>
       <c r="L71" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="72" ht="20" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C72" t="s" s="4">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="5"/>
@@ -4394,18 +4418,18 @@
       <c r="J72" s="5"/>
       <c r="K72" s="6"/>
       <c r="L72" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" t="s" s="3">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B73" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C73" t="s" s="4">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="5"/>
@@ -4416,18 +4440,18 @@
       <c r="J73" s="5"/>
       <c r="K73" s="6"/>
       <c r="L73" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" ht="20" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B74" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C74" t="s" s="4">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="5"/>
@@ -4438,18 +4462,18 @@
       <c r="J74" s="5"/>
       <c r="K74" s="6"/>
       <c r="L74" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="75" ht="20" customHeight="1">
       <c r="A75" t="s" s="3">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B75" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C75" t="s" s="4">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="5"/>
@@ -4460,18 +4484,18 @@
       <c r="J75" s="5"/>
       <c r="K75" s="6"/>
       <c r="L75" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C76" t="s" s="4">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -4482,18 +4506,18 @@
       <c r="J76" s="5"/>
       <c r="K76" s="6"/>
       <c r="L76" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" t="s" s="3">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B77" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C77" t="s" s="4">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="5"/>
@@ -4504,18 +4528,18 @@
       <c r="J77" s="5"/>
       <c r="K77" s="6"/>
       <c r="L77" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B78" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C78" t="s" s="4">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="5"/>
@@ -4526,18 +4550,18 @@
       <c r="J78" s="5"/>
       <c r="K78" s="6"/>
       <c r="L78" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" t="s" s="3">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C79" t="s" s="4">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="5"/>
@@ -4548,18 +4572,18 @@
       <c r="J79" s="5"/>
       <c r="K79" s="6"/>
       <c r="L79" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B80" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C80" t="s" s="4">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="5"/>
@@ -4570,18 +4594,18 @@
       <c r="J80" s="5"/>
       <c r="K80" s="6"/>
       <c r="L80" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" t="s" s="3">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B81" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C81" t="s" s="4">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="5"/>
@@ -4592,18 +4616,18 @@
       <c r="J81" s="5"/>
       <c r="K81" s="6"/>
       <c r="L81" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B82" t="s" s="4">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C82" t="s" s="4">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="5"/>
@@ -4614,7 +4638,7 @@
       <c r="J82" s="5"/>
       <c r="K82" s="6"/>
       <c r="L82" t="s" s="4">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
@@ -4720,16 +4744,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="G1" t="s" s="2">
         <v>9</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>4</v>
@@ -4772,13 +4796,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -4789,18 +4813,18 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C4" t="s" s="4">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -4811,18 +4835,18 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C5" t="s" s="4">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -4833,18 +4857,18 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
@@ -4855,18 +4879,18 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D7" s="4">
         <v>10</v>
@@ -4877,18 +4901,18 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="D8" s="4">
         <v>20</v>
@@ -4899,18 +4923,18 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D9" s="4">
         <v>25</v>
@@ -4921,18 +4945,18 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -4943,18 +4967,18 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -4965,18 +4989,18 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -4987,18 +5011,18 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -5009,18 +5033,18 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -5031,18 +5055,18 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C15" t="s" s="4">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -5053,18 +5077,18 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -5075,18 +5099,18 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C17" t="s" s="4">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -5097,18 +5121,18 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -5119,18 +5143,18 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -5141,18 +5165,18 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -5163,18 +5187,18 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -5185,18 +5209,18 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -5207,18 +5231,18 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" t="s" s="4">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
@@ -5231,18 +5255,18 @@
         <v>1</v>
       </c>
       <c r="J23" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C24" t="s" s="4">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
@@ -5255,18 +5279,18 @@
         <v>1</v>
       </c>
       <c r="J24" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C25" t="s" s="4">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
@@ -5279,18 +5303,18 @@
         <v>1</v>
       </c>
       <c r="J25" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
@@ -5303,18 +5327,18 @@
         <v>1</v>
       </c>
       <c r="J26" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4">
@@ -5327,18 +5351,18 @@
         <v>1</v>
       </c>
       <c r="J27" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4">
@@ -5351,18 +5375,18 @@
         <v>1</v>
       </c>
       <c r="J28" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4">
@@ -5375,18 +5399,18 @@
         <v>1</v>
       </c>
       <c r="J29" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C30" t="s" s="4">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4">
@@ -5399,18 +5423,18 @@
         <v>1</v>
       </c>
       <c r="J30" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4">
@@ -5423,18 +5447,18 @@
         <v>1</v>
       </c>
       <c r="J31" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4">
@@ -5447,18 +5471,18 @@
         <v>1</v>
       </c>
       <c r="J32" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4">
@@ -5471,18 +5495,18 @@
         <v>1</v>
       </c>
       <c r="J33" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4">
@@ -5495,18 +5519,18 @@
         <v>1</v>
       </c>
       <c r="J34" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4">
@@ -5519,18 +5543,18 @@
         <v>1</v>
       </c>
       <c r="J35" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4">
@@ -5543,18 +5567,18 @@
         <v>1</v>
       </c>
       <c r="J36" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4">
@@ -5567,18 +5591,18 @@
         <v>1</v>
       </c>
       <c r="J37" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4">
@@ -5591,18 +5615,18 @@
         <v>1</v>
       </c>
       <c r="J38" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4">
@@ -5615,18 +5639,18 @@
         <v>1</v>
       </c>
       <c r="J39" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4">
@@ -5639,18 +5663,18 @@
         <v>1</v>
       </c>
       <c r="J40" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4">
@@ -5663,18 +5687,18 @@
         <v>1</v>
       </c>
       <c r="J41" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4">
@@ -5687,18 +5711,18 @@
         <v>1</v>
       </c>
       <c r="J42" t="s" s="4">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4">
@@ -5709,18 +5733,18 @@
       <c r="H43" s="5"/>
       <c r="I43" s="6"/>
       <c r="J43" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4">
@@ -5731,18 +5755,18 @@
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
       <c r="J44" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4">
@@ -5753,18 +5777,18 @@
       <c r="H45" s="5"/>
       <c r="I45" s="6"/>
       <c r="J45" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4">
@@ -5775,18 +5799,18 @@
       <c r="H46" s="5"/>
       <c r="I46" s="6"/>
       <c r="J46" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4">
@@ -5797,18 +5821,18 @@
       <c r="H47" s="5"/>
       <c r="I47" s="6"/>
       <c r="J47" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -5819,18 +5843,18 @@
       <c r="H48" s="5"/>
       <c r="I48" s="6"/>
       <c r="J48" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -5841,18 +5865,18 @@
       <c r="H49" s="5"/>
       <c r="I49" s="6"/>
       <c r="J49" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -5863,18 +5887,18 @@
       <c r="H50" s="5"/>
       <c r="I50" s="6"/>
       <c r="J50" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -5885,18 +5909,18 @@
       <c r="H51" s="5"/>
       <c r="I51" s="6"/>
       <c r="J51" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -5907,18 +5931,18 @@
       <c r="H52" s="5"/>
       <c r="I52" s="6"/>
       <c r="J52" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -5929,18 +5953,18 @@
       <c r="H53" s="5"/>
       <c r="I53" s="6"/>
       <c r="J53" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -5951,18 +5975,18 @@
       <c r="H54" s="5"/>
       <c r="I54" s="6"/>
       <c r="J54" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -5973,18 +5997,18 @@
       <c r="H55" s="5"/>
       <c r="I55" s="6"/>
       <c r="J55" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -5995,18 +6019,18 @@
       <c r="H56" s="5"/>
       <c r="I56" s="6"/>
       <c r="J56" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -6017,18 +6041,18 @@
       <c r="H57" s="5"/>
       <c r="I57" s="6"/>
       <c r="J57" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -6039,18 +6063,18 @@
       <c r="H58" s="5"/>
       <c r="I58" s="6"/>
       <c r="J58" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -6061,18 +6085,18 @@
       <c r="H59" s="5"/>
       <c r="I59" s="6"/>
       <c r="J59" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -6083,18 +6107,18 @@
       <c r="H60" s="5"/>
       <c r="I60" s="6"/>
       <c r="J60" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -6105,18 +6129,18 @@
       <c r="H61" s="5"/>
       <c r="I61" s="6"/>
       <c r="J61" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -6127,7 +6151,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="6"/>
       <c r="J62" t="s" s="4">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -6144,7 +6168,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -6163,16 +6187,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>334</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -6203,7 +6227,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -6220,7 +6244,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="E4" s="4">
         <v>30</v>
@@ -6237,7 +6261,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s" s="4">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
@@ -6254,7 +6278,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s" s="4">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="E6" s="4">
         <v>10</v>
@@ -6271,7 +6295,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
@@ -6288,7 +6312,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="E8" s="4">
         <v>2</v>
@@ -6305,7 +6329,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -6322,7 +6346,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="E10" s="4">
         <v>50</v>
@@ -6339,7 +6363,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s" s="4">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="E11" s="4">
         <v>30</v>
@@ -6356,7 +6380,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="E12" s="4">
         <v>20</v>
@@ -6373,7 +6397,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="E13" s="4">
         <v>10</v>
@@ -6390,7 +6414,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s" s="4">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
@@ -6407,7 +6431,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="4">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E15" s="4">
         <v>2</v>
@@ -6424,7 +6448,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s" s="4">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -6682,6 +6706,74 @@
         <v>103</v>
       </c>
       <c r="E31" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" ht="20" customHeight="1">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s" s="4">
+        <v>107</v>
+      </c>
+      <c r="E32" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" ht="20" customHeight="1">
+      <c r="A33" s="3">
+        <v>31</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s" s="4">
+        <v>111</v>
+      </c>
+      <c r="E33" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" ht="20" customHeight="1">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s" s="4">
+        <v>115</v>
+      </c>
+      <c r="E34" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" ht="20" customHeight="1">
+      <c r="A35" s="3">
+        <v>33</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s" s="4">
+        <v>119</v>
+      </c>
+      <c r="E35" s="4">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed #262 FlixelRL-262 杖の実装
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="348">
   <si>
     <t>id</t>
   </si>
@@ -550,40 +550,55 @@
     <t>Wand</t>
   </si>
   <si>
-    <t>杖1</t>
+    <t>毒の杖</t>
+  </si>
+  <si>
+    <t>相手を毒状態にします</t>
+  </si>
+  <si>
+    <t>WAND2</t>
+  </si>
+  <si>
+    <t>眠りの杖</t>
+  </si>
+  <si>
+    <t>相手を眠らせます</t>
+  </si>
+  <si>
+    <t>WAND3</t>
+  </si>
+  <si>
+    <t>麻痺の杖</t>
+  </si>
+  <si>
+    <t>相手を麻痺させます</t>
+  </si>
+  <si>
+    <t>WAND4</t>
+  </si>
+  <si>
+    <t>混乱の杖</t>
+  </si>
+  <si>
+    <t>相手を混乱させます</t>
+  </si>
+  <si>
+    <t>WAND5</t>
+  </si>
+  <si>
+    <t>怒りの杖</t>
+  </si>
+  <si>
+    <t>相手を怒り状態にします</t>
+  </si>
+  <si>
+    <t>WAND6</t>
+  </si>
+  <si>
+    <t>杖6</t>
   </si>
   <si>
     <t>杖の説明文</t>
-  </si>
-  <si>
-    <t>WAND2</t>
-  </si>
-  <si>
-    <t>杖2</t>
-  </si>
-  <si>
-    <t>WAND3</t>
-  </si>
-  <si>
-    <t>杖3</t>
-  </si>
-  <si>
-    <t>WAND4</t>
-  </si>
-  <si>
-    <t>杖4</t>
-  </si>
-  <si>
-    <t>WAND5</t>
-  </si>
-  <si>
-    <t>杖5</t>
-  </si>
-  <si>
-    <t>WAND6</t>
-  </si>
-  <si>
-    <t>杖6</t>
   </si>
   <si>
     <t>WAND7</t>
@@ -1257,7 +1272,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1319,6 +1334,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4305,7 +4323,9 @@
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
+      <c r="J67" t="s" s="4">
+        <v>26</v>
+      </c>
       <c r="K67" s="6"/>
       <c r="L67" t="s" s="4">
         <v>179</v>
@@ -4327,21 +4347,23 @@
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
+      <c r="J68" t="s" s="4">
+        <v>105</v>
+      </c>
       <c r="K68" s="6"/>
       <c r="L68" t="s" s="4">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
       <c r="A69" t="s" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B69" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C69" t="s" s="4">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="5"/>
@@ -4349,21 +4371,23 @@
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
+      <c r="J69" t="s" s="4">
+        <v>109</v>
+      </c>
       <c r="K69" s="6"/>
       <c r="L69" t="s" s="4">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
       <c r="A70" t="s" s="3">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B70" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C70" t="s" s="4">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="5"/>
@@ -4371,21 +4395,23 @@
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
+      <c r="J70" t="s" s="4">
+        <v>113</v>
+      </c>
       <c r="K70" s="6"/>
       <c r="L70" t="s" s="4">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
       <c r="A71" t="s" s="3">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B71" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C71" t="s" s="4">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="5"/>
@@ -4393,21 +4419,23 @@
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
+      <c r="J71" t="s" s="4">
+        <v>117</v>
+      </c>
       <c r="K71" s="6"/>
       <c r="L71" t="s" s="4">
-        <v>179</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" ht="20" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B72" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C72" t="s" s="4">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="5"/>
@@ -4418,18 +4446,18 @@
       <c r="J72" s="5"/>
       <c r="K72" s="6"/>
       <c r="L72" t="s" s="4">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" t="s" s="3">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B73" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C73" t="s" s="4">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="5"/>
@@ -4440,18 +4468,18 @@
       <c r="J73" s="5"/>
       <c r="K73" s="6"/>
       <c r="L73" t="s" s="4">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" ht="20" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B74" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C74" t="s" s="4">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="5"/>
@@ -4462,18 +4490,18 @@
       <c r="J74" s="5"/>
       <c r="K74" s="6"/>
       <c r="L74" t="s" s="4">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="75" ht="20" customHeight="1">
       <c r="A75" t="s" s="3">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B75" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C75" t="s" s="4">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="5"/>
@@ -4484,18 +4512,18 @@
       <c r="J75" s="5"/>
       <c r="K75" s="6"/>
       <c r="L75" t="s" s="4">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B76" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C76" t="s" s="4">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -4506,18 +4534,18 @@
       <c r="J76" s="5"/>
       <c r="K76" s="6"/>
       <c r="L76" t="s" s="4">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" t="s" s="3">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B77" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C77" t="s" s="4">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="5"/>
@@ -4528,18 +4556,18 @@
       <c r="J77" s="5"/>
       <c r="K77" s="6"/>
       <c r="L77" t="s" s="4">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B78" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C78" t="s" s="4">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="5"/>
@@ -4550,18 +4578,18 @@
       <c r="J78" s="5"/>
       <c r="K78" s="6"/>
       <c r="L78" t="s" s="4">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" t="s" s="3">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B79" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C79" t="s" s="4">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="5"/>
@@ -4572,18 +4600,18 @@
       <c r="J79" s="5"/>
       <c r="K79" s="6"/>
       <c r="L79" t="s" s="4">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B80" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C80" t="s" s="4">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="5"/>
@@ -4594,18 +4622,18 @@
       <c r="J80" s="5"/>
       <c r="K80" s="6"/>
       <c r="L80" t="s" s="4">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" t="s" s="3">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B81" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C81" t="s" s="4">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="5"/>
@@ -4616,18 +4644,18 @@
       <c r="J81" s="5"/>
       <c r="K81" s="6"/>
       <c r="L81" t="s" s="4">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="B82" t="s" s="4">
         <v>177</v>
       </c>
       <c r="C82" t="s" s="4">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="5"/>
@@ -4638,7 +4666,7 @@
       <c r="J82" s="5"/>
       <c r="K82" s="6"/>
       <c r="L82" t="s" s="4">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
@@ -4744,16 +4772,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="G1" t="s" s="2">
         <v>9</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>4</v>
@@ -4796,13 +4824,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -4813,18 +4841,18 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C4" t="s" s="4">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -4835,18 +4863,18 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
+        <v>224</v>
+      </c>
+      <c r="B5" t="s" s="4">
         <v>219</v>
       </c>
-      <c r="B5" t="s" s="4">
-        <v>214</v>
-      </c>
       <c r="C5" t="s" s="4">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -4857,18 +4885,18 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
@@ -4879,18 +4907,18 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="D7" s="4">
         <v>10</v>
@@ -4901,18 +4929,18 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="D8" s="4">
         <v>20</v>
@@ -4923,18 +4951,18 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="D9" s="4">
         <v>25</v>
@@ -4945,18 +4973,18 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -4967,18 +4995,18 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -4989,18 +5017,18 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -5011,18 +5039,18 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -5033,18 +5061,18 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -5055,18 +5083,18 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C15" t="s" s="4">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -5077,18 +5105,18 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -5099,18 +5127,18 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C17" t="s" s="4">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -5121,18 +5149,18 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -5143,18 +5171,18 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -5165,18 +5193,18 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -5187,18 +5215,18 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -5209,18 +5237,18 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -5231,18 +5259,18 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" t="s" s="4">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
@@ -5255,18 +5283,18 @@
         <v>1</v>
       </c>
       <c r="J23" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C24" t="s" s="4">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
@@ -5279,18 +5307,18 @@
         <v>1</v>
       </c>
       <c r="J24" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
+        <v>266</v>
+      </c>
+      <c r="B25" t="s" s="4">
         <v>261</v>
       </c>
-      <c r="B25" t="s" s="4">
-        <v>256</v>
-      </c>
       <c r="C25" t="s" s="4">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
@@ -5303,18 +5331,18 @@
         <v>1</v>
       </c>
       <c r="J25" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
@@ -5327,18 +5355,18 @@
         <v>1</v>
       </c>
       <c r="J26" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4">
@@ -5351,18 +5379,18 @@
         <v>1</v>
       </c>
       <c r="J27" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4">
@@ -5375,18 +5403,18 @@
         <v>1</v>
       </c>
       <c r="J28" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4">
@@ -5399,18 +5427,18 @@
         <v>1</v>
       </c>
       <c r="J29" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C30" t="s" s="4">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4">
@@ -5423,18 +5451,18 @@
         <v>1</v>
       </c>
       <c r="J30" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4">
@@ -5447,18 +5475,18 @@
         <v>1</v>
       </c>
       <c r="J31" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4">
@@ -5471,18 +5499,18 @@
         <v>1</v>
       </c>
       <c r="J32" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4">
@@ -5495,18 +5523,18 @@
         <v>1</v>
       </c>
       <c r="J33" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4">
@@ -5519,18 +5547,18 @@
         <v>1</v>
       </c>
       <c r="J34" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4">
@@ -5543,18 +5571,18 @@
         <v>1</v>
       </c>
       <c r="J35" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4">
@@ -5567,18 +5595,18 @@
         <v>1</v>
       </c>
       <c r="J36" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4">
@@ -5591,18 +5619,18 @@
         <v>1</v>
       </c>
       <c r="J37" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4">
@@ -5615,18 +5643,18 @@
         <v>1</v>
       </c>
       <c r="J38" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4">
@@ -5639,18 +5667,18 @@
         <v>1</v>
       </c>
       <c r="J39" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4">
@@ -5663,18 +5691,18 @@
         <v>1</v>
       </c>
       <c r="J40" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4">
@@ -5687,18 +5715,18 @@
         <v>1</v>
       </c>
       <c r="J41" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4">
@@ -5711,18 +5739,18 @@
         <v>1</v>
       </c>
       <c r="J42" t="s" s="4">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4">
@@ -5733,18 +5761,18 @@
       <c r="H43" s="5"/>
       <c r="I43" s="6"/>
       <c r="J43" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4">
@@ -5755,18 +5783,18 @@
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
       <c r="J44" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
+        <v>308</v>
+      </c>
+      <c r="B45" t="s" s="4">
         <v>303</v>
       </c>
-      <c r="B45" t="s" s="4">
-        <v>298</v>
-      </c>
       <c r="C45" t="s" s="4">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4">
@@ -5777,18 +5805,18 @@
       <c r="H45" s="5"/>
       <c r="I45" s="6"/>
       <c r="J45" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4">
@@ -5799,18 +5827,18 @@
       <c r="H46" s="5"/>
       <c r="I46" s="6"/>
       <c r="J46" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4">
@@ -5821,18 +5849,18 @@
       <c r="H47" s="5"/>
       <c r="I47" s="6"/>
       <c r="J47" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -5843,18 +5871,18 @@
       <c r="H48" s="5"/>
       <c r="I48" s="6"/>
       <c r="J48" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -5865,18 +5893,18 @@
       <c r="H49" s="5"/>
       <c r="I49" s="6"/>
       <c r="J49" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -5887,18 +5915,18 @@
       <c r="H50" s="5"/>
       <c r="I50" s="6"/>
       <c r="J50" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -5909,18 +5937,18 @@
       <c r="H51" s="5"/>
       <c r="I51" s="6"/>
       <c r="J51" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -5931,18 +5959,18 @@
       <c r="H52" s="5"/>
       <c r="I52" s="6"/>
       <c r="J52" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -5953,18 +5981,18 @@
       <c r="H53" s="5"/>
       <c r="I53" s="6"/>
       <c r="J53" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -5975,18 +6003,18 @@
       <c r="H54" s="5"/>
       <c r="I54" s="6"/>
       <c r="J54" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -5997,18 +6025,18 @@
       <c r="H55" s="5"/>
       <c r="I55" s="6"/>
       <c r="J55" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -6019,18 +6047,18 @@
       <c r="H56" s="5"/>
       <c r="I56" s="6"/>
       <c r="J56" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -6041,18 +6069,18 @@
       <c r="H57" s="5"/>
       <c r="I57" s="6"/>
       <c r="J57" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -6063,18 +6091,18 @@
       <c r="H58" s="5"/>
       <c r="I58" s="6"/>
       <c r="J58" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -6085,18 +6113,18 @@
       <c r="H59" s="5"/>
       <c r="I59" s="6"/>
       <c r="J59" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -6107,18 +6135,18 @@
       <c r="H60" s="5"/>
       <c r="I60" s="6"/>
       <c r="J60" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -6129,18 +6157,18 @@
       <c r="H61" s="5"/>
       <c r="I61" s="6"/>
       <c r="J61" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -6151,7 +6179,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="6"/>
       <c r="J62" t="s" s="4">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -6168,7 +6196,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -6187,16 +6215,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -6227,7 +6255,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -6244,7 +6272,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E4" s="4">
         <v>30</v>
@@ -6261,7 +6289,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s" s="4">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
@@ -6278,7 +6306,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s" s="4">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E6" s="4">
         <v>10</v>
@@ -6295,7 +6323,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
@@ -6312,7 +6340,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="E8" s="4">
         <v>2</v>
@@ -6329,7 +6357,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -6346,7 +6374,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="E10" s="4">
         <v>50</v>
@@ -6363,7 +6391,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s" s="4">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="E11" s="4">
         <v>30</v>
@@ -6380,7 +6408,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="E12" s="4">
         <v>20</v>
@@ -6397,7 +6425,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="E13" s="4">
         <v>10</v>
@@ -6414,7 +6442,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s" s="4">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
@@ -6431,7 +6459,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="4">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="E15" s="4">
         <v>2</v>
@@ -6448,7 +6476,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s" s="4">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -6776,6 +6804,81 @@
       <c r="E35" s="4">
         <v>20</v>
       </c>
+    </row>
+    <row r="36" ht="20" customHeight="1">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="C36" s="4">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s" s="4">
+        <v>176</v>
+      </c>
+      <c r="E36" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" ht="20" customHeight="1">
+      <c r="A37" s="3">
+        <v>35</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s" s="4">
+        <v>180</v>
+      </c>
+      <c r="E37" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" ht="20" customHeight="1">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s" s="4">
+        <v>183</v>
+      </c>
+      <c r="E38" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" ht="20" customHeight="1">
+      <c r="A39" s="3">
+        <v>37</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s" s="4">
+        <v>186</v>
+      </c>
+      <c r="E39" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" ht="20" customHeight="1">
+      <c r="A40" s="21"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed #359 FlixelRL-359 封印の薬を実装する
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="391">
   <si>
     <t>id</t>
   </si>
@@ -403,18 +403,24 @@
     <t>PORTION27</t>
   </si>
   <si>
-    <t>薬27</t>
+    <t>封印の薬</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>封印状態になります</t>
+  </si>
+  <si>
+    <t>PORTION28</t>
+  </si>
+  <si>
+    <t>薬28</t>
   </si>
   <si>
     <t>飲むとHPが1回復します</t>
   </si>
   <si>
-    <t>PORTION28</t>
-  </si>
-  <si>
-    <t>薬28</t>
-  </si>
-  <si>
     <t>PORTION29</t>
   </si>
   <si>
@@ -613,16 +619,19 @@
     <t>WAND7</t>
   </si>
   <si>
-    <t>杖7</t>
+    <t>封印の杖</t>
+  </si>
+  <si>
+    <t>相手を封印状態にします</t>
+  </si>
+  <si>
+    <t>WAND8</t>
+  </si>
+  <si>
+    <t>杖8</t>
   </si>
   <si>
     <t>杖の説明文</t>
-  </si>
-  <si>
-    <t>WAND8</t>
-  </si>
-  <si>
-    <t>杖8</t>
   </si>
   <si>
     <t>WAND9</t>
@@ -4096,39 +4105,39 @@
       <c r="C45" t="s" s="4">
         <v>129</v>
       </c>
-      <c r="D45" s="4">
-        <v>1</v>
-      </c>
+      <c r="D45" s="6"/>
       <c r="E45" s="5">
         <v>10</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="5"/>
+      <c r="H45" t="s" s="4">
+        <v>130</v>
+      </c>
       <c r="I45" s="6"/>
       <c r="J45" s="5">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="K45" s="5">
         <f>J45*0.35</f>
-        <v>1.05</v>
+        <v>105</v>
       </c>
       <c r="L45" s="5">
         <v>226</v>
       </c>
       <c r="M45" t="s" s="4">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s" s="4">
         <v>43</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
@@ -4151,18 +4160,18 @@
         <v>227</v>
       </c>
       <c r="M46" t="s" s="4">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B47" t="s" s="4">
         <v>43</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -4185,18 +4194,18 @@
         <v>228</v>
       </c>
       <c r="M47" t="s" s="4">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>43</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
@@ -4219,18 +4228,18 @@
         <v>229</v>
       </c>
       <c r="M48" t="s" s="4">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B49" t="s" s="4">
         <v>43</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -4253,18 +4262,18 @@
         <v>230</v>
       </c>
       <c r="M49" t="s" s="4">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>43</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
@@ -4287,18 +4296,18 @@
         <v>231</v>
       </c>
       <c r="M50" t="s" s="4">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5"/>
@@ -4306,7 +4315,7 @@
         <v>10</v>
       </c>
       <c r="G51" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="6"/>
@@ -4321,18 +4330,18 @@
         <v>232</v>
       </c>
       <c r="M51" t="s" s="4">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="5"/>
@@ -4340,7 +4349,7 @@
         <v>30</v>
       </c>
       <c r="G52" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="6"/>
@@ -4355,18 +4364,18 @@
         <v>233</v>
       </c>
       <c r="M52" t="s" s="4">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5"/>
@@ -4374,7 +4383,7 @@
         <v>100</v>
       </c>
       <c r="G53" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="6"/>
@@ -4389,18 +4398,18 @@
         <v>234</v>
       </c>
       <c r="M53" t="s" s="4">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
@@ -4419,18 +4428,18 @@
         <v>235</v>
       </c>
       <c r="M54" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="5"/>
@@ -4449,18 +4458,18 @@
         <v>236</v>
       </c>
       <c r="M55" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="5"/>
@@ -4479,18 +4488,18 @@
         <v>237</v>
       </c>
       <c r="M56" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="5"/>
@@ -4509,18 +4518,18 @@
         <v>238</v>
       </c>
       <c r="M57" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="5"/>
@@ -4539,18 +4548,18 @@
         <v>239</v>
       </c>
       <c r="M58" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="5"/>
@@ -4569,18 +4578,18 @@
         <v>240</v>
       </c>
       <c r="M59" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
@@ -4599,18 +4608,18 @@
         <v>241</v>
       </c>
       <c r="M60" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5"/>
@@ -4629,18 +4638,18 @@
         <v>242</v>
       </c>
       <c r="M61" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="5"/>
@@ -4659,18 +4668,18 @@
         <v>243</v>
       </c>
       <c r="M62" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" t="s" s="3">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C63" t="s" s="4">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="5"/>
@@ -4689,18 +4698,18 @@
         <v>244</v>
       </c>
       <c r="M63" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
       <c r="A64" t="s" s="3">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C64" t="s" s="4">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="5"/>
@@ -4719,18 +4728,18 @@
         <v>245</v>
       </c>
       <c r="M64" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" t="s" s="3">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C65" t="s" s="4">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="5"/>
@@ -4749,18 +4758,18 @@
         <v>246</v>
       </c>
       <c r="M65" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" t="s" s="3">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C66" t="s" s="4">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="5"/>
@@ -4779,18 +4788,18 @@
         <v>247</v>
       </c>
       <c r="M66" t="s" s="4">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
       <c r="A67" t="s" s="3">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B67" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C67" t="s" s="4">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="5"/>
@@ -4811,18 +4820,18 @@
         <v>248</v>
       </c>
       <c r="M67" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" ht="20" customHeight="1">
       <c r="A68" t="s" s="3">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B68" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C68" t="s" s="4">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="5"/>
@@ -4843,18 +4852,18 @@
         <v>249</v>
       </c>
       <c r="M68" t="s" s="4">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
       <c r="A69" t="s" s="3">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B69" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C69" t="s" s="4">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="5"/>
@@ -4875,18 +4884,18 @@
         <v>250</v>
       </c>
       <c r="M69" t="s" s="4">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
       <c r="A70" t="s" s="3">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B70" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C70" t="s" s="4">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="5"/>
@@ -4907,18 +4916,18 @@
         <v>251</v>
       </c>
       <c r="M70" t="s" s="4">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
       <c r="A71" t="s" s="3">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C71" t="s" s="4">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="5"/>
@@ -4939,18 +4948,18 @@
         <v>252</v>
       </c>
       <c r="M71" t="s" s="4">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="72" ht="20" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C72" t="s" s="4">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="5"/>
@@ -4971,48 +4980,50 @@
         <v>253</v>
       </c>
       <c r="M72" t="s" s="4">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" t="s" s="3">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B73" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C73" t="s" s="4">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
+      <c r="H73" t="s" s="4">
+        <v>130</v>
+      </c>
       <c r="I73" s="6"/>
       <c r="J73" s="5">
-        <v>3</v>
+        <v>900</v>
       </c>
       <c r="K73" s="5">
         <f>J73*0.35</f>
-        <v>1.05</v>
+        <v>315</v>
       </c>
       <c r="L73" s="5">
         <v>254</v>
       </c>
       <c r="M73" t="s" s="4">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="74" ht="20" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B74" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C74" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="5"/>
@@ -5031,18 +5042,18 @@
         <v>255</v>
       </c>
       <c r="M74" t="s" s="4">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" ht="20" customHeight="1">
       <c r="A75" t="s" s="3">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B75" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C75" t="s" s="4">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="5"/>
@@ -5061,18 +5072,18 @@
         <v>256</v>
       </c>
       <c r="M75" t="s" s="4">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C76" t="s" s="4">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -5091,18 +5102,18 @@
         <v>257</v>
       </c>
       <c r="M76" t="s" s="4">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" t="s" s="3">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B77" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C77" t="s" s="4">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="5"/>
@@ -5121,18 +5132,18 @@
         <v>258</v>
       </c>
       <c r="M77" t="s" s="4">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B78" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C78" t="s" s="4">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="5"/>
@@ -5151,18 +5162,18 @@
         <v>259</v>
       </c>
       <c r="M78" t="s" s="4">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" t="s" s="3">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C79" t="s" s="4">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="5"/>
@@ -5181,18 +5192,18 @@
         <v>260</v>
       </c>
       <c r="M79" t="s" s="4">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B80" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C80" t="s" s="4">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="5"/>
@@ -5211,18 +5222,18 @@
         <v>261</v>
       </c>
       <c r="M80" t="s" s="4">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" t="s" s="3">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B81" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C81" t="s" s="4">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="5"/>
@@ -5241,18 +5252,18 @@
         <v>262</v>
       </c>
       <c r="M81" t="s" s="4">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B82" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C82" t="s" s="4">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="5"/>
@@ -5271,18 +5282,18 @@
         <v>263</v>
       </c>
       <c r="M82" t="s" s="4">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
       <c r="A83" t="s" s="3">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B83" t="s" s="4">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C83" t="s" s="4">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="5"/>
@@ -5301,18 +5312,18 @@
         <v>264</v>
       </c>
       <c r="M83" t="s" s="4">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="84" ht="20" customHeight="1">
       <c r="A84" t="s" s="3">
+        <v>226</v>
+      </c>
+      <c r="B84" t="s" s="4">
         <v>223</v>
       </c>
-      <c r="B84" t="s" s="4">
-        <v>220</v>
-      </c>
       <c r="C84" t="s" s="4">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D84" s="6"/>
       <c r="E84" s="5"/>
@@ -5331,18 +5342,18 @@
         <v>265</v>
       </c>
       <c r="M84" t="s" s="4">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="85" ht="20" customHeight="1">
       <c r="A85" t="s" s="3">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B85" t="s" s="4">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C85" t="s" s="4">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D85" s="6"/>
       <c r="E85" s="5"/>
@@ -5361,18 +5372,18 @@
         <v>266</v>
       </c>
       <c r="M85" t="s" s="4">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="86" ht="20" customHeight="1">
       <c r="A86" t="s" s="3">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B86" t="s" s="4">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C86" t="s" s="4">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="5"/>
@@ -5391,18 +5402,18 @@
         <v>267</v>
       </c>
       <c r="M86" t="s" s="4">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="87" ht="20" customHeight="1">
       <c r="A87" t="s" s="3">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B87" t="s" s="4">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C87" t="s" s="4">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D87" s="6"/>
       <c r="E87" s="5"/>
@@ -5421,18 +5432,18 @@
         <v>268</v>
       </c>
       <c r="M87" t="s" s="4">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="88" ht="20" customHeight="1">
       <c r="A88" t="s" s="3">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B88" t="s" s="4">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C88" t="s" s="4">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D88" s="6"/>
       <c r="E88" s="5"/>
@@ -5451,18 +5462,18 @@
         <v>269</v>
       </c>
       <c r="M88" t="s" s="4">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="89" ht="20" customHeight="1">
       <c r="A89" t="s" s="3">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B89" t="s" s="4">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C89" t="s" s="4">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D89" s="6"/>
       <c r="E89" s="5"/>
@@ -5481,18 +5492,18 @@
         <v>270</v>
       </c>
       <c r="M89" t="s" s="4">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="90" ht="20" customHeight="1">
       <c r="A90" t="s" s="3">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B90" t="s" s="4">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C90" t="s" s="4">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D90" s="6"/>
       <c r="E90" s="5"/>
@@ -5511,7 +5522,7 @@
         <v>271</v>
       </c>
       <c r="M90" t="s" s="4">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -5564,16 +5575,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G1" t="s" s="2">
         <v>7</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>4</v>
@@ -5634,13 +5645,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -5661,18 +5672,18 @@
         <v>100</v>
       </c>
       <c r="M3" t="s" s="4">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
+        <v>251</v>
+      </c>
+      <c r="B4" t="s" s="4">
         <v>248</v>
       </c>
-      <c r="B4" t="s" s="4">
-        <v>245</v>
-      </c>
       <c r="C4" t="s" s="4">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -5693,18 +5704,18 @@
         <v>101</v>
       </c>
       <c r="M4" t="s" s="4">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C5" t="s" s="4">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -5725,18 +5736,18 @@
         <v>102</v>
       </c>
       <c r="M5" t="s" s="4">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
@@ -5757,18 +5768,18 @@
         <v>103</v>
       </c>
       <c r="M6" t="s" s="4">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D7" s="4">
         <v>7</v>
@@ -5789,18 +5800,18 @@
         <v>104</v>
       </c>
       <c r="M7" t="s" s="4">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D8" s="4">
         <v>8</v>
@@ -5821,18 +5832,18 @@
         <v>105</v>
       </c>
       <c r="M8" t="s" s="4">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D9" s="4">
         <v>10</v>
@@ -5853,18 +5864,18 @@
         <v>106</v>
       </c>
       <c r="M9" t="s" s="4">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -5885,18 +5896,18 @@
         <v>107</v>
       </c>
       <c r="M10" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -5917,18 +5928,18 @@
         <v>108</v>
       </c>
       <c r="M11" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -5949,18 +5960,18 @@
         <v>109</v>
       </c>
       <c r="M12" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -5981,18 +5992,18 @@
         <v>110</v>
       </c>
       <c r="M13" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -6013,18 +6024,18 @@
         <v>111</v>
       </c>
       <c r="M14" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C15" t="s" s="4">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -6045,18 +6056,18 @@
         <v>112</v>
       </c>
       <c r="M15" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -6077,18 +6088,18 @@
         <v>113</v>
       </c>
       <c r="M16" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C17" t="s" s="4">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -6109,18 +6120,18 @@
         <v>114</v>
       </c>
       <c r="M17" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -6141,18 +6152,18 @@
         <v>115</v>
       </c>
       <c r="M18" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -6173,18 +6184,18 @@
         <v>116</v>
       </c>
       <c r="M19" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -6205,18 +6216,18 @@
         <v>117</v>
       </c>
       <c r="M20" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -6237,18 +6248,18 @@
         <v>118</v>
       </c>
       <c r="M21" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -6269,18 +6280,18 @@
         <v>119</v>
       </c>
       <c r="M22" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
@@ -6303,18 +6314,18 @@
         <v>120</v>
       </c>
       <c r="M23" t="s" s="4">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
+        <v>300</v>
+      </c>
+      <c r="B24" t="s" s="4">
         <v>297</v>
       </c>
-      <c r="B24" t="s" s="4">
-        <v>294</v>
-      </c>
       <c r="C24" t="s" s="4">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
@@ -6337,18 +6348,18 @@
         <v>121</v>
       </c>
       <c r="M24" t="s" s="4">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C25" t="s" s="4">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
@@ -6371,18 +6382,18 @@
         <v>122</v>
       </c>
       <c r="M25" t="s" s="4">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
@@ -6405,18 +6416,18 @@
         <v>123</v>
       </c>
       <c r="M26" t="s" s="4">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4">
@@ -6439,18 +6450,18 @@
         <v>124</v>
       </c>
       <c r="M27" t="s" s="4">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4">
@@ -6473,18 +6484,18 @@
         <v>125</v>
       </c>
       <c r="M28" t="s" s="4">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4">
@@ -6507,18 +6518,18 @@
         <v>126</v>
       </c>
       <c r="M29" t="s" s="4">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C30" t="s" s="4">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4">
@@ -6541,18 +6552,18 @@
         <v>127</v>
       </c>
       <c r="M30" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4">
@@ -6575,18 +6586,18 @@
         <v>128</v>
       </c>
       <c r="M31" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4">
@@ -6609,18 +6620,18 @@
         <v>129</v>
       </c>
       <c r="M32" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4">
@@ -6643,18 +6654,18 @@
         <v>130</v>
       </c>
       <c r="M33" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4">
@@ -6677,18 +6688,18 @@
         <v>131</v>
       </c>
       <c r="M34" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4">
@@ -6711,18 +6722,18 @@
         <v>132</v>
       </c>
       <c r="M35" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4">
@@ -6745,18 +6756,18 @@
         <v>133</v>
       </c>
       <c r="M36" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4">
@@ -6779,18 +6790,18 @@
         <v>134</v>
       </c>
       <c r="M37" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4">
@@ -6813,18 +6824,18 @@
         <v>135</v>
       </c>
       <c r="M38" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4">
@@ -6847,18 +6858,18 @@
         <v>136</v>
       </c>
       <c r="M39" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4">
@@ -6881,18 +6892,18 @@
         <v>137</v>
       </c>
       <c r="M40" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4">
@@ -6915,18 +6926,18 @@
         <v>138</v>
       </c>
       <c r="M41" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4">
@@ -6949,18 +6960,18 @@
         <v>139</v>
       </c>
       <c r="M42" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4">
@@ -6981,18 +6992,18 @@
         <v>140</v>
       </c>
       <c r="M43" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
+        <v>349</v>
+      </c>
+      <c r="B44" t="s" s="4">
         <v>346</v>
       </c>
-      <c r="B44" t="s" s="4">
-        <v>343</v>
-      </c>
       <c r="C44" t="s" s="4">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4">
@@ -7013,18 +7024,18 @@
         <v>141</v>
       </c>
       <c r="M44" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4">
@@ -7045,18 +7056,18 @@
         <v>142</v>
       </c>
       <c r="M45" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4">
@@ -7077,18 +7088,18 @@
         <v>143</v>
       </c>
       <c r="M46" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4">
@@ -7109,18 +7120,18 @@
         <v>144</v>
       </c>
       <c r="M47" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -7141,18 +7152,18 @@
         <v>145</v>
       </c>
       <c r="M48" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -7173,18 +7184,18 @@
         <v>146</v>
       </c>
       <c r="M49" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -7205,18 +7216,18 @@
         <v>147</v>
       </c>
       <c r="M50" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -7237,18 +7248,18 @@
         <v>148</v>
       </c>
       <c r="M51" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -7269,18 +7280,18 @@
         <v>149</v>
       </c>
       <c r="M52" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -7301,18 +7312,18 @@
         <v>150</v>
       </c>
       <c r="M53" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -7333,18 +7344,18 @@
         <v>151</v>
       </c>
       <c r="M54" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -7365,18 +7376,18 @@
         <v>152</v>
       </c>
       <c r="M55" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -7397,18 +7408,18 @@
         <v>153</v>
       </c>
       <c r="M56" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -7429,18 +7440,18 @@
         <v>154</v>
       </c>
       <c r="M57" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -7461,18 +7472,18 @@
         <v>155</v>
       </c>
       <c r="M58" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -7493,18 +7504,18 @@
         <v>156</v>
       </c>
       <c r="M59" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -7525,18 +7536,18 @@
         <v>157</v>
       </c>
       <c r="M60" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -7557,18 +7568,18 @@
         <v>158</v>
       </c>
       <c r="M61" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -7589,7 +7600,7 @@
         <v>159</v>
       </c>
       <c r="M62" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -7606,7 +7617,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -7625,16 +7636,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -7665,7 +7676,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -7682,7 +7693,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E4" s="4">
         <v>30</v>
@@ -7699,7 +7710,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s" s="4">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
@@ -7716,7 +7727,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s" s="4">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="E6" s="4">
         <v>10</v>
@@ -7733,7 +7744,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
@@ -7750,7 +7761,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E8" s="4">
         <v>2</v>
@@ -7767,7 +7778,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -7784,7 +7795,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="E10" s="4">
         <v>50</v>
@@ -7801,7 +7812,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="E11" s="4">
         <v>30</v>
@@ -7818,7 +7829,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="E12" s="4">
         <v>20</v>
@@ -7835,7 +7846,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E13" s="4">
         <v>10</v>
@@ -7852,7 +7863,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s" s="4">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
@@ -7869,7 +7880,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="4">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="E15" s="4">
         <v>2</v>
@@ -7886,7 +7897,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s" s="4">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -8243,7 +8254,7 @@
         <v>10</v>
       </c>
       <c r="D37" t="s" s="4">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E37" s="4">
         <v>10</v>
@@ -8260,7 +8271,7 @@
         <v>10</v>
       </c>
       <c r="D38" t="s" s="4">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E38" s="4">
         <v>10</v>
@@ -8277,7 +8288,7 @@
         <v>10</v>
       </c>
       <c r="D39" t="s" s="4">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E39" s="4">
         <v>10</v>
@@ -8294,7 +8305,7 @@
         <v>10</v>
       </c>
       <c r="D40" t="s" s="4">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E40" s="4">
         <v>10</v>
@@ -8311,7 +8322,7 @@
         <v>10</v>
       </c>
       <c r="D41" t="s" s="4">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E41" s="4">
         <v>10</v>
@@ -8328,9 +8339,43 @@
         <v>10</v>
       </c>
       <c r="D42" t="s" s="4">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E42" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" ht="20" customHeight="1">
+      <c r="A43" s="3">
+        <v>41</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1</v>
+      </c>
+      <c r="C43" s="4">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s" s="4">
+        <v>128</v>
+      </c>
+      <c r="E43" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" ht="20" customHeight="1">
+      <c r="A44" s="3">
+        <v>42</v>
+      </c>
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s" s="4">
+        <v>200</v>
+      </c>
+      <c r="E44" s="4">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed #370 FlixelRL-370 力の指輪
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -754,7 +754,7 @@
     <t>attr</t>
   </si>
   <si>
-    <t>rustless</t>
+    <t>ext_val</t>
   </si>
   <si>
     <t>WEAPON1</t>
@@ -5625,7 +5625,7 @@
         <v>13</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s" s="4">
         <v>13</v>

</xml_diff>

<commit_message>
fixed #380 FlixelRL-380 守りの指輪
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="393">
   <si>
     <t>id</t>
   </si>
@@ -1066,16 +1066,19 @@
     <t>RING2</t>
   </si>
   <si>
-    <t>指輪ダミー2</t>
+    <t>守りの指輪</t>
+  </si>
+  <si>
+    <t>耐久力が1ポイント上昇します</t>
+  </si>
+  <si>
+    <t>RING3</t>
+  </si>
+  <si>
+    <t>指輪ダミー3</t>
   </si>
   <si>
     <t>指輪の説明文</t>
-  </si>
-  <si>
-    <t>RING3</t>
-  </si>
-  <si>
-    <t>指輪ダミー3</t>
   </si>
   <si>
     <t>RING4</t>
@@ -7017,11 +7020,11 @@
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
       <c r="J44" s="5">
-        <v>3</v>
+        <v>500</v>
       </c>
       <c r="K44" s="5">
         <f>J44*0.35</f>
-        <v>1.05</v>
+        <v>175</v>
       </c>
       <c r="L44" s="5">
         <v>141</v>
@@ -7059,18 +7062,18 @@
         <v>142</v>
       </c>
       <c r="M45" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B46" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4">
@@ -7091,18 +7094,18 @@
         <v>143</v>
       </c>
       <c r="M46" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B47" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4">
@@ -7123,18 +7126,18 @@
         <v>144</v>
       </c>
       <c r="M47" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -7155,18 +7158,18 @@
         <v>145</v>
       </c>
       <c r="M48" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B49" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -7187,18 +7190,18 @@
         <v>146</v>
       </c>
       <c r="M49" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -7219,18 +7222,18 @@
         <v>147</v>
       </c>
       <c r="M50" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B51" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -7251,18 +7254,18 @@
         <v>148</v>
       </c>
       <c r="M51" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B52" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -7283,18 +7286,18 @@
         <v>149</v>
       </c>
       <c r="M52" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B53" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -7315,18 +7318,18 @@
         <v>150</v>
       </c>
       <c r="M53" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B54" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -7347,18 +7350,18 @@
         <v>151</v>
       </c>
       <c r="M54" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B55" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -7379,18 +7382,18 @@
         <v>152</v>
       </c>
       <c r="M55" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B56" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -7411,18 +7414,18 @@
         <v>153</v>
       </c>
       <c r="M56" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B57" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -7443,18 +7446,18 @@
         <v>154</v>
       </c>
       <c r="M57" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B58" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -7475,18 +7478,18 @@
         <v>155</v>
       </c>
       <c r="M58" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B59" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -7507,18 +7510,18 @@
         <v>156</v>
       </c>
       <c r="M59" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B60" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -7539,18 +7542,18 @@
         <v>157</v>
       </c>
       <c r="M60" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B61" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -7571,18 +7574,18 @@
         <v>158</v>
       </c>
       <c r="M61" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B62" t="s" s="4">
         <v>346</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -7603,7 +7606,7 @@
         <v>159</v>
       </c>
       <c r="M62" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -7639,16 +7642,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">

</xml_diff>

<commit_message>
fixed #392 FlixelRL-392 ワープの薬
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="397">
   <si>
     <t>id</t>
   </si>
@@ -415,18 +415,24 @@
     <t>PORTION28</t>
   </si>
   <si>
-    <t>薬28</t>
+    <t>ワープの薬</t>
+  </si>
+  <si>
+    <t>warp</t>
+  </si>
+  <si>
+    <t>どこか別の場所にワープします</t>
+  </si>
+  <si>
+    <t>PORTION29</t>
+  </si>
+  <si>
+    <t>薬29</t>
   </si>
   <si>
     <t>飲むとHPが1回復します</t>
   </si>
   <si>
-    <t>PORTION29</t>
-  </si>
-  <si>
-    <t>薬29</t>
-  </si>
-  <si>
     <t>PORTION30</t>
   </si>
   <si>
@@ -628,16 +634,19 @@
     <t>WAND8</t>
   </si>
   <si>
-    <t>杖8</t>
+    <t>ワープの杖</t>
+  </si>
+  <si>
+    <t>相手をどこか別の場所にワープします</t>
+  </si>
+  <si>
+    <t>WAND9</t>
+  </si>
+  <si>
+    <t>杖9</t>
   </si>
   <si>
     <t>杖の説明文</t>
-  </si>
-  <si>
-    <t>WAND9</t>
-  </si>
-  <si>
-    <t>杖9</t>
   </si>
   <si>
     <t>WAND10</t>
@@ -4148,39 +4157,39 @@
       <c r="C46" t="s" s="4">
         <v>133</v>
       </c>
-      <c r="D46" s="4">
-        <v>1</v>
-      </c>
+      <c r="D46" s="6"/>
       <c r="E46" s="5">
         <v>10</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="5"/>
+      <c r="H46" t="s" s="4">
+        <v>134</v>
+      </c>
       <c r="I46" s="6"/>
       <c r="J46" s="5">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="K46" s="5">
         <f>J46*0.35</f>
-        <v>1.05</v>
+        <v>105</v>
       </c>
       <c r="L46" s="5">
         <v>227</v>
       </c>
       <c r="M46" t="s" s="4">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B47" t="s" s="4">
         <v>43</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -4203,18 +4212,18 @@
         <v>228</v>
       </c>
       <c r="M47" t="s" s="4">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>43</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
@@ -4237,18 +4246,18 @@
         <v>229</v>
       </c>
       <c r="M48" t="s" s="4">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s" s="4">
         <v>43</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -4271,18 +4280,18 @@
         <v>230</v>
       </c>
       <c r="M49" t="s" s="4">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>43</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
@@ -4305,18 +4314,18 @@
         <v>231</v>
       </c>
       <c r="M50" t="s" s="4">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5"/>
@@ -4324,7 +4333,7 @@
         <v>10</v>
       </c>
       <c r="G51" t="s" s="4">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="6"/>
@@ -4339,18 +4348,18 @@
         <v>232</v>
       </c>
       <c r="M51" t="s" s="4">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="5"/>
@@ -4358,7 +4367,7 @@
         <v>30</v>
       </c>
       <c r="G52" t="s" s="4">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="6"/>
@@ -4373,18 +4382,18 @@
         <v>233</v>
       </c>
       <c r="M52" t="s" s="4">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5"/>
@@ -4392,7 +4401,7 @@
         <v>100</v>
       </c>
       <c r="G53" t="s" s="4">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="6"/>
@@ -4407,18 +4416,18 @@
         <v>234</v>
       </c>
       <c r="M53" t="s" s="4">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
@@ -4437,18 +4446,18 @@
         <v>235</v>
       </c>
       <c r="M54" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="5"/>
@@ -4467,18 +4476,18 @@
         <v>236</v>
       </c>
       <c r="M55" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="5"/>
@@ -4497,18 +4506,18 @@
         <v>237</v>
       </c>
       <c r="M56" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="5"/>
@@ -4527,18 +4536,18 @@
         <v>238</v>
       </c>
       <c r="M57" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="5"/>
@@ -4557,18 +4566,18 @@
         <v>239</v>
       </c>
       <c r="M58" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="5"/>
@@ -4587,18 +4596,18 @@
         <v>240</v>
       </c>
       <c r="M59" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
@@ -4617,18 +4626,18 @@
         <v>241</v>
       </c>
       <c r="M60" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5"/>
@@ -4647,18 +4656,18 @@
         <v>242</v>
       </c>
       <c r="M61" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="5"/>
@@ -4677,18 +4686,18 @@
         <v>243</v>
       </c>
       <c r="M62" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" t="s" s="3">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C63" t="s" s="4">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="5"/>
@@ -4707,18 +4716,18 @@
         <v>244</v>
       </c>
       <c r="M63" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
       <c r="A64" t="s" s="3">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C64" t="s" s="4">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="5"/>
@@ -4737,18 +4746,18 @@
         <v>245</v>
       </c>
       <c r="M64" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" t="s" s="3">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C65" t="s" s="4">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="5"/>
@@ -4767,18 +4776,18 @@
         <v>246</v>
       </c>
       <c r="M65" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" t="s" s="3">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C66" t="s" s="4">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="5"/>
@@ -4797,18 +4806,18 @@
         <v>247</v>
       </c>
       <c r="M66" t="s" s="4">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
       <c r="A67" t="s" s="3">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B67" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C67" t="s" s="4">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="5"/>
@@ -4829,18 +4838,18 @@
         <v>248</v>
       </c>
       <c r="M67" t="s" s="4">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" ht="20" customHeight="1">
       <c r="A68" t="s" s="3">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B68" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C68" t="s" s="4">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="5"/>
@@ -4861,18 +4870,18 @@
         <v>249</v>
       </c>
       <c r="M68" t="s" s="4">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
       <c r="A69" t="s" s="3">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B69" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C69" t="s" s="4">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="5"/>
@@ -4893,18 +4902,18 @@
         <v>250</v>
       </c>
       <c r="M69" t="s" s="4">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
       <c r="A70" t="s" s="3">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B70" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C70" t="s" s="4">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="5"/>
@@ -4925,18 +4934,18 @@
         <v>251</v>
       </c>
       <c r="M70" t="s" s="4">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
       <c r="A71" t="s" s="3">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C71" t="s" s="4">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="5"/>
@@ -4957,18 +4966,18 @@
         <v>252</v>
       </c>
       <c r="M71" t="s" s="4">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72" ht="20" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C72" t="s" s="4">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="5"/>
@@ -4989,18 +4998,18 @@
         <v>253</v>
       </c>
       <c r="M72" t="s" s="4">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" t="s" s="3">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B73" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C73" t="s" s="4">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="5"/>
@@ -5021,48 +5030,50 @@
         <v>254</v>
       </c>
       <c r="M73" t="s" s="4">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" ht="20" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B74" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C74" t="s" s="4">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
+      <c r="H74" t="s" s="4">
+        <v>134</v>
+      </c>
       <c r="I74" s="6"/>
       <c r="J74" s="5">
-        <v>3</v>
+        <v>900</v>
       </c>
       <c r="K74" s="5">
         <f>J74*0.35</f>
-        <v>1.05</v>
+        <v>315</v>
       </c>
       <c r="L74" s="5">
         <v>255</v>
       </c>
       <c r="M74" t="s" s="4">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" ht="20" customHeight="1">
       <c r="A75" t="s" s="3">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B75" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C75" t="s" s="4">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="5"/>
@@ -5081,18 +5092,18 @@
         <v>256</v>
       </c>
       <c r="M75" t="s" s="4">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C76" t="s" s="4">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -5111,18 +5122,18 @@
         <v>257</v>
       </c>
       <c r="M76" t="s" s="4">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" t="s" s="3">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B77" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C77" t="s" s="4">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="5"/>
@@ -5141,18 +5152,18 @@
         <v>258</v>
       </c>
       <c r="M77" t="s" s="4">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B78" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C78" t="s" s="4">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="5"/>
@@ -5171,18 +5182,18 @@
         <v>259</v>
       </c>
       <c r="M78" t="s" s="4">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" t="s" s="3">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C79" t="s" s="4">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="5"/>
@@ -5201,18 +5212,18 @@
         <v>260</v>
       </c>
       <c r="M79" t="s" s="4">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B80" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C80" t="s" s="4">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="5"/>
@@ -5231,18 +5242,18 @@
         <v>261</v>
       </c>
       <c r="M80" t="s" s="4">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" t="s" s="3">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B81" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C81" t="s" s="4">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="5"/>
@@ -5261,18 +5272,18 @@
         <v>262</v>
       </c>
       <c r="M81" t="s" s="4">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B82" t="s" s="4">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C82" t="s" s="4">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="5"/>
@@ -5291,18 +5302,18 @@
         <v>263</v>
       </c>
       <c r="M82" t="s" s="4">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
       <c r="A83" t="s" s="3">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B83" t="s" s="4">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C83" t="s" s="4">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="5"/>
@@ -5321,18 +5332,18 @@
         <v>264</v>
       </c>
       <c r="M83" t="s" s="4">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="84" ht="20" customHeight="1">
       <c r="A84" t="s" s="3">
+        <v>229</v>
+      </c>
+      <c r="B84" t="s" s="4">
         <v>226</v>
       </c>
-      <c r="B84" t="s" s="4">
-        <v>223</v>
-      </c>
       <c r="C84" t="s" s="4">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D84" s="6"/>
       <c r="E84" s="5"/>
@@ -5351,18 +5362,18 @@
         <v>265</v>
       </c>
       <c r="M84" t="s" s="4">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="85" ht="20" customHeight="1">
       <c r="A85" t="s" s="3">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B85" t="s" s="4">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C85" t="s" s="4">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D85" s="6"/>
       <c r="E85" s="5"/>
@@ -5381,18 +5392,18 @@
         <v>266</v>
       </c>
       <c r="M85" t="s" s="4">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="86" ht="20" customHeight="1">
       <c r="A86" t="s" s="3">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B86" t="s" s="4">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C86" t="s" s="4">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="5"/>
@@ -5411,18 +5422,18 @@
         <v>267</v>
       </c>
       <c r="M86" t="s" s="4">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="87" ht="20" customHeight="1">
       <c r="A87" t="s" s="3">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B87" t="s" s="4">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C87" t="s" s="4">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D87" s="6"/>
       <c r="E87" s="5"/>
@@ -5441,18 +5452,18 @@
         <v>268</v>
       </c>
       <c r="M87" t="s" s="4">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="88" ht="20" customHeight="1">
       <c r="A88" t="s" s="3">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B88" t="s" s="4">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C88" t="s" s="4">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D88" s="6"/>
       <c r="E88" s="5"/>
@@ -5471,18 +5482,18 @@
         <v>269</v>
       </c>
       <c r="M88" t="s" s="4">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="89" ht="20" customHeight="1">
       <c r="A89" t="s" s="3">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B89" t="s" s="4">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C89" t="s" s="4">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D89" s="6"/>
       <c r="E89" s="5"/>
@@ -5501,18 +5512,18 @@
         <v>270</v>
       </c>
       <c r="M89" t="s" s="4">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="90" ht="20" customHeight="1">
       <c r="A90" t="s" s="3">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B90" t="s" s="4">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C90" t="s" s="4">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D90" s="6"/>
       <c r="E90" s="5"/>
@@ -5531,7 +5542,7 @@
         <v>271</v>
       </c>
       <c r="M90" t="s" s="4">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -5584,16 +5595,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G1" t="s" s="2">
         <v>7</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>4</v>
@@ -5654,13 +5665,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -5681,18 +5692,18 @@
         <v>100</v>
       </c>
       <c r="M3" t="s" s="4">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
+        <v>254</v>
+      </c>
+      <c r="B4" t="s" s="4">
         <v>251</v>
       </c>
-      <c r="B4" t="s" s="4">
-        <v>248</v>
-      </c>
       <c r="C4" t="s" s="4">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -5713,18 +5724,18 @@
         <v>101</v>
       </c>
       <c r="M4" t="s" s="4">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C5" t="s" s="4">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -5745,18 +5756,18 @@
         <v>102</v>
       </c>
       <c r="M5" t="s" s="4">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
@@ -5777,18 +5788,18 @@
         <v>103</v>
       </c>
       <c r="M6" t="s" s="4">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D7" s="4">
         <v>7</v>
@@ -5809,18 +5820,18 @@
         <v>104</v>
       </c>
       <c r="M7" t="s" s="4">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D8" s="4">
         <v>8</v>
@@ -5841,18 +5852,18 @@
         <v>105</v>
       </c>
       <c r="M8" t="s" s="4">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D9" s="4">
         <v>10</v>
@@ -5873,18 +5884,18 @@
         <v>106</v>
       </c>
       <c r="M9" t="s" s="4">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -5905,18 +5916,18 @@
         <v>107</v>
       </c>
       <c r="M10" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -5937,18 +5948,18 @@
         <v>108</v>
       </c>
       <c r="M11" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -5969,18 +5980,18 @@
         <v>109</v>
       </c>
       <c r="M12" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -6001,18 +6012,18 @@
         <v>110</v>
       </c>
       <c r="M13" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -6033,18 +6044,18 @@
         <v>111</v>
       </c>
       <c r="M14" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C15" t="s" s="4">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -6065,18 +6076,18 @@
         <v>112</v>
       </c>
       <c r="M15" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -6097,18 +6108,18 @@
         <v>113</v>
       </c>
       <c r="M16" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C17" t="s" s="4">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -6129,18 +6140,18 @@
         <v>114</v>
       </c>
       <c r="M17" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -6161,18 +6172,18 @@
         <v>115</v>
       </c>
       <c r="M18" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -6193,18 +6204,18 @@
         <v>116</v>
       </c>
       <c r="M19" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -6225,18 +6236,18 @@
         <v>117</v>
       </c>
       <c r="M20" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -6257,18 +6268,18 @@
         <v>118</v>
       </c>
       <c r="M21" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -6289,18 +6300,18 @@
         <v>119</v>
       </c>
       <c r="M22" t="s" s="4">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
@@ -6323,18 +6334,18 @@
         <v>120</v>
       </c>
       <c r="M23" t="s" s="4">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
+        <v>303</v>
+      </c>
+      <c r="B24" t="s" s="4">
         <v>300</v>
       </c>
-      <c r="B24" t="s" s="4">
-        <v>297</v>
-      </c>
       <c r="C24" t="s" s="4">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
@@ -6357,18 +6368,18 @@
         <v>121</v>
       </c>
       <c r="M24" t="s" s="4">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C25" t="s" s="4">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
@@ -6391,18 +6402,18 @@
         <v>122</v>
       </c>
       <c r="M25" t="s" s="4">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
@@ -6425,18 +6436,18 @@
         <v>123</v>
       </c>
       <c r="M26" t="s" s="4">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4">
@@ -6459,18 +6470,18 @@
         <v>124</v>
       </c>
       <c r="M27" t="s" s="4">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4">
@@ -6493,18 +6504,18 @@
         <v>125</v>
       </c>
       <c r="M28" t="s" s="4">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4">
@@ -6527,18 +6538,18 @@
         <v>126</v>
       </c>
       <c r="M29" t="s" s="4">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C30" t="s" s="4">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4">
@@ -6561,18 +6572,18 @@
         <v>127</v>
       </c>
       <c r="M30" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4">
@@ -6595,18 +6606,18 @@
         <v>128</v>
       </c>
       <c r="M31" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4">
@@ -6629,18 +6640,18 @@
         <v>129</v>
       </c>
       <c r="M32" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4">
@@ -6663,18 +6674,18 @@
         <v>130</v>
       </c>
       <c r="M33" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4">
@@ -6697,18 +6708,18 @@
         <v>131</v>
       </c>
       <c r="M34" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4">
@@ -6731,18 +6742,18 @@
         <v>132</v>
       </c>
       <c r="M35" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4">
@@ -6765,18 +6776,18 @@
         <v>133</v>
       </c>
       <c r="M36" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4">
@@ -6799,18 +6810,18 @@
         <v>134</v>
       </c>
       <c r="M37" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4">
@@ -6833,18 +6844,18 @@
         <v>135</v>
       </c>
       <c r="M38" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4">
@@ -6867,18 +6878,18 @@
         <v>136</v>
       </c>
       <c r="M39" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4">
@@ -6901,18 +6912,18 @@
         <v>137</v>
       </c>
       <c r="M40" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4">
@@ -6935,18 +6946,18 @@
         <v>138</v>
       </c>
       <c r="M41" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4">
@@ -6969,18 +6980,18 @@
         <v>139</v>
       </c>
       <c r="M42" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D43" s="5">
         <v>1</v>
@@ -7001,18 +7012,18 @@
         <v>140</v>
       </c>
       <c r="M43" t="s" s="4">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
+        <v>352</v>
+      </c>
+      <c r="B44" t="s" s="4">
         <v>349</v>
       </c>
-      <c r="B44" t="s" s="4">
-        <v>346</v>
-      </c>
       <c r="C44" t="s" s="4">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4">
@@ -7033,18 +7044,18 @@
         <v>141</v>
       </c>
       <c r="M44" t="s" s="4">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="6"/>
@@ -7067,18 +7078,18 @@
         <v>142</v>
       </c>
       <c r="M45" t="s" s="4">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4">
@@ -7099,18 +7110,18 @@
         <v>143</v>
       </c>
       <c r="M46" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4">
@@ -7131,18 +7142,18 @@
         <v>144</v>
       </c>
       <c r="M47" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -7163,18 +7174,18 @@
         <v>145</v>
       </c>
       <c r="M48" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -7195,18 +7206,18 @@
         <v>146</v>
       </c>
       <c r="M49" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -7227,18 +7238,18 @@
         <v>147</v>
       </c>
       <c r="M50" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -7259,18 +7270,18 @@
         <v>148</v>
       </c>
       <c r="M51" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -7291,18 +7302,18 @@
         <v>149</v>
       </c>
       <c r="M52" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -7323,18 +7334,18 @@
         <v>150</v>
       </c>
       <c r="M53" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -7355,18 +7366,18 @@
         <v>151</v>
       </c>
       <c r="M54" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -7387,18 +7398,18 @@
         <v>152</v>
       </c>
       <c r="M55" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -7419,18 +7430,18 @@
         <v>153</v>
       </c>
       <c r="M56" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -7451,18 +7462,18 @@
         <v>154</v>
       </c>
       <c r="M57" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -7483,18 +7494,18 @@
         <v>155</v>
       </c>
       <c r="M58" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -7515,18 +7526,18 @@
         <v>156</v>
       </c>
       <c r="M59" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -7547,18 +7558,18 @@
         <v>157</v>
       </c>
       <c r="M60" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -7579,18 +7590,18 @@
         <v>158</v>
       </c>
       <c r="M61" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -7611,7 +7622,7 @@
         <v>159</v>
       </c>
       <c r="M62" t="s" s="4">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -7628,7 +7639,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -7647,16 +7658,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -7687,7 +7698,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -7704,7 +7715,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E4" s="4">
         <v>30</v>
@@ -7721,7 +7732,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s" s="4">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
@@ -7738,7 +7749,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s" s="4">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E6" s="4">
         <v>10</v>
@@ -7755,7 +7766,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
@@ -7772,7 +7783,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E8" s="4">
         <v>2</v>
@@ -7789,7 +7800,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -7806,7 +7817,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="E10" s="4">
         <v>50</v>
@@ -7823,7 +7834,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s" s="4">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="E11" s="4">
         <v>30</v>
@@ -7840,7 +7851,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E12" s="4">
         <v>20</v>
@@ -7857,7 +7868,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="E13" s="4">
         <v>10</v>
@@ -7874,7 +7885,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s" s="4">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
@@ -7891,7 +7902,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="4">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E15" s="4">
         <v>2</v>
@@ -7908,7 +7919,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s" s="4">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -8265,7 +8276,7 @@
         <v>10</v>
       </c>
       <c r="D37" t="s" s="4">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E37" s="4">
         <v>10</v>
@@ -8282,7 +8293,7 @@
         <v>10</v>
       </c>
       <c r="D38" t="s" s="4">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E38" s="4">
         <v>10</v>
@@ -8299,7 +8310,7 @@
         <v>10</v>
       </c>
       <c r="D39" t="s" s="4">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E39" s="4">
         <v>10</v>
@@ -8316,7 +8327,7 @@
         <v>10</v>
       </c>
       <c r="D40" t="s" s="4">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E40" s="4">
         <v>10</v>
@@ -8333,7 +8344,7 @@
         <v>10</v>
       </c>
       <c r="D41" t="s" s="4">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E41" s="4">
         <v>10</v>
@@ -8350,7 +8361,7 @@
         <v>10</v>
       </c>
       <c r="D42" t="s" s="4">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E42" s="4">
         <v>10</v>
@@ -8384,7 +8395,7 @@
         <v>10</v>
       </c>
       <c r="D44" t="s" s="4">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E44" s="4">
         <v>10</v>
@@ -8401,7 +8412,7 @@
         <v>10</v>
       </c>
       <c r="D45" t="s" s="4">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="E45" s="4">
         <v>10</v>
@@ -8418,7 +8429,7 @@
         <v>10</v>
       </c>
       <c r="D46" t="s" s="4">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E46" s="4">
         <v>10</v>
@@ -8435,9 +8446,43 @@
         <v>10</v>
       </c>
       <c r="D47" t="s" s="4">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="E47" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" ht="20" customHeight="1">
+      <c r="A48" s="3">
+        <v>46</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="C48" s="4">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s" s="4">
+        <v>132</v>
+      </c>
+      <c r="E48" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" ht="20" customHeight="1">
+      <c r="A49" s="3">
+        <v>47</v>
+      </c>
+      <c r="B49" s="4">
+        <v>1</v>
+      </c>
+      <c r="C49" s="4">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s" s="4">
+        <v>205</v>
+      </c>
+      <c r="E49" s="4">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed #391 FlixelRL-391 ワープの杖
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="399">
   <si>
     <t>id</t>
   </si>
@@ -643,16 +643,22 @@
     <t>WAND9</t>
   </si>
   <si>
-    <t>杖9</t>
+    <t>チェンジの杖</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>相手とプレイヤーの位置を入れ替えます</t>
+  </si>
+  <si>
+    <t>WAND10</t>
+  </si>
+  <si>
+    <t>杖10</t>
   </si>
   <si>
     <t>杖の説明文</t>
-  </si>
-  <si>
-    <t>WAND10</t>
-  </si>
-  <si>
-    <t>杖10</t>
   </si>
   <si>
     <t>WAND11</t>
@@ -5079,31 +5085,33 @@
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
+      <c r="H75" t="s" s="4">
+        <v>210</v>
+      </c>
       <c r="I75" s="6"/>
       <c r="J75" s="5">
-        <v>3</v>
+        <v>900</v>
       </c>
       <c r="K75" s="5">
         <f>J75*0.35</f>
-        <v>1.05</v>
+        <v>315</v>
       </c>
       <c r="L75" s="5">
         <v>256</v>
       </c>
       <c r="M75" t="s" s="4">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B76" t="s" s="4">
         <v>184</v>
       </c>
       <c r="C76" t="s" s="4">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -5122,18 +5130,18 @@
         <v>257</v>
       </c>
       <c r="M76" t="s" s="4">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" t="s" s="3">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B77" t="s" s="4">
         <v>184</v>
       </c>
       <c r="C77" t="s" s="4">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="5"/>
@@ -5152,18 +5160,18 @@
         <v>258</v>
       </c>
       <c r="M77" t="s" s="4">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B78" t="s" s="4">
         <v>184</v>
       </c>
       <c r="C78" t="s" s="4">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="5"/>
@@ -5182,18 +5190,18 @@
         <v>259</v>
       </c>
       <c r="M78" t="s" s="4">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" t="s" s="3">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B79" t="s" s="4">
         <v>184</v>
       </c>
       <c r="C79" t="s" s="4">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="5"/>
@@ -5212,18 +5220,18 @@
         <v>260</v>
       </c>
       <c r="M79" t="s" s="4">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B80" t="s" s="4">
         <v>184</v>
       </c>
       <c r="C80" t="s" s="4">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="5"/>
@@ -5242,18 +5250,18 @@
         <v>261</v>
       </c>
       <c r="M80" t="s" s="4">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" t="s" s="3">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B81" t="s" s="4">
         <v>184</v>
       </c>
       <c r="C81" t="s" s="4">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="5"/>
@@ -5272,18 +5280,18 @@
         <v>262</v>
       </c>
       <c r="M81" t="s" s="4">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B82" t="s" s="4">
         <v>184</v>
       </c>
       <c r="C82" t="s" s="4">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="5"/>
@@ -5302,18 +5310,18 @@
         <v>263</v>
       </c>
       <c r="M82" t="s" s="4">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
       <c r="A83" t="s" s="3">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B83" t="s" s="4">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C83" t="s" s="4">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="5"/>
@@ -5332,18 +5340,18 @@
         <v>264</v>
       </c>
       <c r="M83" t="s" s="4">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" ht="20" customHeight="1">
       <c r="A84" t="s" s="3">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B84" t="s" s="4">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C84" t="s" s="4">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D84" s="6"/>
       <c r="E84" s="5"/>
@@ -5362,18 +5370,18 @@
         <v>265</v>
       </c>
       <c r="M84" t="s" s="4">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="85" ht="20" customHeight="1">
       <c r="A85" t="s" s="3">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B85" t="s" s="4">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C85" t="s" s="4">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D85" s="6"/>
       <c r="E85" s="5"/>
@@ -5392,18 +5400,18 @@
         <v>266</v>
       </c>
       <c r="M85" t="s" s="4">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="86" ht="20" customHeight="1">
       <c r="A86" t="s" s="3">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B86" t="s" s="4">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C86" t="s" s="4">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="5"/>
@@ -5422,18 +5430,18 @@
         <v>267</v>
       </c>
       <c r="M86" t="s" s="4">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="87" ht="20" customHeight="1">
       <c r="A87" t="s" s="3">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B87" t="s" s="4">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C87" t="s" s="4">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D87" s="6"/>
       <c r="E87" s="5"/>
@@ -5452,18 +5460,18 @@
         <v>268</v>
       </c>
       <c r="M87" t="s" s="4">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" ht="20" customHeight="1">
       <c r="A88" t="s" s="3">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B88" t="s" s="4">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C88" t="s" s="4">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D88" s="6"/>
       <c r="E88" s="5"/>
@@ -5482,18 +5490,18 @@
         <v>269</v>
       </c>
       <c r="M88" t="s" s="4">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="89" ht="20" customHeight="1">
       <c r="A89" t="s" s="3">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B89" t="s" s="4">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C89" t="s" s="4">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D89" s="6"/>
       <c r="E89" s="5"/>
@@ -5512,18 +5520,18 @@
         <v>270</v>
       </c>
       <c r="M89" t="s" s="4">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="90" ht="20" customHeight="1">
       <c r="A90" t="s" s="3">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B90" t="s" s="4">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C90" t="s" s="4">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D90" s="6"/>
       <c r="E90" s="5"/>
@@ -5542,7 +5550,7 @@
         <v>271</v>
       </c>
       <c r="M90" t="s" s="4">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -5595,16 +5603,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G1" t="s" s="2">
         <v>7</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>4</v>
@@ -5665,13 +5673,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -5692,18 +5700,18 @@
         <v>100</v>
       </c>
       <c r="M3" t="s" s="4">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C4" t="s" s="4">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -5724,18 +5732,18 @@
         <v>101</v>
       </c>
       <c r="M4" t="s" s="4">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C5" t="s" s="4">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -5756,18 +5764,18 @@
         <v>102</v>
       </c>
       <c r="M5" t="s" s="4">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
@@ -5788,18 +5796,18 @@
         <v>103</v>
       </c>
       <c r="M6" t="s" s="4">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D7" s="4">
         <v>7</v>
@@ -5820,18 +5828,18 @@
         <v>104</v>
       </c>
       <c r="M7" t="s" s="4">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D8" s="4">
         <v>8</v>
@@ -5852,18 +5860,18 @@
         <v>105</v>
       </c>
       <c r="M8" t="s" s="4">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D9" s="4">
         <v>10</v>
@@ -5884,18 +5892,18 @@
         <v>106</v>
       </c>
       <c r="M9" t="s" s="4">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -5916,18 +5924,18 @@
         <v>107</v>
       </c>
       <c r="M10" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -5948,18 +5956,18 @@
         <v>108</v>
       </c>
       <c r="M11" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -5980,18 +5988,18 @@
         <v>109</v>
       </c>
       <c r="M12" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -6012,18 +6020,18 @@
         <v>110</v>
       </c>
       <c r="M13" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -6044,18 +6052,18 @@
         <v>111</v>
       </c>
       <c r="M14" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C15" t="s" s="4">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -6076,18 +6084,18 @@
         <v>112</v>
       </c>
       <c r="M15" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -6108,18 +6116,18 @@
         <v>113</v>
       </c>
       <c r="M16" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C17" t="s" s="4">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -6140,18 +6148,18 @@
         <v>114</v>
       </c>
       <c r="M17" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -6172,18 +6180,18 @@
         <v>115</v>
       </c>
       <c r="M18" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -6204,18 +6212,18 @@
         <v>116</v>
       </c>
       <c r="M19" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -6236,18 +6244,18 @@
         <v>117</v>
       </c>
       <c r="M20" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -6268,18 +6276,18 @@
         <v>118</v>
       </c>
       <c r="M21" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -6300,18 +6308,18 @@
         <v>119</v>
       </c>
       <c r="M22" t="s" s="4">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
@@ -6334,18 +6342,18 @@
         <v>120</v>
       </c>
       <c r="M23" t="s" s="4">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C24" t="s" s="4">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
@@ -6368,18 +6376,18 @@
         <v>121</v>
       </c>
       <c r="M24" t="s" s="4">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C25" t="s" s="4">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
@@ -6402,18 +6410,18 @@
         <v>122</v>
       </c>
       <c r="M25" t="s" s="4">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
@@ -6436,18 +6444,18 @@
         <v>123</v>
       </c>
       <c r="M26" t="s" s="4">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4">
@@ -6470,18 +6478,18 @@
         <v>124</v>
       </c>
       <c r="M27" t="s" s="4">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4">
@@ -6504,18 +6512,18 @@
         <v>125</v>
       </c>
       <c r="M28" t="s" s="4">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4">
@@ -6538,18 +6546,18 @@
         <v>126</v>
       </c>
       <c r="M29" t="s" s="4">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C30" t="s" s="4">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4">
@@ -6572,18 +6580,18 @@
         <v>127</v>
       </c>
       <c r="M30" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4">
@@ -6606,18 +6614,18 @@
         <v>128</v>
       </c>
       <c r="M31" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4">
@@ -6640,18 +6648,18 @@
         <v>129</v>
       </c>
       <c r="M32" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4">
@@ -6674,18 +6682,18 @@
         <v>130</v>
       </c>
       <c r="M33" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4">
@@ -6708,18 +6716,18 @@
         <v>131</v>
       </c>
       <c r="M34" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4">
@@ -6742,18 +6750,18 @@
         <v>132</v>
       </c>
       <c r="M35" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4">
@@ -6776,18 +6784,18 @@
         <v>133</v>
       </c>
       <c r="M36" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4">
@@ -6810,18 +6818,18 @@
         <v>134</v>
       </c>
       <c r="M37" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4">
@@ -6844,18 +6852,18 @@
         <v>135</v>
       </c>
       <c r="M38" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4">
@@ -6878,18 +6886,18 @@
         <v>136</v>
       </c>
       <c r="M39" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4">
@@ -6912,18 +6920,18 @@
         <v>137</v>
       </c>
       <c r="M40" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4">
@@ -6946,18 +6954,18 @@
         <v>138</v>
       </c>
       <c r="M41" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4">
@@ -6980,18 +6988,18 @@
         <v>139</v>
       </c>
       <c r="M42" t="s" s="4">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D43" s="5">
         <v>1</v>
@@ -7012,18 +7020,18 @@
         <v>140</v>
       </c>
       <c r="M43" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4">
@@ -7044,18 +7052,18 @@
         <v>141</v>
       </c>
       <c r="M44" t="s" s="4">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="6"/>
@@ -7078,18 +7086,18 @@
         <v>142</v>
       </c>
       <c r="M45" t="s" s="4">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4">
@@ -7110,18 +7118,18 @@
         <v>143</v>
       </c>
       <c r="M46" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4">
@@ -7142,18 +7150,18 @@
         <v>144</v>
       </c>
       <c r="M47" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -7174,18 +7182,18 @@
         <v>145</v>
       </c>
       <c r="M48" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -7206,18 +7214,18 @@
         <v>146</v>
       </c>
       <c r="M49" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -7238,18 +7246,18 @@
         <v>147</v>
       </c>
       <c r="M50" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -7270,18 +7278,18 @@
         <v>148</v>
       </c>
       <c r="M51" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -7302,18 +7310,18 @@
         <v>149</v>
       </c>
       <c r="M52" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -7334,18 +7342,18 @@
         <v>150</v>
       </c>
       <c r="M53" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -7366,18 +7374,18 @@
         <v>151</v>
       </c>
       <c r="M54" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -7398,18 +7406,18 @@
         <v>152</v>
       </c>
       <c r="M55" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -7430,18 +7438,18 @@
         <v>153</v>
       </c>
       <c r="M56" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -7462,18 +7470,18 @@
         <v>154</v>
       </c>
       <c r="M57" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -7494,18 +7502,18 @@
         <v>155</v>
       </c>
       <c r="M58" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -7526,18 +7534,18 @@
         <v>156</v>
       </c>
       <c r="M59" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -7558,18 +7566,18 @@
         <v>157</v>
       </c>
       <c r="M60" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -7590,18 +7598,18 @@
         <v>158</v>
       </c>
       <c r="M61" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -7622,7 +7630,7 @@
         <v>159</v>
       </c>
       <c r="M62" t="s" s="4">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -7658,16 +7666,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -7698,7 +7706,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -7715,7 +7723,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E4" s="4">
         <v>30</v>
@@ -7732,7 +7740,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s" s="4">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
@@ -7749,7 +7757,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s" s="4">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E6" s="4">
         <v>10</v>
@@ -7766,7 +7774,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
@@ -7783,7 +7791,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E8" s="4">
         <v>2</v>
@@ -7800,7 +7808,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -7817,7 +7825,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E10" s="4">
         <v>50</v>
@@ -7834,7 +7842,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s" s="4">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E11" s="4">
         <v>30</v>
@@ -7851,7 +7859,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E12" s="4">
         <v>20</v>
@@ -7868,7 +7876,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E13" s="4">
         <v>10</v>
@@ -7885,7 +7893,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s" s="4">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
@@ -7902,7 +7910,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="4">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E15" s="4">
         <v>2</v>
@@ -7919,7 +7927,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s" s="4">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -8412,7 +8420,7 @@
         <v>10</v>
       </c>
       <c r="D45" t="s" s="4">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E45" s="4">
         <v>10</v>
@@ -8429,7 +8437,7 @@
         <v>10</v>
       </c>
       <c r="D46" t="s" s="4">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E46" s="4">
         <v>10</v>
@@ -8446,7 +8454,7 @@
         <v>10</v>
       </c>
       <c r="D47" t="s" s="4">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E47" s="4">
         <v>10</v>

</xml_diff>

<commit_message>
fixed #401 FlixelRL-401 眠りよけの指輪
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="401">
   <si>
     <t>id</t>
   </si>
@@ -142,10 +142,10 @@
     <t>FOOD16</t>
   </si>
   <si>
-    <t>PORTION1</t>
-  </si>
-  <si>
-    <t>Portion</t>
+    <t>POTION1</t>
+  </si>
+  <si>
+    <t>Potion</t>
   </si>
   <si>
     <t>回復薬10</t>
@@ -154,7 +154,7 @@
     <t>飲むとHPが10回復します</t>
   </si>
   <si>
-    <t>PORTION2</t>
+    <t>POTION2</t>
   </si>
   <si>
     <t>回復薬20</t>
@@ -163,7 +163,7 @@
     <t>飲むとHPが20回復します</t>
   </si>
   <si>
-    <t>PORTION3</t>
+    <t>POTION3</t>
   </si>
   <si>
     <t>回復薬30</t>
@@ -172,7 +172,7 @@
     <t>飲むとHPが30回復します</t>
   </si>
   <si>
-    <t>PORTION4</t>
+    <t>POTION4</t>
   </si>
   <si>
     <t>回復薬40</t>
@@ -181,7 +181,7 @@
     <t>飲むとHPが40回復します</t>
   </si>
   <si>
-    <t>PORTION5</t>
+    <t>POTION5</t>
   </si>
   <si>
     <t>回復薬50</t>
@@ -190,7 +190,7 @@
     <t>飲むとHPが50回復します</t>
   </si>
   <si>
-    <t>PORTION6</t>
+    <t>POTION6</t>
   </si>
   <si>
     <t>回復薬60</t>
@@ -199,7 +199,7 @@
     <t>飲むとHPが60回復します</t>
   </si>
   <si>
-    <t>PORTION7</t>
+    <t>POTION7</t>
   </si>
   <si>
     <t>回復薬70</t>
@@ -208,7 +208,7 @@
     <t>飲むとHPが70回復します</t>
   </si>
   <si>
-    <t>PORTION8</t>
+    <t>POTION8</t>
   </si>
   <si>
     <t>回復薬80</t>
@@ -217,7 +217,7 @@
     <t>飲むとHPが80回復します</t>
   </si>
   <si>
-    <t>PORTION9</t>
+    <t>POTION9</t>
   </si>
   <si>
     <t>回復薬90</t>
@@ -226,7 +226,7 @@
     <t>飲むとHPが90回復します</t>
   </si>
   <si>
-    <t>PORTION10</t>
+    <t>POTION10</t>
   </si>
   <si>
     <t>回復薬100</t>
@@ -235,7 +235,7 @@
     <t>飲むとHPが100回復します</t>
   </si>
   <si>
-    <t>PORTION11</t>
+    <t>POTION11</t>
   </si>
   <si>
     <t>回復薬110</t>
@@ -244,7 +244,7 @@
     <t>飲むとHPが110回復します</t>
   </si>
   <si>
-    <t>PORTION12</t>
+    <t>POTION12</t>
   </si>
   <si>
     <t>回復薬120</t>
@@ -253,7 +253,7 @@
     <t>飲むとHPが120回復します</t>
   </si>
   <si>
-    <t>PORTION13</t>
+    <t>POTION13</t>
   </si>
   <si>
     <t>回復薬130</t>
@@ -262,7 +262,7 @@
     <t>飲むとHPが130回復します</t>
   </si>
   <si>
-    <t>PORTION14</t>
+    <t>POTION14</t>
   </si>
   <si>
     <t>回復薬140</t>
@@ -271,7 +271,7 @@
     <t>飲むとHPが140回復します</t>
   </si>
   <si>
-    <t>PORTION15</t>
+    <t>POTION15</t>
   </si>
   <si>
     <t>回復薬150</t>
@@ -280,7 +280,7 @@
     <t>飲むとHPが150回復します</t>
   </si>
   <si>
-    <t>PORTION16</t>
+    <t>POTION16</t>
   </si>
   <si>
     <t>回復薬160</t>
@@ -289,7 +289,7 @@
     <t>飲むとHPが160回復します</t>
   </si>
   <si>
-    <t>PORTION17</t>
+    <t>POTION17</t>
   </si>
   <si>
     <t>命の薬</t>
@@ -301,7 +301,7 @@
     <t>最大HPが上昇します</t>
   </si>
   <si>
-    <t>PORTION18</t>
+    <t>POTION18</t>
   </si>
   <si>
     <t>胃拡張の薬</t>
@@ -310,7 +310,7 @@
     <t>最大満腹度が上昇します</t>
   </si>
   <si>
-    <t>PORTION19</t>
+    <t>POTION19</t>
   </si>
   <si>
     <t>力の薬</t>
@@ -319,7 +319,7 @@
     <t>力が上昇します</t>
   </si>
   <si>
-    <t>PORTION20</t>
+    <t>POTION20</t>
   </si>
   <si>
     <t>毒薬</t>
@@ -328,7 +328,7 @@
     <t>猛毒の薬。飲んではいけません</t>
   </si>
   <si>
-    <t>PORTION21</t>
+    <t>POTION21</t>
   </si>
   <si>
     <t>眠り薬</t>
@@ -340,7 +340,7 @@
     <t>飲むと眠くなる薬</t>
   </si>
   <si>
-    <t>PORTION22</t>
+    <t>POTION22</t>
   </si>
   <si>
     <t>しびれ薬</t>
@@ -352,7 +352,7 @@
     <t>しびれて動けなくなります</t>
   </si>
   <si>
-    <t>PORTION23</t>
+    <t>POTION23</t>
   </si>
   <si>
     <t>混乱の薬</t>
@@ -364,7 +364,7 @@
     <t>混乱する薬</t>
   </si>
   <si>
-    <t>PORTION24</t>
+    <t>POTION24</t>
   </si>
   <si>
     <t>怒りの薬</t>
@@ -376,7 +376,7 @@
     <t>怒り状態になります</t>
   </si>
   <si>
-    <t>PORTION25</t>
+    <t>POTION25</t>
   </si>
   <si>
     <t>元気になる薬</t>
@@ -388,7 +388,7 @@
     <t>元気状態になります</t>
   </si>
   <si>
-    <t>PORTION26</t>
+    <t>POTION26</t>
   </si>
   <si>
     <t>いやしの薬</t>
@@ -400,7 +400,7 @@
     <t>状態異常が回復します</t>
   </si>
   <si>
-    <t>PORTION27</t>
+    <t>POTION27</t>
   </si>
   <si>
     <t>封印の薬</t>
@@ -412,7 +412,7 @@
     <t>封印状態になります</t>
   </si>
   <si>
-    <t>PORTION28</t>
+    <t>POTION28</t>
   </si>
   <si>
     <t>ワープの薬</t>
@@ -424,7 +424,7 @@
     <t>どこか別の場所にワープします</t>
   </si>
   <si>
-    <t>PORTION29</t>
+    <t>POTION29</t>
   </si>
   <si>
     <t>薬29</t>
@@ -433,19 +433,19 @@
     <t>飲むとHPが1回復します</t>
   </si>
   <si>
-    <t>PORTION30</t>
+    <t>POTION30</t>
   </si>
   <si>
     <t>薬30</t>
   </si>
   <si>
-    <t>PORTION31</t>
+    <t>POTION31</t>
   </si>
   <si>
     <t>薬31</t>
   </si>
   <si>
-    <t>PORTION32</t>
+    <t>POTION32</t>
   </si>
   <si>
     <t>薬32</t>
@@ -1099,22 +1099,28 @@
     <t>RING4</t>
   </si>
   <si>
-    <t>指輪ダミー4</t>
+    <t>眠りよけの指輪</t>
+  </si>
+  <si>
+    <t>眠り状態を防ぎます</t>
+  </si>
+  <si>
+    <t>RING5</t>
+  </si>
+  <si>
+    <t>混乱よけの指輪</t>
+  </si>
+  <si>
+    <t>混乱状態を防ぎます</t>
+  </si>
+  <si>
+    <t>RING6</t>
+  </si>
+  <si>
+    <t>指輪ダミー6</t>
   </si>
   <si>
     <t>指輪の説明文</t>
-  </si>
-  <si>
-    <t>RING5</t>
-  </si>
-  <si>
-    <t>指輪ダミー5</t>
-  </si>
-  <si>
-    <t>RING6</t>
-  </si>
-  <si>
-    <t>指輪ダミー6</t>
   </si>
   <si>
     <t>RING7</t>
@@ -2585,7 +2591,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.82812" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="1" customWidth="1"/>
@@ -7076,11 +7082,11 @@
       </c>
       <c r="I45" s="6"/>
       <c r="J45" s="5">
-        <v>3</v>
+        <v>500</v>
       </c>
       <c r="K45" s="5">
         <f>J45*0.35</f>
-        <v>1.05</v>
+        <v>175</v>
       </c>
       <c r="L45" s="5">
         <v>142</v>
@@ -7100,19 +7106,19 @@
         <v>361</v>
       </c>
       <c r="D46" s="5"/>
-      <c r="E46" s="4">
-        <v>1</v>
-      </c>
+      <c r="E46" s="6"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="G46" t="s" s="4">
+        <v>106</v>
+      </c>
       <c r="H46" s="5"/>
       <c r="I46" s="6"/>
       <c r="J46" s="5">
-        <v>3</v>
+        <v>2000</v>
       </c>
       <c r="K46" s="5">
         <f>J46*0.35</f>
-        <v>1.05</v>
+        <v>700</v>
       </c>
       <c r="L46" s="5">
         <v>143</v>
@@ -7132,36 +7138,36 @@
         <v>364</v>
       </c>
       <c r="D47" s="5"/>
-      <c r="E47" s="4">
-        <v>1</v>
-      </c>
+      <c r="E47" s="6"/>
       <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="G47" t="s" s="4">
+        <v>114</v>
+      </c>
       <c r="H47" s="5"/>
       <c r="I47" s="6"/>
       <c r="J47" s="5">
-        <v>3</v>
+        <v>2000</v>
       </c>
       <c r="K47" s="5">
         <f>J47*0.35</f>
-        <v>1.05</v>
+        <v>700</v>
       </c>
       <c r="L47" s="5">
         <v>144</v>
       </c>
       <c r="M47" t="s" s="4">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -7182,18 +7188,18 @@
         <v>145</v>
       </c>
       <c r="M48" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B49" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -7214,18 +7220,18 @@
         <v>146</v>
       </c>
       <c r="M49" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -7246,18 +7252,18 @@
         <v>147</v>
       </c>
       <c r="M50" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B51" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -7278,18 +7284,18 @@
         <v>148</v>
       </c>
       <c r="M51" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B52" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -7310,18 +7316,18 @@
         <v>149</v>
       </c>
       <c r="M52" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B53" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -7342,18 +7348,18 @@
         <v>150</v>
       </c>
       <c r="M53" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B54" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -7374,18 +7380,18 @@
         <v>151</v>
       </c>
       <c r="M54" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B55" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -7406,18 +7412,18 @@
         <v>152</v>
       </c>
       <c r="M55" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B56" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -7438,18 +7444,18 @@
         <v>153</v>
       </c>
       <c r="M56" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B57" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -7470,18 +7476,18 @@
         <v>154</v>
       </c>
       <c r="M57" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B58" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -7502,18 +7508,18 @@
         <v>155</v>
       </c>
       <c r="M58" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B59" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -7534,18 +7540,18 @@
         <v>156</v>
       </c>
       <c r="M59" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B60" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -7566,18 +7572,18 @@
         <v>157</v>
       </c>
       <c r="M60" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B61" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -7598,18 +7604,18 @@
         <v>158</v>
       </c>
       <c r="M61" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B62" t="s" s="4">
         <v>351</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -7630,7 +7636,7 @@
         <v>159</v>
       </c>
       <c r="M62" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -7666,16 +7672,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">

</xml_diff>

<commit_message>
fixed #255 FlixelRL-255 反撃の鎧
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="403">
   <si>
     <t>id</t>
   </si>
@@ -988,16 +988,22 @@
     <t>ARMOR8</t>
   </si>
   <si>
-    <t>鎧ダミー8</t>
+    <t>反撃の鎧</t>
+  </si>
+  <si>
+    <t>counter</t>
+  </si>
+  <si>
+    <t>敵の攻撃で受けたダメージを相手に少し与える鎧。防御力5</t>
+  </si>
+  <si>
+    <t>ARMOR9</t>
+  </si>
+  <si>
+    <t>鎧ダミー9</t>
   </si>
   <si>
     <t>防具の説明文</t>
-  </si>
-  <si>
-    <t>ARMOR9</t>
-  </si>
-  <si>
-    <t>鎧ダミー9</t>
   </si>
   <si>
     <t>ARMOR10</t>
@@ -5585,7 +5591,7 @@
     <col min="4" max="4" width="3.125" style="7" customWidth="1"/>
     <col min="5" max="5" width="3.125" style="7" customWidth="1"/>
     <col min="6" max="6" width="3.125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="5.28906" style="7" customWidth="1"/>
+    <col min="7" max="7" width="6.39844" style="7" customWidth="1"/>
     <col min="8" max="8" width="6" style="7" customWidth="1"/>
     <col min="9" max="9" width="3.875" style="7" customWidth="1"/>
     <col min="10" max="10" width="4" style="7" customWidth="1"/>
@@ -6567,37 +6573,39 @@
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="G30" t="s" s="4">
+        <v>325</v>
+      </c>
       <c r="H30" s="5"/>
       <c r="I30" s="4">
         <v>1</v>
       </c>
       <c r="J30" s="5">
-        <v>3</v>
+        <v>2000</v>
       </c>
       <c r="K30" s="5">
         <f>J30*0.35</f>
-        <v>1.05</v>
+        <v>700</v>
       </c>
       <c r="L30" s="5">
         <v>127</v>
       </c>
       <c r="M30" t="s" s="4">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B31" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4">
@@ -6620,18 +6628,18 @@
         <v>128</v>
       </c>
       <c r="M31" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B32" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4">
@@ -6654,18 +6662,18 @@
         <v>129</v>
       </c>
       <c r="M32" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B33" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4">
@@ -6688,18 +6696,18 @@
         <v>130</v>
       </c>
       <c r="M33" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B34" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C34" t="s" s="4">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4">
@@ -6722,18 +6730,18 @@
         <v>131</v>
       </c>
       <c r="M34" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B35" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4">
@@ -6756,18 +6764,18 @@
         <v>132</v>
       </c>
       <c r="M35" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B36" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C36" t="s" s="4">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4">
@@ -6790,18 +6798,18 @@
         <v>133</v>
       </c>
       <c r="M36" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B37" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C37" t="s" s="4">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4">
@@ -6824,18 +6832,18 @@
         <v>134</v>
       </c>
       <c r="M37" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B38" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4">
@@ -6858,18 +6866,18 @@
         <v>135</v>
       </c>
       <c r="M38" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B39" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C39" t="s" s="4">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4">
@@ -6892,18 +6900,18 @@
         <v>136</v>
       </c>
       <c r="M39" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B40" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C40" t="s" s="4">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4">
@@ -6926,18 +6934,18 @@
         <v>137</v>
       </c>
       <c r="M40" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B41" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C41" t="s" s="4">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4">
@@ -6960,18 +6968,18 @@
         <v>138</v>
       </c>
       <c r="M41" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B42" t="s" s="4">
         <v>302</v>
       </c>
       <c r="C42" t="s" s="4">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4">
@@ -6994,18 +7002,18 @@
         <v>139</v>
       </c>
       <c r="M42" t="s" s="4">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D43" s="5">
         <v>1</v>
@@ -7026,18 +7034,18 @@
         <v>140</v>
       </c>
       <c r="M43" t="s" s="4">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4">
@@ -7058,18 +7066,18 @@
         <v>141</v>
       </c>
       <c r="M44" t="s" s="4">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C45" t="s" s="4">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="6"/>
@@ -7092,18 +7100,18 @@
         <v>142</v>
       </c>
       <c r="M45" t="s" s="4">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C46" t="s" s="4">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="6"/>
@@ -7124,18 +7132,18 @@
         <v>143</v>
       </c>
       <c r="M46" t="s" s="4">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="6"/>
@@ -7156,18 +7164,18 @@
         <v>144</v>
       </c>
       <c r="M47" t="s" s="4">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C48" t="s" s="4">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -7188,18 +7196,18 @@
         <v>145</v>
       </c>
       <c r="M48" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -7220,18 +7228,18 @@
         <v>146</v>
       </c>
       <c r="M49" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -7252,18 +7260,18 @@
         <v>147</v>
       </c>
       <c r="M50" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -7284,18 +7292,18 @@
         <v>148</v>
       </c>
       <c r="M51" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -7316,18 +7324,18 @@
         <v>149</v>
       </c>
       <c r="M52" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -7348,18 +7356,18 @@
         <v>150</v>
       </c>
       <c r="M53" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -7380,18 +7388,18 @@
         <v>151</v>
       </c>
       <c r="M54" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -7412,18 +7420,18 @@
         <v>152</v>
       </c>
       <c r="M55" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -7444,18 +7452,18 @@
         <v>153</v>
       </c>
       <c r="M56" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -7476,18 +7484,18 @@
         <v>154</v>
       </c>
       <c r="M57" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -7508,18 +7516,18 @@
         <v>155</v>
       </c>
       <c r="M58" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -7540,18 +7548,18 @@
         <v>156</v>
       </c>
       <c r="M59" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -7572,18 +7580,18 @@
         <v>157</v>
       </c>
       <c r="M60" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -7604,18 +7612,18 @@
         <v>158</v>
       </c>
       <c r="M61" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -7636,7 +7644,7 @@
         <v>159</v>
       </c>
       <c r="M62" t="s" s="4">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -7653,7 +7661,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -7672,16 +7680,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -8426,7 +8434,7 @@
         <v>10</v>
       </c>
       <c r="D45" t="s" s="4">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E45" s="4">
         <v>10</v>
@@ -8443,7 +8451,7 @@
         <v>10</v>
       </c>
       <c r="D46" t="s" s="4">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E46" s="4">
         <v>10</v>
@@ -8460,7 +8468,7 @@
         <v>10</v>
       </c>
       <c r="D47" t="s" s="4">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E47" s="4">
         <v>10</v>
@@ -8497,6 +8505,40 @@
         <v>205</v>
       </c>
       <c r="E49" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" ht="20" customHeight="1">
+      <c r="A50" s="3">
+        <v>48</v>
+      </c>
+      <c r="B50" s="4">
+        <v>1</v>
+      </c>
+      <c r="C50" s="4">
+        <v>10</v>
+      </c>
+      <c r="D50" t="s" s="4">
+        <v>362</v>
+      </c>
+      <c r="E50" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" ht="20" customHeight="1">
+      <c r="A51" s="3">
+        <v>49</v>
+      </c>
+      <c r="B51" s="4">
+        <v>1</v>
+      </c>
+      <c r="C51" s="4">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s" s="4">
+        <v>365</v>
+      </c>
+      <c r="E51" s="4">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed #400 FlixelRL-400 通過の指輪
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="405">
   <si>
     <t>id</t>
   </si>
@@ -1123,16 +1123,22 @@
     <t>RING6</t>
   </si>
   <si>
-    <t>指輪ダミー6</t>
+    <t>通過の指輪</t>
+  </si>
+  <si>
+    <t>passage</t>
+  </si>
+  <si>
+    <t>透明な壁を移動できるようになります</t>
+  </si>
+  <si>
+    <t>RING7</t>
+  </si>
+  <si>
+    <t>指輪ダミー7</t>
   </si>
   <si>
     <t>指輪の説明文</t>
-  </si>
-  <si>
-    <t>RING7</t>
-  </si>
-  <si>
-    <t>指輪ダミー7</t>
   </si>
   <si>
     <t>RING8</t>
@@ -7178,36 +7184,36 @@
         <v>369</v>
       </c>
       <c r="D48" s="5"/>
-      <c r="E48" s="4">
-        <v>1</v>
-      </c>
+      <c r="E48" s="6"/>
       <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="G48" t="s" s="4">
+        <v>370</v>
+      </c>
       <c r="H48" s="5"/>
       <c r="I48" s="6"/>
       <c r="J48" s="5">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="K48" s="5">
         <f>J48*0.35</f>
-        <v>1.05</v>
+        <v>1050</v>
       </c>
       <c r="L48" s="5">
         <v>145</v>
       </c>
       <c r="M48" t="s" s="4">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B49" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -7228,18 +7234,18 @@
         <v>146</v>
       </c>
       <c r="M49" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -7260,18 +7266,18 @@
         <v>147</v>
       </c>
       <c r="M50" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B51" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -7292,18 +7298,18 @@
         <v>148</v>
       </c>
       <c r="M51" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B52" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -7324,18 +7330,18 @@
         <v>149</v>
       </c>
       <c r="M52" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B53" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -7356,18 +7362,18 @@
         <v>150</v>
       </c>
       <c r="M53" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B54" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -7388,18 +7394,18 @@
         <v>151</v>
       </c>
       <c r="M54" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B55" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C55" t="s" s="4">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -7420,18 +7426,18 @@
         <v>152</v>
       </c>
       <c r="M55" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B56" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C56" t="s" s="4">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -7452,18 +7458,18 @@
         <v>153</v>
       </c>
       <c r="M56" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B57" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C57" t="s" s="4">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -7484,18 +7490,18 @@
         <v>154</v>
       </c>
       <c r="M57" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B58" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -7516,18 +7522,18 @@
         <v>155</v>
       </c>
       <c r="M58" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B59" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C59" t="s" s="4">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -7548,18 +7554,18 @@
         <v>156</v>
       </c>
       <c r="M59" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B60" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C60" t="s" s="4">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -7580,18 +7586,18 @@
         <v>157</v>
       </c>
       <c r="M60" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B61" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C61" t="s" s="4">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -7612,18 +7618,18 @@
         <v>158</v>
       </c>
       <c r="M61" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B62" t="s" s="4">
         <v>353</v>
       </c>
       <c r="C62" t="s" s="4">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -7644,7 +7650,7 @@
         <v>159</v>
       </c>
       <c r="M62" t="s" s="4">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -7680,16 +7686,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">

</xml_diff>

<commit_message>
fixed #497 FlixelRL-497 Floor7〜10の敵を設定
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -799,10 +799,10 @@
     <t>Weapon</t>
   </si>
   <si>
-    <t>竹刀</t>
-  </si>
-  <si>
-    <t>竹で作られた刀。攻撃力1</t>
+    <t>木の棒</t>
+  </si>
+  <si>
+    <t>ただの木の棒。攻撃力2</t>
   </si>
   <si>
     <t>WEAPON2</t>
@@ -811,7 +811,7 @@
     <t>木刀</t>
   </si>
   <si>
-    <t>木で作られた刀。攻撃力2</t>
+    <t>木で作られた刀。攻撃力4</t>
   </si>
   <si>
     <t>WEAPON3</t>
@@ -820,7 +820,7 @@
     <t>ダガー</t>
   </si>
   <si>
-    <t>小型の刃物。攻撃力3</t>
+    <t>小型の刃物。攻撃力6</t>
   </si>
   <si>
     <t>WEAPON4</t>
@@ -829,7 +829,7 @@
     <t>レイピア</t>
   </si>
   <si>
-    <t>細身の剣。攻撃力5</t>
+    <t>細身の剣。攻撃力10</t>
   </si>
   <si>
     <t>WEAPON5</t>
@@ -838,7 +838,7 @@
     <t>三日月刀</t>
   </si>
   <si>
-    <t>よく切れる刀。攻撃力7</t>
+    <t>よく切れる刀。攻撃力14</t>
   </si>
   <si>
     <t>WEAPON6</t>
@@ -847,7 +847,7 @@
     <t>妖刀ムラマサ</t>
   </si>
   <si>
-    <t>妖気を帯びた刀。攻撃力8</t>
+    <t>妖気を帯びた刀。攻撃力16</t>
   </si>
   <si>
     <t>WEAPON7</t>
@@ -856,7 +856,7 @@
     <t>聖騎士の剣</t>
   </si>
   <si>
-    <t>聖なる祝福を受けた剣。攻撃力10</t>
+    <t>聖なる祝福を受けた剣。攻撃力20</t>
   </si>
   <si>
     <t>WEAPON8</t>
@@ -868,7 +868,7 @@
     <t>drill</t>
   </si>
   <si>
-    <t>壁を壊せる武器。しかし一定回数で壊れてしまう。攻撃力5</t>
+    <t>壁を壊せる武器。しかし一定回数で壊れてしまう。攻撃力10</t>
   </si>
   <si>
     <t>WEAPON9</t>
@@ -955,7 +955,7 @@
     <t>ローブ</t>
   </si>
   <si>
-    <t>敵の攻撃を少しだけ防ぐ衣服。防御力1</t>
+    <t>敵の攻撃を少しだけ防ぐ衣服。防御力2</t>
   </si>
   <si>
     <t>ARMOR2</t>
@@ -964,7 +964,7 @@
     <t>毛皮の鎧</t>
   </si>
   <si>
-    <t>丈夫な皮で作られた鎧。防御力2</t>
+    <t>丈夫な皮で作られた鎧。防御力4</t>
   </si>
   <si>
     <t>ARMOR3</t>
@@ -973,7 +973,7 @@
     <t>鎖かたびら</t>
   </si>
   <si>
-    <t>鎖を編んで作られた鎧。防御力3</t>
+    <t>鎖を編んで作られた鎧。防御力6</t>
   </si>
   <si>
     <t>ARMOR4</t>
@@ -982,7 +982,7 @@
     <t>エルフの鎧</t>
   </si>
   <si>
-    <t>エルフが身につける鎧。防御力5</t>
+    <t>エルフが身につける鎧。防御力10</t>
   </si>
   <si>
     <t>ARMOR5</t>
@@ -991,7 +991,7 @@
     <t>メタルアーマー</t>
   </si>
   <si>
-    <t>鋼で作られた丈夫な鎧。防御力7</t>
+    <t>鋼で作られた丈夫な鎧。防御力14</t>
   </si>
   <si>
     <t>ARMOR6</t>
@@ -1000,7 +1000,7 @@
     <t>銀のジャケット</t>
   </si>
   <si>
-    <t>魔法の銀で作られた防具。防御力8</t>
+    <t>魔法の銀で作られた防具。防御力16</t>
   </si>
   <si>
     <t>ARMOR7</t>
@@ -1009,7 +1009,7 @@
     <t>プラチナメイル</t>
   </si>
   <si>
-    <t>プラチナ製の強力な鎧。防御力10</t>
+    <t>プラチナ製の強力な鎧。防御力20</t>
   </si>
   <si>
     <t>ARMOR8</t>
@@ -1021,7 +1021,7 @@
     <t>counter</t>
   </si>
   <si>
-    <t>敵の攻撃で受けたダメージを相手に少し与える鎧。防御力5</t>
+    <t>敵の攻撃で受けたダメージを相手に少し与える鎧。防御力10</t>
   </si>
   <si>
     <t>ARMOR9</t>
@@ -1322,7 +1322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1345,13 +1345,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1380,6 +1406,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4501,11 +4533,11 @@
         <v>1</v>
       </c>
       <c r="J54" s="6">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="K54" s="6">
         <f>J54*0.35</f>
-        <v>1.05</v>
+        <v>350</v>
       </c>
       <c r="L54" s="6">
         <v>235</v>
@@ -4535,11 +4567,11 @@
         <v>2</v>
       </c>
       <c r="J55" s="6">
-        <v>3</v>
+        <v>1500</v>
       </c>
       <c r="K55" s="6">
         <f>J55*0.35</f>
-        <v>1.05</v>
+        <v>525</v>
       </c>
       <c r="L55" s="6">
         <v>236</v>
@@ -4569,11 +4601,11 @@
         <v>1</v>
       </c>
       <c r="J56" s="6">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="K56" s="6">
         <f>J56*0.35</f>
-        <v>1.05</v>
+        <v>350</v>
       </c>
       <c r="L56" s="6">
         <v>237</v>
@@ -4603,11 +4635,11 @@
         <v>1</v>
       </c>
       <c r="J57" s="6">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="K57" s="6">
         <f>J57*0.35</f>
-        <v>1.05</v>
+        <v>350</v>
       </c>
       <c r="L57" s="6">
         <v>238</v>
@@ -5753,7 +5785,7 @@
         <v>261</v>
       </c>
       <c r="D3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -5761,11 +5793,11 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="K3" s="6">
         <f>J3*0.35</f>
-        <v>105</v>
+        <v>17.5</v>
       </c>
       <c r="L3" s="6">
         <v>100</v>
@@ -5785,7 +5817,7 @@
         <v>264</v>
       </c>
       <c r="D4" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -5793,11 +5825,11 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="K4" s="6">
         <f>J4*0.35</f>
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="L4" s="6">
         <v>101</v>
@@ -5817,7 +5849,7 @@
         <v>267</v>
       </c>
       <c r="D5" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -5825,11 +5857,11 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K5" s="6">
         <f>J5*0.35</f>
-        <v>175</v>
+        <v>87.5</v>
       </c>
       <c r="L5" s="6">
         <v>102</v>
@@ -5849,7 +5881,7 @@
         <v>270</v>
       </c>
       <c r="D6" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -5881,7 +5913,7 @@
         <v>273</v>
       </c>
       <c r="D7" s="5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -5913,7 +5945,7 @@
         <v>276</v>
       </c>
       <c r="D8" s="5">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -5945,7 +5977,7 @@
         <v>279</v>
       </c>
       <c r="D9" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -5977,7 +6009,7 @@
         <v>282</v>
       </c>
       <c r="D10" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -6398,7 +6430,7 @@
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -6407,11 +6439,11 @@
         <v>1</v>
       </c>
       <c r="J23" s="6">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="K23" s="6">
         <f>J23*0.35</f>
-        <v>105</v>
+        <v>17.5</v>
       </c>
       <c r="L23" s="6">
         <v>120</v>
@@ -6432,7 +6464,7 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -6441,11 +6473,11 @@
         <v>1</v>
       </c>
       <c r="J24" s="6">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="K24" s="6">
         <f>J24*0.35</f>
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="L24" s="6">
         <v>121</v>
@@ -6466,7 +6498,7 @@
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -6475,11 +6507,11 @@
         <v>1</v>
       </c>
       <c r="J25" s="6">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K25" s="6">
         <f>J25*0.35</f>
-        <v>175</v>
+        <v>87.5</v>
       </c>
       <c r="L25" s="6">
         <v>122</v>
@@ -6500,7 +6532,7 @@
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -6534,7 +6566,7 @@
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -6568,7 +6600,7 @@
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="5">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
@@ -6602,7 +6634,7 @@
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -6636,7 +6668,7 @@
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" t="s" s="5">
@@ -7724,7 +7756,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -7780,13 +7812,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>259</v>
+        <v>15</v>
       </c>
       <c r="E3" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -7797,13 +7829,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="D4" t="s" s="5">
-        <v>263</v>
+        <v>19</v>
       </c>
       <c r="E4" s="5">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -7814,13 +7846,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>266</v>
+        <v>22</v>
       </c>
       <c r="E5" s="5">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -7831,10 +7863,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="5">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>269</v>
+        <v>25</v>
       </c>
       <c r="E6" s="5">
         <v>10</v>
@@ -7851,10 +7883,10 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="5">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="E7" s="5">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -7865,13 +7897,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s" s="5">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="E8" s="5">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -7882,13 +7914,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s" s="5">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="E9" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -7896,16 +7928,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C10" s="5">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s" s="5">
+        <v>269</v>
+      </c>
+      <c r="E10" s="5">
         <v>10</v>
-      </c>
-      <c r="D10" t="s" s="5">
-        <v>310</v>
-      </c>
-      <c r="E10" s="5">
-        <v>50</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -7913,16 +7945,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="5">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C11" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s" s="5">
-        <v>314</v>
+        <v>272</v>
       </c>
       <c r="E11" s="5">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -7930,16 +7962,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="5">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C12" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>317</v>
+        <v>275</v>
       </c>
       <c r="E12" s="5">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -7947,16 +7979,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="5">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C13" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s" s="5">
-        <v>320</v>
+        <v>278</v>
       </c>
       <c r="E13" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
@@ -7970,10 +8002,10 @@
         <v>10</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="E14" s="5">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
@@ -7984,13 +8016,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s" s="5">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="E15" s="5">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -8001,13 +8033,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="E16" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
@@ -8015,16 +8047,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C17" s="5">
-        <v>1000</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s" s="5">
-        <v>15</v>
+        <v>320</v>
       </c>
       <c r="E17" s="5">
-        <v>200</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
@@ -8032,16 +8064,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C18" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s" s="5">
-        <v>19</v>
+        <v>323</v>
       </c>
       <c r="E18" s="5">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -8049,16 +8081,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="5">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C19" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s" s="5">
-        <v>22</v>
+        <v>326</v>
       </c>
       <c r="E19" s="5">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
@@ -8066,16 +8098,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="5">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C20" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s" s="5">
-        <v>25</v>
+        <v>329</v>
       </c>
       <c r="E20" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
@@ -8086,7 +8118,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s" s="5">
         <v>42</v>
@@ -8103,7 +8135,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s" s="5">
         <v>46</v>
@@ -8134,10 +8166,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C24" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s" s="5">
         <v>52</v>
@@ -8151,10 +8183,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C25" s="5">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s" s="5">
         <v>55</v>
@@ -8168,10 +8200,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="5">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C26" s="5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s" s="5">
         <v>58</v>
@@ -8188,7 +8220,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s" s="5">
         <v>91</v>
@@ -8222,7 +8254,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s" s="5">
         <v>98</v>
@@ -8239,13 +8271,13 @@
         <v>1</v>
       </c>
       <c r="C30" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s" s="5">
         <v>101</v>
       </c>
       <c r="E30" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
@@ -8256,13 +8288,13 @@
         <v>1</v>
       </c>
       <c r="C31" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s" s="5">
         <v>104</v>
       </c>
       <c r="E31" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
@@ -8273,13 +8305,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s" s="5">
         <v>108</v>
       </c>
       <c r="E32" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
@@ -8290,13 +8322,13 @@
         <v>1</v>
       </c>
       <c r="C33" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D33" t="s" s="5">
         <v>112</v>
       </c>
       <c r="E33" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -8307,13 +8339,13 @@
         <v>1</v>
       </c>
       <c r="C34" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D34" t="s" s="5">
         <v>116</v>
       </c>
       <c r="E34" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
@@ -8324,13 +8356,13 @@
         <v>1</v>
       </c>
       <c r="C35" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s" s="5">
         <v>120</v>
       </c>
       <c r="E35" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
@@ -8341,13 +8373,13 @@
         <v>1</v>
       </c>
       <c r="C36" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D36" t="s" s="5">
         <v>124</v>
       </c>
       <c r="E36" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
@@ -8355,13 +8387,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C37" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s" s="5">
-        <v>190</v>
+        <v>128</v>
       </c>
       <c r="E37" s="5">
         <v>10</v>
@@ -8375,10 +8407,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s" s="5">
-        <v>194</v>
+        <v>132</v>
       </c>
       <c r="E38" s="5">
         <v>10</v>
@@ -8392,13 +8424,13 @@
         <v>1</v>
       </c>
       <c r="C39" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s" s="5">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="E39" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
@@ -8409,13 +8441,13 @@
         <v>1</v>
       </c>
       <c r="C40" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D40" t="s" s="5">
-        <v>200</v>
+        <v>167</v>
       </c>
       <c r="E40" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
@@ -8426,10 +8458,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D41" t="s" s="5">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="E41" s="5">
         <v>10</v>
@@ -8443,10 +8475,10 @@
         <v>1</v>
       </c>
       <c r="C42" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D42" t="s" s="5">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E42" s="5">
         <v>10</v>
@@ -8460,10 +8492,10 @@
         <v>1</v>
       </c>
       <c r="C43" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D43" t="s" s="5">
-        <v>128</v>
+        <v>197</v>
       </c>
       <c r="E43" s="5">
         <v>10</v>
@@ -8477,10 +8509,10 @@
         <v>1</v>
       </c>
       <c r="C44" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D44" t="s" s="5">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E44" s="5">
         <v>10</v>
@@ -8494,13 +8526,13 @@
         <v>1</v>
       </c>
       <c r="C45" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D45" t="s" s="5">
-        <v>361</v>
+        <v>203</v>
       </c>
       <c r="E45" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
@@ -8511,13 +8543,13 @@
         <v>1</v>
       </c>
       <c r="C46" s="5">
-        <v>10</v>
-      </c>
-      <c r="D46" t="s" s="5">
-        <v>365</v>
+        <v>50</v>
+      </c>
+      <c r="D46" t="s" s="10">
+        <v>206</v>
       </c>
       <c r="E46" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
@@ -8525,13 +8557,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C47" s="5">
-        <v>10</v>
-      </c>
-      <c r="D47" t="s" s="5">
-        <v>368</v>
+        <v>50</v>
+      </c>
+      <c r="D47" t="s" s="11">
+        <v>209</v>
       </c>
       <c r="E47" s="5">
         <v>10</v>
@@ -8545,10 +8577,10 @@
         <v>1</v>
       </c>
       <c r="C48" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D48" t="s" s="5">
-        <v>132</v>
+        <v>212</v>
       </c>
       <c r="E48" s="5">
         <v>10</v>
@@ -8562,10 +8594,10 @@
         <v>1</v>
       </c>
       <c r="C49" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D49" t="s" s="5">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E49" s="5">
         <v>10</v>
@@ -8582,7 +8614,7 @@
         <v>10</v>
       </c>
       <c r="D50" t="s" s="5">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="E50" s="5">
         <v>10</v>
@@ -8599,9 +8631,60 @@
         <v>10</v>
       </c>
       <c r="D51" t="s" s="5">
+        <v>365</v>
+      </c>
+      <c r="E51" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" ht="20" customHeight="1">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1</v>
+      </c>
+      <c r="C52" s="5">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s" s="5">
+        <v>368</v>
+      </c>
+      <c r="E52" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" ht="20" customHeight="1">
+      <c r="A53" s="3">
+        <v>51</v>
+      </c>
+      <c r="B53" s="5">
+        <v>20</v>
+      </c>
+      <c r="C53" s="5">
+        <v>50</v>
+      </c>
+      <c r="D53" t="s" s="5">
+        <v>371</v>
+      </c>
+      <c r="E53" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" ht="20" customHeight="1">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54" s="5">
+        <v>20</v>
+      </c>
+      <c r="C54" s="5">
+        <v>50</v>
+      </c>
+      <c r="D54" t="s" s="5">
         <v>374</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E54" s="5">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed #395 FlixelRL-395 HP交換の杖
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="417">
   <si>
     <t>id</t>
   </si>
@@ -676,18 +676,24 @@
     <t>WAND10</t>
   </si>
   <si>
-    <t>杖10</t>
+    <t>HP交換の杖</t>
+  </si>
+  <si>
+    <t>hpswap</t>
+  </si>
+  <si>
+    <t>相手とプレイヤーのHPを入れ替えます</t>
+  </si>
+  <si>
+    <t>WAND11</t>
+  </si>
+  <si>
+    <t>杖11</t>
   </si>
   <si>
     <t>杖の説明文</t>
   </si>
   <si>
-    <t>WAND11</t>
-  </si>
-  <si>
-    <t>杖11</t>
-  </si>
-  <si>
     <t>WAND12</t>
   </si>
   <si>
@@ -1256,6 +1262,9 @@
   </si>
   <si>
     <t>ratio</t>
+  </si>
+  <si>
+    <t>comment</t>
   </si>
 </sst>
 </file>
@@ -5220,31 +5229,33 @@
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
+      <c r="H76" t="s" s="5">
+        <v>221</v>
+      </c>
       <c r="I76" s="7"/>
       <c r="J76" s="6">
-        <v>3</v>
+        <v>1500</v>
       </c>
       <c r="K76" s="6">
         <f>J76*0.35</f>
-        <v>1.05</v>
+        <v>525</v>
       </c>
       <c r="L76" s="6">
         <v>257</v>
       </c>
       <c r="M76" t="s" s="5">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" t="s" s="3">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B77" t="s" s="5">
         <v>191</v>
       </c>
       <c r="C77" t="s" s="5">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="6"/>
@@ -5263,18 +5274,18 @@
         <v>258</v>
       </c>
       <c r="M77" t="s" s="5">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B78" t="s" s="5">
         <v>191</v>
       </c>
       <c r="C78" t="s" s="5">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="6"/>
@@ -5293,18 +5304,18 @@
         <v>259</v>
       </c>
       <c r="M78" t="s" s="5">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" t="s" s="3">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B79" t="s" s="5">
         <v>191</v>
       </c>
       <c r="C79" t="s" s="5">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="6"/>
@@ -5323,18 +5334,18 @@
         <v>260</v>
       </c>
       <c r="M79" t="s" s="5">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B80" t="s" s="5">
         <v>191</v>
       </c>
       <c r="C80" t="s" s="5">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="6"/>
@@ -5353,18 +5364,18 @@
         <v>261</v>
       </c>
       <c r="M80" t="s" s="5">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" t="s" s="3">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B81" t="s" s="5">
         <v>191</v>
       </c>
       <c r="C81" t="s" s="5">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="6"/>
@@ -5383,18 +5394,18 @@
         <v>262</v>
       </c>
       <c r="M81" t="s" s="5">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B82" t="s" s="5">
         <v>191</v>
       </c>
       <c r="C82" t="s" s="5">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="6"/>
@@ -5413,18 +5424,18 @@
         <v>263</v>
       </c>
       <c r="M82" t="s" s="5">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
       <c r="A83" t="s" s="3">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B83" t="s" s="5">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C83" t="s" s="5">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="6"/>
@@ -5443,18 +5454,18 @@
         <v>264</v>
       </c>
       <c r="M83" t="s" s="5">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="84" ht="20" customHeight="1">
       <c r="A84" t="s" s="3">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B84" t="s" s="5">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C84" t="s" s="5">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="6"/>
@@ -5473,18 +5484,18 @@
         <v>265</v>
       </c>
       <c r="M84" t="s" s="5">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="85" ht="20" customHeight="1">
       <c r="A85" t="s" s="3">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B85" t="s" s="5">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C85" t="s" s="5">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="6"/>
@@ -5503,18 +5514,18 @@
         <v>266</v>
       </c>
       <c r="M85" t="s" s="5">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="86" ht="20" customHeight="1">
       <c r="A86" t="s" s="3">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B86" t="s" s="5">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C86" t="s" s="5">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="6"/>
@@ -5533,18 +5544,18 @@
         <v>267</v>
       </c>
       <c r="M86" t="s" s="5">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="87" ht="20" customHeight="1">
       <c r="A87" t="s" s="3">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B87" t="s" s="5">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C87" t="s" s="5">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="6"/>
@@ -5563,18 +5574,18 @@
         <v>268</v>
       </c>
       <c r="M87" t="s" s="5">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="88" ht="20" customHeight="1">
       <c r="A88" t="s" s="3">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B88" t="s" s="5">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C88" t="s" s="5">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="6"/>
@@ -5593,18 +5604,18 @@
         <v>269</v>
       </c>
       <c r="M88" t="s" s="5">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="89" ht="20" customHeight="1">
       <c r="A89" t="s" s="3">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B89" t="s" s="5">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C89" t="s" s="5">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="6"/>
@@ -5623,18 +5634,18 @@
         <v>270</v>
       </c>
       <c r="M89" t="s" s="5">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="90" ht="20" customHeight="1">
       <c r="A90" t="s" s="3">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B90" t="s" s="5">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C90" t="s" s="5">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D90" s="7"/>
       <c r="E90" s="6"/>
@@ -5653,7 +5664,7 @@
         <v>271</v>
       </c>
       <c r="M90" t="s" s="5">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -5706,16 +5717,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="G1" t="s" s="2">
         <v>7</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>4</v>
@@ -5776,13 +5787,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D3" s="5">
         <v>2</v>
@@ -5803,18 +5814,18 @@
         <v>100</v>
       </c>
       <c r="M3" t="s" s="5">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D4" s="5">
         <v>4</v>
@@ -5835,18 +5846,18 @@
         <v>101</v>
       </c>
       <c r="M4" t="s" s="5">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D5" s="5">
         <v>6</v>
@@ -5867,18 +5878,18 @@
         <v>102</v>
       </c>
       <c r="M5" t="s" s="5">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D6" s="5">
         <v>10</v>
@@ -5899,18 +5910,18 @@
         <v>103</v>
       </c>
       <c r="M6" t="s" s="5">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B7" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C7" t="s" s="5">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D7" s="5">
         <v>14</v>
@@ -5931,18 +5942,18 @@
         <v>104</v>
       </c>
       <c r="M7" t="s" s="5">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C8" t="s" s="5">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D8" s="5">
         <v>16</v>
@@ -5963,18 +5974,18 @@
         <v>105</v>
       </c>
       <c r="M8" t="s" s="5">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B9" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D9" s="5">
         <v>20</v>
@@ -5995,18 +6006,18 @@
         <v>106</v>
       </c>
       <c r="M9" t="s" s="5">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B10" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C10" t="s" s="5">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D10" s="5">
         <v>10</v>
@@ -6014,7 +6025,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" t="s" s="5">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="H10" s="6">
         <v>50</v>
@@ -6031,18 +6042,18 @@
         <v>107</v>
       </c>
       <c r="M10" t="s" s="5">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B11" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C11" t="s" s="5">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
@@ -6063,18 +6074,18 @@
         <v>108</v>
       </c>
       <c r="M11" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B12" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C12" t="s" s="5">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
@@ -6095,18 +6106,18 @@
         <v>109</v>
       </c>
       <c r="M12" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B13" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C13" t="s" s="5">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
@@ -6127,18 +6138,18 @@
         <v>110</v>
       </c>
       <c r="M13" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B14" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C14" t="s" s="5">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
@@ -6159,18 +6170,18 @@
         <v>111</v>
       </c>
       <c r="M14" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B15" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C15" t="s" s="5">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
@@ -6191,18 +6202,18 @@
         <v>112</v>
       </c>
       <c r="M15" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B16" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C16" t="s" s="5">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D16" s="5">
         <v>1</v>
@@ -6223,18 +6234,18 @@
         <v>113</v>
       </c>
       <c r="M16" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B17" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C17" t="s" s="5">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D17" s="5">
         <v>1</v>
@@ -6255,18 +6266,18 @@
         <v>114</v>
       </c>
       <c r="M17" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B18" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C18" t="s" s="5">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -6287,18 +6298,18 @@
         <v>115</v>
       </c>
       <c r="M18" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B19" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C19" t="s" s="5">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D19" s="5">
         <v>1</v>
@@ -6319,18 +6330,18 @@
         <v>116</v>
       </c>
       <c r="M19" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B20" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C20" t="s" s="5">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D20" s="5">
         <v>1</v>
@@ -6351,18 +6362,18 @@
         <v>117</v>
       </c>
       <c r="M20" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B21" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C21" t="s" s="5">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D21" s="5">
         <v>1</v>
@@ -6383,18 +6394,18 @@
         <v>118</v>
       </c>
       <c r="M21" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B22" t="s" s="5">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C22" t="s" s="5">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
@@ -6415,18 +6426,18 @@
         <v>119</v>
       </c>
       <c r="M22" t="s" s="5">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B23" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C23" t="s" s="5">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="5">
@@ -6449,18 +6460,18 @@
         <v>120</v>
       </c>
       <c r="M23" t="s" s="5">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B24" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C24" t="s" s="5">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="5">
@@ -6483,18 +6494,18 @@
         <v>121</v>
       </c>
       <c r="M24" t="s" s="5">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B25" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C25" t="s" s="5">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="5">
@@ -6517,18 +6528,18 @@
         <v>122</v>
       </c>
       <c r="M25" t="s" s="5">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B26" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C26" t="s" s="5">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="5">
@@ -6551,18 +6562,18 @@
         <v>123</v>
       </c>
       <c r="M26" t="s" s="5">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B27" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C27" t="s" s="5">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="5">
@@ -6585,18 +6596,18 @@
         <v>124</v>
       </c>
       <c r="M27" t="s" s="5">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B28" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C28" t="s" s="5">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="5">
@@ -6619,18 +6630,18 @@
         <v>125</v>
       </c>
       <c r="M28" t="s" s="5">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B29" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C29" t="s" s="5">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="5">
@@ -6653,18 +6664,18 @@
         <v>126</v>
       </c>
       <c r="M29" t="s" s="5">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B30" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C30" t="s" s="5">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="5">
@@ -6672,7 +6683,7 @@
       </c>
       <c r="F30" s="6"/>
       <c r="G30" t="s" s="5">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="5">
@@ -6689,18 +6700,18 @@
         <v>127</v>
       </c>
       <c r="M30" t="s" s="5">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B31" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C31" t="s" s="5">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="5">
@@ -6723,18 +6734,18 @@
         <v>128</v>
       </c>
       <c r="M31" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B32" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C32" t="s" s="5">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="5">
@@ -6757,18 +6768,18 @@
         <v>129</v>
       </c>
       <c r="M32" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B33" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C33" t="s" s="5">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="5">
@@ -6791,18 +6802,18 @@
         <v>130</v>
       </c>
       <c r="M33" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B34" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C34" t="s" s="5">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="5">
@@ -6825,18 +6836,18 @@
         <v>131</v>
       </c>
       <c r="M34" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B35" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C35" t="s" s="5">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="5">
@@ -6859,18 +6870,18 @@
         <v>132</v>
       </c>
       <c r="M35" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B36" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C36" t="s" s="5">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="5">
@@ -6893,18 +6904,18 @@
         <v>133</v>
       </c>
       <c r="M36" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B37" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C37" t="s" s="5">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="5">
@@ -6927,18 +6938,18 @@
         <v>134</v>
       </c>
       <c r="M37" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B38" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C38" t="s" s="5">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="5">
@@ -6961,18 +6972,18 @@
         <v>135</v>
       </c>
       <c r="M38" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B39" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C39" t="s" s="5">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="5">
@@ -6995,18 +7006,18 @@
         <v>136</v>
       </c>
       <c r="M39" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B40" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C40" t="s" s="5">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="5">
@@ -7029,18 +7040,18 @@
         <v>137</v>
       </c>
       <c r="M40" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B41" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C41" t="s" s="5">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="5">
@@ -7063,18 +7074,18 @@
         <v>138</v>
       </c>
       <c r="M41" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B42" t="s" s="5">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C42" t="s" s="5">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="5">
@@ -7097,18 +7108,18 @@
         <v>139</v>
       </c>
       <c r="M42" t="s" s="5">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B43" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C43" t="s" s="5">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D43" s="6">
         <v>1</v>
@@ -7129,18 +7140,18 @@
         <v>140</v>
       </c>
       <c r="M43" t="s" s="5">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B44" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C44" t="s" s="5">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="5">
@@ -7161,18 +7172,18 @@
         <v>141</v>
       </c>
       <c r="M44" t="s" s="5">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B45" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C45" t="s" s="5">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="7"/>
@@ -7195,18 +7206,18 @@
         <v>142</v>
       </c>
       <c r="M45" t="s" s="5">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B46" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C46" t="s" s="5">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="7"/>
@@ -7227,18 +7238,18 @@
         <v>143</v>
       </c>
       <c r="M46" t="s" s="5">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B47" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C47" t="s" s="5">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="7"/>
@@ -7259,24 +7270,24 @@
         <v>144</v>
       </c>
       <c r="M47" t="s" s="5">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B48" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C48" t="s" s="5">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="7"/>
       <c r="F48" s="6"/>
       <c r="G48" t="s" s="5">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="7"/>
@@ -7291,18 +7302,18 @@
         <v>145</v>
       </c>
       <c r="M48" t="s" s="5">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B49" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C49" t="s" s="5">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="5">
@@ -7323,18 +7334,18 @@
         <v>146</v>
       </c>
       <c r="M49" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B50" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C50" t="s" s="5">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="5">
@@ -7355,18 +7366,18 @@
         <v>147</v>
       </c>
       <c r="M50" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B51" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C51" t="s" s="5">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5">
@@ -7387,18 +7398,18 @@
         <v>148</v>
       </c>
       <c r="M51" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B52" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C52" t="s" s="5">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="5">
@@ -7419,18 +7430,18 @@
         <v>149</v>
       </c>
       <c r="M52" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B53" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C53" t="s" s="5">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5">
@@ -7451,18 +7462,18 @@
         <v>150</v>
       </c>
       <c r="M53" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B54" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C54" t="s" s="5">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5">
@@ -7483,18 +7494,18 @@
         <v>151</v>
       </c>
       <c r="M54" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B55" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C55" t="s" s="5">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="5">
@@ -7515,18 +7526,18 @@
         <v>152</v>
       </c>
       <c r="M55" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B56" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C56" t="s" s="5">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="5">
@@ -7547,18 +7558,18 @@
         <v>153</v>
       </c>
       <c r="M56" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B57" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C57" t="s" s="5">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="5">
@@ -7579,18 +7590,18 @@
         <v>154</v>
       </c>
       <c r="M57" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B58" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C58" t="s" s="5">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="5">
@@ -7611,18 +7622,18 @@
         <v>155</v>
       </c>
       <c r="M58" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B59" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C59" t="s" s="5">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="5">
@@ -7643,18 +7654,18 @@
         <v>156</v>
       </c>
       <c r="M59" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B60" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C60" t="s" s="5">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="5">
@@ -7675,18 +7686,18 @@
         <v>157</v>
       </c>
       <c r="M60" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B61" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C61" t="s" s="5">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5">
@@ -7707,18 +7718,18 @@
         <v>158</v>
       </c>
       <c r="M61" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B62" t="s" s="5">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C62" t="s" s="5">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="5">
@@ -7739,7 +7750,7 @@
         <v>159</v>
       </c>
       <c r="M62" t="s" s="5">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -7756,7 +7767,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -7767,7 +7778,8 @@
     <col min="3" max="3" width="5.90625" style="9" customWidth="1"/>
     <col min="4" max="4" width="9.19531" style="9" customWidth="1"/>
     <col min="5" max="5" width="9.375" style="9" customWidth="1"/>
-    <col min="6" max="256" width="12.25" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="9" customWidth="1"/>
+    <col min="7" max="256" width="12.25" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -7775,16 +7787,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>413</v>
+        <v>415</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>416</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -7803,6 +7818,9 @@
       <c r="E2" t="s" s="5">
         <v>13</v>
       </c>
+      <c r="F2" t="s" s="5">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="3">
@@ -7818,7 +7836,10 @@
         <v>15</v>
       </c>
       <c r="E3" s="5">
-        <v>100</v>
+        <v>500</v>
+      </c>
+      <c r="F3" t="s" s="5">
+        <v>17</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -7835,7 +7856,10 @@
         <v>19</v>
       </c>
       <c r="E4" s="5">
-        <v>25</v>
+        <v>120</v>
+      </c>
+      <c r="F4" t="s" s="5">
+        <v>20</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -7852,7 +7876,10 @@
         <v>22</v>
       </c>
       <c r="E5" s="5">
-        <v>25</v>
+        <v>120</v>
+      </c>
+      <c r="F5" t="s" s="5">
+        <v>23</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -7869,7 +7896,10 @@
         <v>25</v>
       </c>
       <c r="E6" s="5">
-        <v>10</v>
+        <v>50</v>
+      </c>
+      <c r="F6" t="s" s="5">
+        <v>26</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -7883,10 +7913,13 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="5">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E7" s="5">
-        <v>50</v>
+        <v>500</v>
+      </c>
+      <c r="F7" t="s" s="5">
+        <v>263</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -7900,10 +7933,13 @@
         <v>20</v>
       </c>
       <c r="D8" t="s" s="5">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E8" s="5">
-        <v>30</v>
+        <v>300</v>
+      </c>
+      <c r="F8" t="s" s="5">
+        <v>266</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -7917,10 +7953,13 @@
         <v>30</v>
       </c>
       <c r="D9" t="s" s="5">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E9" s="5">
-        <v>20</v>
+        <v>200</v>
+      </c>
+      <c r="F9" t="s" s="5">
+        <v>269</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -7934,10 +7973,13 @@
         <v>40</v>
       </c>
       <c r="D10" t="s" s="5">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E10" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F10" t="s" s="5">
+        <v>272</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -7951,10 +7993,13 @@
         <v>50</v>
       </c>
       <c r="D11" t="s" s="5">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E11" s="5">
-        <v>5</v>
+        <v>50</v>
+      </c>
+      <c r="F11" t="s" s="5">
+        <v>275</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -7968,10 +8013,13 @@
         <v>50</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E12" s="5">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="F12" t="s" s="5">
+        <v>278</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -7985,10 +8033,13 @@
         <v>50</v>
       </c>
       <c r="D13" t="s" s="5">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E13" s="5">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="F13" t="s" s="5">
+        <v>281</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
@@ -7999,13 +8050,16 @@
         <v>1</v>
       </c>
       <c r="C14" s="5">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>310</v>
+        <v>283</v>
       </c>
       <c r="E14" s="5">
         <v>50</v>
+      </c>
+      <c r="F14" t="s" s="5">
+        <v>284</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
@@ -8016,13 +8070,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s" s="5">
+        <v>312</v>
+      </c>
+      <c r="E15" s="5">
+        <v>500</v>
+      </c>
+      <c r="F15" t="s" s="5">
         <v>314</v>
-      </c>
-      <c r="E15" s="5">
-        <v>30</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -8033,13 +8090,16 @@
         <v>1</v>
       </c>
       <c r="C16" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s" s="5">
+        <v>316</v>
+      </c>
+      <c r="E16" s="5">
+        <v>300</v>
+      </c>
+      <c r="F16" t="s" s="5">
         <v>317</v>
-      </c>
-      <c r="E16" s="5">
-        <v>20</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
@@ -8047,16 +8107,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="5">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s" s="5">
+        <v>319</v>
+      </c>
+      <c r="E17" s="5">
+        <v>200</v>
+      </c>
+      <c r="F17" t="s" s="5">
         <v>320</v>
-      </c>
-      <c r="E17" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
@@ -8064,16 +8127,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C18" s="5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s" s="5">
+        <v>322</v>
+      </c>
+      <c r="E18" s="5">
+        <v>100</v>
+      </c>
+      <c r="F18" t="s" s="5">
         <v>323</v>
-      </c>
-      <c r="E18" s="5">
-        <v>5</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -8081,16 +8147,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="5">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C19" s="5">
         <v>50</v>
       </c>
       <c r="D19" t="s" s="5">
+        <v>325</v>
+      </c>
+      <c r="E19" s="5">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s" s="5">
         <v>326</v>
-      </c>
-      <c r="E19" s="5">
-        <v>2</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
@@ -8098,16 +8167,19 @@
         <v>18</v>
       </c>
       <c r="B20" s="5">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C20" s="5">
         <v>50</v>
       </c>
       <c r="D20" t="s" s="5">
+        <v>328</v>
+      </c>
+      <c r="E20" s="5">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s" s="5">
         <v>329</v>
-      </c>
-      <c r="E20" s="5">
-        <v>1</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
@@ -8115,16 +8187,19 @@
         <v>19</v>
       </c>
       <c r="B21" s="5">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C21" s="5">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s" s="5">
-        <v>42</v>
+        <v>331</v>
       </c>
       <c r="E21" s="5">
-        <v>200</v>
+        <v>10</v>
+      </c>
+      <c r="F21" t="s" s="5">
+        <v>332</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
@@ -8132,16 +8207,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C22" s="5">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s" s="5">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="D22" t="s" s="10">
+        <v>334</v>
       </c>
       <c r="E22" s="5">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="F22" t="s" s="5">
+        <v>335</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
@@ -8152,13 +8230,16 @@
         <v>1</v>
       </c>
       <c r="C23" s="5">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s" s="5">
-        <v>49</v>
+        <v>3</v>
+      </c>
+      <c r="D23" t="s" s="11">
+        <v>42</v>
       </c>
       <c r="E23" s="5">
-        <v>50</v>
+        <v>1000</v>
+      </c>
+      <c r="F23" t="s" s="5">
+        <v>44</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
@@ -8166,16 +8247,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C24" s="5">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s" s="5">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E24" s="5">
-        <v>25</v>
+        <v>500</v>
+      </c>
+      <c r="F24" t="s" s="5">
+        <v>47</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
@@ -8183,16 +8267,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="5">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C25" s="5">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s" s="5">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E25" s="5">
-        <v>12</v>
+        <v>250</v>
+      </c>
+      <c r="F25" t="s" s="5">
+        <v>50</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
@@ -8200,16 +8287,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="5">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C26" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s" s="5">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E26" s="5">
-        <v>5</v>
+        <v>120</v>
+      </c>
+      <c r="F26" t="s" s="5">
+        <v>53</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
@@ -8217,16 +8307,19 @@
         <v>25</v>
       </c>
       <c r="B27" s="5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C27" s="5">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D27" t="s" s="5">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="E27" s="5">
-        <v>100</v>
+        <v>60</v>
+      </c>
+      <c r="F27" t="s" s="5">
+        <v>56</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
@@ -8234,16 +8327,19 @@
         <v>26</v>
       </c>
       <c r="B28" s="5">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C28" s="5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s" s="5">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="E28" s="5">
-        <v>50</v>
+        <v>30</v>
+      </c>
+      <c r="F28" t="s" s="5">
+        <v>59</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
@@ -8257,10 +8353,13 @@
         <v>5</v>
       </c>
       <c r="D29" t="s" s="5">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E29" s="5">
-        <v>50</v>
+        <v>500</v>
+      </c>
+      <c r="F29" t="s" s="5">
+        <v>92</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
@@ -8271,13 +8370,16 @@
         <v>1</v>
       </c>
       <c r="C30" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s" s="5">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E30" s="5">
-        <v>10</v>
+        <v>500</v>
+      </c>
+      <c r="F30" t="s" s="5">
+        <v>96</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
@@ -8288,13 +8390,16 @@
         <v>1</v>
       </c>
       <c r="C31" s="5">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s" s="5">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E31" s="5">
-        <v>10</v>
+        <v>500</v>
+      </c>
+      <c r="F31" t="s" s="5">
+        <v>99</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
@@ -8308,10 +8413,13 @@
         <v>50</v>
       </c>
       <c r="D32" t="s" s="5">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E32" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F32" t="s" s="5">
+        <v>102</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
@@ -8325,10 +8433,13 @@
         <v>50</v>
       </c>
       <c r="D33" t="s" s="5">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E33" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F33" t="s" s="5">
+        <v>105</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -8342,10 +8453,13 @@
         <v>50</v>
       </c>
       <c r="D34" t="s" s="5">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E34" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F34" t="s" s="5">
+        <v>109</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
@@ -8359,10 +8473,13 @@
         <v>50</v>
       </c>
       <c r="D35" t="s" s="5">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E35" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F35" t="s" s="5">
+        <v>113</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
@@ -8376,10 +8493,13 @@
         <v>50</v>
       </c>
       <c r="D36" t="s" s="5">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E36" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F36" t="s" s="5">
+        <v>117</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
@@ -8387,16 +8507,19 @@
         <v>35</v>
       </c>
       <c r="B37" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C37" s="5">
         <v>50</v>
       </c>
       <c r="D37" t="s" s="5">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E37" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F37" t="s" s="5">
+        <v>121</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
@@ -8410,10 +8533,13 @@
         <v>50</v>
       </c>
       <c r="D38" t="s" s="5">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E38" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F38" t="s" s="5">
+        <v>125</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
@@ -8421,16 +8547,19 @@
         <v>37</v>
       </c>
       <c r="B39" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C39" s="5">
         <v>50</v>
       </c>
       <c r="D39" t="s" s="5">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="E39" s="5">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="F39" t="s" s="5">
+        <v>129</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
@@ -8444,10 +8573,13 @@
         <v>50</v>
       </c>
       <c r="D40" t="s" s="5">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="E40" s="5">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="F40" t="s" s="5">
+        <v>133</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
@@ -8455,16 +8587,19 @@
         <v>39</v>
       </c>
       <c r="B41" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C41" s="5">
         <v>50</v>
       </c>
       <c r="D41" t="s" s="5">
-        <v>190</v>
+        <v>145</v>
       </c>
       <c r="E41" s="5">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="F41" t="s" s="5">
+        <v>147</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -8472,16 +8607,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C42" s="5">
         <v>50</v>
       </c>
       <c r="D42" t="s" s="5">
-        <v>194</v>
+        <v>150</v>
       </c>
       <c r="E42" s="5">
         <v>10</v>
+      </c>
+      <c r="F42" t="s" s="5">
+        <v>151</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
@@ -8495,10 +8633,13 @@
         <v>50</v>
       </c>
       <c r="D43" t="s" s="5">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="E43" s="5">
-        <v>10</v>
+        <v>50</v>
+      </c>
+      <c r="F43" t="s" s="5">
+        <v>164</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
@@ -8512,10 +8653,13 @@
         <v>50</v>
       </c>
       <c r="D44" t="s" s="5">
-        <v>200</v>
+        <v>167</v>
       </c>
       <c r="E44" s="5">
-        <v>10</v>
+        <v>50</v>
+      </c>
+      <c r="F44" t="s" s="5">
+        <v>168</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
@@ -8529,10 +8673,13 @@
         <v>50</v>
       </c>
       <c r="D45" t="s" s="5">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="E45" s="5">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="F45" t="s" s="5">
+        <v>192</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
@@ -8545,11 +8692,14 @@
       <c r="C46" s="5">
         <v>50</v>
       </c>
-      <c r="D46" t="s" s="10">
-        <v>206</v>
+      <c r="D46" t="s" s="5">
+        <v>194</v>
       </c>
       <c r="E46" s="5">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="F46" t="s" s="5">
+        <v>195</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
@@ -8557,16 +8707,19 @@
         <v>45</v>
       </c>
       <c r="B47" s="5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C47" s="5">
         <v>50</v>
       </c>
-      <c r="D47" t="s" s="11">
-        <v>209</v>
+      <c r="D47" t="s" s="5">
+        <v>197</v>
       </c>
       <c r="E47" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F47" t="s" s="5">
+        <v>198</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
@@ -8580,10 +8733,13 @@
         <v>50</v>
       </c>
       <c r="D48" t="s" s="5">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="E48" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F48" t="s" s="5">
+        <v>201</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
@@ -8597,10 +8753,13 @@
         <v>50</v>
       </c>
       <c r="D49" t="s" s="5">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E49" s="5">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="F49" t="s" s="5">
+        <v>204</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
@@ -8611,13 +8770,16 @@
         <v>1</v>
       </c>
       <c r="C50" s="5">
-        <v>10</v>
-      </c>
-      <c r="D50" t="s" s="5">
-        <v>361</v>
+        <v>50</v>
+      </c>
+      <c r="D50" t="s" s="10">
+        <v>206</v>
       </c>
       <c r="E50" s="5">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="F50" t="s" s="5">
+        <v>207</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
@@ -8625,16 +8787,19 @@
         <v>49</v>
       </c>
       <c r="B51" s="5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C51" s="5">
-        <v>10</v>
-      </c>
-      <c r="D51" t="s" s="5">
-        <v>365</v>
+        <v>50</v>
+      </c>
+      <c r="D51" t="s" s="11">
+        <v>209</v>
       </c>
       <c r="E51" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F51" t="s" s="5">
+        <v>210</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
@@ -8645,13 +8810,16 @@
         <v>1</v>
       </c>
       <c r="C52" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D52" t="s" s="5">
-        <v>368</v>
+        <v>212</v>
       </c>
       <c r="E52" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F52" t="s" s="5">
+        <v>213</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
@@ -8659,16 +8827,19 @@
         <v>51</v>
       </c>
       <c r="B53" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C53" s="5">
         <v>50</v>
       </c>
       <c r="D53" t="s" s="5">
-        <v>371</v>
+        <v>215</v>
       </c>
       <c r="E53" s="5">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="F53" t="s" s="5">
+        <v>216</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
@@ -8682,10 +8853,113 @@
         <v>50</v>
       </c>
       <c r="D54" t="s" s="5">
+        <v>219</v>
+      </c>
+      <c r="E54" s="5">
+        <v>50</v>
+      </c>
+      <c r="F54" t="s" s="5">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="55" ht="20" customHeight="1">
+      <c r="A55" s="3">
+        <v>53</v>
+      </c>
+      <c r="B55" s="5">
+        <v>1</v>
+      </c>
+      <c r="C55" s="5">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s" s="5">
+        <v>363</v>
+      </c>
+      <c r="E55" s="5">
+        <v>100</v>
+      </c>
+      <c r="F55" t="s" s="5">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="56" ht="20" customHeight="1">
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56" s="5">
+        <v>1</v>
+      </c>
+      <c r="C56" s="5">
+        <v>10</v>
+      </c>
+      <c r="D56" t="s" s="5">
+        <v>367</v>
+      </c>
+      <c r="E56" s="5">
+        <v>100</v>
+      </c>
+      <c r="F56" t="s" s="5">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="57" ht="20" customHeight="1">
+      <c r="A57" s="3">
+        <v>55</v>
+      </c>
+      <c r="B57" s="5">
+        <v>1</v>
+      </c>
+      <c r="C57" s="5">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s" s="5">
+        <v>370</v>
+      </c>
+      <c r="E57" s="5">
+        <v>100</v>
+      </c>
+      <c r="F57" t="s" s="5">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="58" ht="20" customHeight="1">
+      <c r="A58" s="3">
+        <v>56</v>
+      </c>
+      <c r="B58" s="5">
+        <v>20</v>
+      </c>
+      <c r="C58" s="5">
+        <v>50</v>
+      </c>
+      <c r="D58" t="s" s="5">
+        <v>373</v>
+      </c>
+      <c r="E58" s="5">
+        <v>100</v>
+      </c>
+      <c r="F58" t="s" s="5">
         <v>374</v>
       </c>
-      <c r="E54" s="5">
-        <v>10</v>
+    </row>
+    <row r="59" ht="20" customHeight="1">
+      <c r="A59" s="3">
+        <v>57</v>
+      </c>
+      <c r="B59" s="5">
+        <v>20</v>
+      </c>
+      <c r="C59" s="5">
+        <v>50</v>
+      </c>
+      <c r="D59" t="s" s="5">
+        <v>376</v>
+      </c>
+      <c r="E59" s="5">
+        <v>100</v>
+      </c>
+      <c r="F59" t="s" s="5">
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #546 FlixelRL-546 Floor11〜15の敵の設定
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -730,37 +730,37 @@
     <t>Orb</t>
   </si>
   <si>
-    <t>赤のオーブ</t>
-  </si>
-  <si>
-    <t>ぶつけた敵を即死させます</t>
+    <t>赤ネコのオーブ</t>
+  </si>
+  <si>
+    <t>ぶつけた敵を即死させます。使うとネコはいなくなります</t>
   </si>
   <si>
     <t>ORB2</t>
   </si>
   <si>
-    <t>青のオーブ</t>
-  </si>
-  <si>
-    <t>すべての敵の特殊攻撃を無効化します</t>
+    <t>青ネコのオーブ</t>
+  </si>
+  <si>
+    <t>すべての敵の特殊攻撃を無効化します。使うとネコはいなくなります</t>
   </si>
   <si>
     <t>ORB3</t>
   </si>
   <si>
-    <t>白のオーブ</t>
-  </si>
-  <si>
-    <t>死亡しても一度だけ復活できます</t>
+    <t>白ネコのオーブ</t>
+  </si>
+  <si>
+    <t>死亡しても一度だけ復活できます。使うとネコはいなくなります</t>
   </si>
   <si>
     <t>ORB4</t>
   </si>
   <si>
-    <t>緑のオーブ</t>
-  </si>
-  <si>
-    <t>無敵状態になります</t>
+    <t>緑ネコのオーブ</t>
+  </si>
+  <si>
+    <t>無敵状態になります。使うとネコはいなくなります</t>
   </si>
   <si>
     <t>ORB5</t>

</xml_diff>

<commit_message>
fixed #346 FlixelRL-346 青オーブを実装する
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -733,7 +733,7 @@
     <t>赤ネコのオーブ</t>
   </si>
   <si>
-    <t>ぶつけた敵を即死させます。使うとネコはいなくなります</t>
+    <t>ぶつけた敵を即死させます。使うと赤ネコはいなくなります</t>
   </si>
   <si>
     <t>ORB2</t>
@@ -742,7 +742,7 @@
     <t>青ネコのオーブ</t>
   </si>
   <si>
-    <t>すべての敵の特殊攻撃を無効化します。使うとネコはいなくなります</t>
+    <t>次のフロアにワープします。使うと青ネコはいなくなります</t>
   </si>
   <si>
     <t>ORB3</t>
@@ -751,7 +751,7 @@
     <t>白ネコのオーブ</t>
   </si>
   <si>
-    <t>死亡しても一度だけ復活できます。使うとネコはいなくなります</t>
+    <t>死亡しても一度だけ復活できます。使うと白ネコはいなくなります</t>
   </si>
   <si>
     <t>ORB4</t>
@@ -760,7 +760,7 @@
     <t>緑ネコのオーブ</t>
   </si>
   <si>
-    <t>無敵状態になります。使うとネコはいなくなります</t>
+    <t>無敵状態になります。使うと緑ネコはいなくなります</t>
   </si>
   <si>
     <t>ORB5</t>

</xml_diff>

<commit_message>
fixed #550 FlixelRL-550 麻痺の巻物
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="424">
   <si>
     <t>id</t>
   </si>
@@ -532,40 +532,61 @@
     <t>SCROLL8</t>
   </si>
   <si>
-    <t>巻物8</t>
+    <t>麻痺の巻物</t>
+  </si>
+  <si>
+    <t>すべての敵を麻痺させます</t>
+  </si>
+  <si>
+    <t>SCROLL9</t>
+  </si>
+  <si>
+    <t>眠りの巻物</t>
+  </si>
+  <si>
+    <t>すべての敵を眠らせます</t>
+  </si>
+  <si>
+    <t>SCROLL10</t>
+  </si>
+  <si>
+    <t>混乱の巻物</t>
+  </si>
+  <si>
+    <t>すべての敵を混乱させます</t>
+  </si>
+  <si>
+    <t>SCROLL11</t>
+  </si>
+  <si>
+    <t>武器合成の巻物</t>
+  </si>
+  <si>
+    <t>weponadd</t>
+  </si>
+  <si>
+    <t>所持している武器を装備中の武器に合成します</t>
+  </si>
+  <si>
+    <t>SCROLL12</t>
+  </si>
+  <si>
+    <t>防具合成の巻物</t>
+  </si>
+  <si>
+    <t>armoradd</t>
+  </si>
+  <si>
+    <t>所持している防具を装備中の防具に合成します</t>
+  </si>
+  <si>
+    <t>SCROLL13</t>
+  </si>
+  <si>
+    <t>巻物13</t>
   </si>
   <si>
     <t>巻物の説明文</t>
-  </si>
-  <si>
-    <t>SCROLL9</t>
-  </si>
-  <si>
-    <t>巻物9</t>
-  </si>
-  <si>
-    <t>SCROLL10</t>
-  </si>
-  <si>
-    <t>巻物10</t>
-  </si>
-  <si>
-    <t>SCROLL11</t>
-  </si>
-  <si>
-    <t>巻物11</t>
-  </si>
-  <si>
-    <t>SCROLL12</t>
-  </si>
-  <si>
-    <t>巻物12</t>
-  </si>
-  <si>
-    <t>SCROLL13</t>
-  </si>
-  <si>
-    <t>巻物13</t>
   </si>
   <si>
     <t>SCROLL14</t>
@@ -1331,7 +1352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1380,13 +1401,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1421,6 +1453,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2688,7 +2723,7 @@
     <col min="5" max="5" width="4.75" style="1" customWidth="1"/>
     <col min="6" max="6" width="4.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="4.75" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.125" style="1" customWidth="1"/>
     <col min="9" max="9" width="4.75" style="1" customWidth="1"/>
     <col min="10" max="10" width="4" style="1" customWidth="1"/>
     <col min="11" max="11" width="4" style="1" customWidth="1"/>
@@ -4542,11 +4577,11 @@
         <v>1</v>
       </c>
       <c r="J54" s="6">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="K54" s="6">
         <f>J54*0.35</f>
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="L54" s="6">
         <v>235</v>
@@ -4576,11 +4611,11 @@
         <v>2</v>
       </c>
       <c r="J55" s="6">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="K55" s="6">
         <f>J55*0.35</f>
-        <v>525</v>
+        <v>1050</v>
       </c>
       <c r="L55" s="6">
         <v>236</v>
@@ -4669,16 +4704,20 @@
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
+      <c r="F58" s="6">
+        <v>1</v>
+      </c>
       <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
+      <c r="H58" t="s" s="5">
+        <v>110</v>
+      </c>
       <c r="I58" s="7"/>
       <c r="J58" s="6">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="K58" s="6">
         <f>J58*0.35</f>
-        <v>1.05</v>
+        <v>350</v>
       </c>
       <c r="L58" s="6">
         <v>239</v>
@@ -4699,123 +4738,135 @@
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
+      <c r="F59" s="6">
+        <v>1</v>
+      </c>
       <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
+      <c r="H59" t="s" s="5">
+        <v>106</v>
+      </c>
       <c r="I59" s="7"/>
       <c r="J59" s="6">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="K59" s="6">
         <f>J59*0.35</f>
-        <v>1.05</v>
+        <v>350</v>
       </c>
       <c r="L59" s="6">
         <v>240</v>
       </c>
       <c r="M59" t="s" s="5">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B60" t="s" s="5">
         <v>146</v>
       </c>
       <c r="C60" t="s" s="5">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
+      <c r="F60" s="6">
+        <v>1</v>
+      </c>
       <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
+      <c r="H60" t="s" s="5">
+        <v>114</v>
+      </c>
       <c r="I60" s="7"/>
       <c r="J60" s="6">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="K60" s="6">
         <f>J60*0.35</f>
-        <v>1.05</v>
+        <v>350</v>
       </c>
       <c r="L60" s="6">
         <v>241</v>
       </c>
       <c r="M60" t="s" s="5">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B61" t="s" s="5">
         <v>146</v>
       </c>
       <c r="C61" t="s" s="5">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
+      <c r="H61" t="s" s="5">
+        <v>182</v>
+      </c>
       <c r="I61" s="7"/>
       <c r="J61" s="6">
-        <v>3</v>
+        <v>1500</v>
       </c>
       <c r="K61" s="6">
         <f>J61*0.35</f>
-        <v>1.05</v>
+        <v>525</v>
       </c>
       <c r="L61" s="6">
         <v>242</v>
       </c>
       <c r="M61" t="s" s="5">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B62" t="s" s="5">
         <v>146</v>
       </c>
       <c r="C62" t="s" s="5">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
-      <c r="H62" s="6"/>
+      <c r="H62" t="s" s="5">
+        <v>186</v>
+      </c>
       <c r="I62" s="7"/>
       <c r="J62" s="6">
-        <v>3</v>
+        <v>1500</v>
       </c>
       <c r="K62" s="6">
         <f>J62*0.35</f>
-        <v>1.05</v>
+        <v>525</v>
       </c>
       <c r="L62" s="6">
         <v>243</v>
       </c>
       <c r="M62" t="s" s="5">
-        <v>173</v>
+        <v>187</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" t="s" s="3">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B63" t="s" s="5">
         <v>146</v>
       </c>
       <c r="C63" t="s" s="5">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="6"/>
@@ -4834,18 +4885,18 @@
         <v>244</v>
       </c>
       <c r="M63" t="s" s="5">
-        <v>173</v>
+        <v>190</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
       <c r="A64" t="s" s="3">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="B64" t="s" s="5">
         <v>146</v>
       </c>
       <c r="C64" t="s" s="5">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="6"/>
@@ -4864,18 +4915,18 @@
         <v>245</v>
       </c>
       <c r="M64" t="s" s="5">
-        <v>173</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" t="s" s="3">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B65" t="s" s="5">
         <v>146</v>
       </c>
       <c r="C65" t="s" s="5">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="6"/>
@@ -4894,18 +4945,18 @@
         <v>246</v>
       </c>
       <c r="M65" t="s" s="5">
-        <v>173</v>
+        <v>190</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" t="s" s="3">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B66" t="s" s="5">
         <v>146</v>
       </c>
       <c r="C66" t="s" s="5">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="6"/>
@@ -4924,18 +4975,18 @@
         <v>247</v>
       </c>
       <c r="M66" t="s" s="5">
-        <v>173</v>
+        <v>190</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
       <c r="A67" t="s" s="3">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B67" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C67" t="s" s="5">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="6"/>
@@ -4956,18 +5007,18 @@
         <v>248</v>
       </c>
       <c r="M67" t="s" s="5">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" ht="20" customHeight="1">
       <c r="A68" t="s" s="3">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B68" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C68" t="s" s="5">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="6"/>
@@ -4988,18 +5039,18 @@
         <v>249</v>
       </c>
       <c r="M68" t="s" s="5">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
       <c r="A69" t="s" s="3">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B69" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C69" t="s" s="5">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="6"/>
@@ -5020,18 +5071,18 @@
         <v>250</v>
       </c>
       <c r="M69" t="s" s="5">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
       <c r="A70" t="s" s="3">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B70" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C70" t="s" s="5">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="6"/>
@@ -5052,18 +5103,18 @@
         <v>251</v>
       </c>
       <c r="M70" t="s" s="5">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
       <c r="A71" t="s" s="3">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="B71" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C71" t="s" s="5">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="6"/>
@@ -5084,18 +5135,18 @@
         <v>252</v>
       </c>
       <c r="M71" t="s" s="5">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" ht="20" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="B72" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C72" t="s" s="5">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="6"/>
@@ -5116,18 +5167,18 @@
         <v>253</v>
       </c>
       <c r="M72" t="s" s="5">
-        <v>208</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" t="s" s="3">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="B73" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C73" t="s" s="5">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="6"/>
@@ -5148,18 +5199,18 @@
         <v>254</v>
       </c>
       <c r="M73" t="s" s="5">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" ht="20" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="B74" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C74" t="s" s="5">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="6"/>
@@ -5180,25 +5231,25 @@
         <v>255</v>
       </c>
       <c r="M74" t="s" s="5">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="75" ht="20" customHeight="1">
       <c r="A75" t="s" s="3">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="B75" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C75" t="s" s="5">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
       <c r="H75" t="s" s="5">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="I75" s="7"/>
       <c r="J75" s="6">
@@ -5212,25 +5263,25 @@
         <v>256</v>
       </c>
       <c r="M75" t="s" s="5">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
       <c r="A76" t="s" s="3">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B76" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C76" t="s" s="5">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
       <c r="H76" t="s" s="5">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="I76" s="7"/>
       <c r="J76" s="6">
@@ -5244,18 +5295,18 @@
         <v>257</v>
       </c>
       <c r="M76" t="s" s="5">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" t="s" s="3">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="B77" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C77" t="s" s="5">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="6"/>
@@ -5274,18 +5325,18 @@
         <v>258</v>
       </c>
       <c r="M77" t="s" s="5">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="B78" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C78" t="s" s="5">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="6"/>
@@ -5304,18 +5355,18 @@
         <v>259</v>
       </c>
       <c r="M78" t="s" s="5">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" t="s" s="3">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="B79" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C79" t="s" s="5">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="6"/>
@@ -5334,18 +5385,18 @@
         <v>260</v>
       </c>
       <c r="M79" t="s" s="5">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
       <c r="A80" t="s" s="3">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="B80" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C80" t="s" s="5">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="6"/>
@@ -5364,18 +5415,18 @@
         <v>261</v>
       </c>
       <c r="M80" t="s" s="5">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" t="s" s="3">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="B81" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C81" t="s" s="5">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="6"/>
@@ -5394,18 +5445,18 @@
         <v>262</v>
       </c>
       <c r="M81" t="s" s="5">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
       <c r="A82" t="s" s="3">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="B82" t="s" s="5">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C82" t="s" s="5">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="6"/>
@@ -5424,18 +5475,18 @@
         <v>263</v>
       </c>
       <c r="M82" t="s" s="5">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
       <c r="A83" t="s" s="3">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="B83" t="s" s="5">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C83" t="s" s="5">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="6"/>
@@ -5454,18 +5505,18 @@
         <v>264</v>
       </c>
       <c r="M83" t="s" s="5">
-        <v>239</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" ht="20" customHeight="1">
       <c r="A84" t="s" s="3">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="B84" t="s" s="5">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C84" t="s" s="5">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="6"/>
@@ -5484,18 +5535,18 @@
         <v>265</v>
       </c>
       <c r="M84" t="s" s="5">
-        <v>242</v>
+        <v>249</v>
       </c>
     </row>
     <row r="85" ht="20" customHeight="1">
       <c r="A85" t="s" s="3">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="B85" t="s" s="5">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C85" t="s" s="5">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="6"/>
@@ -5514,18 +5565,18 @@
         <v>266</v>
       </c>
       <c r="M85" t="s" s="5">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86" ht="20" customHeight="1">
       <c r="A86" t="s" s="3">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="B86" t="s" s="5">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C86" t="s" s="5">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="6"/>
@@ -5544,18 +5595,18 @@
         <v>267</v>
       </c>
       <c r="M86" t="s" s="5">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="87" ht="20" customHeight="1">
       <c r="A87" t="s" s="3">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="B87" t="s" s="5">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C87" t="s" s="5">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="6"/>
@@ -5574,18 +5625,18 @@
         <v>268</v>
       </c>
       <c r="M87" t="s" s="5">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" ht="20" customHeight="1">
       <c r="A88" t="s" s="3">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B88" t="s" s="5">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C88" t="s" s="5">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="6"/>
@@ -5604,18 +5655,18 @@
         <v>269</v>
       </c>
       <c r="M88" t="s" s="5">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89" ht="20" customHeight="1">
       <c r="A89" t="s" s="3">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="B89" t="s" s="5">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C89" t="s" s="5">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="6"/>
@@ -5634,18 +5685,18 @@
         <v>270</v>
       </c>
       <c r="M89" t="s" s="5">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="90" ht="20" customHeight="1">
       <c r="A90" t="s" s="3">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="B90" t="s" s="5">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C90" t="s" s="5">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="D90" s="7"/>
       <c r="E90" s="6"/>
@@ -5664,7 +5715,7 @@
         <v>271</v>
       </c>
       <c r="M90" t="s" s="5">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -5717,16 +5768,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="G1" t="s" s="2">
         <v>7</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>4</v>
@@ -5787,13 +5838,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="D3" s="5">
         <v>2</v>
@@ -5814,18 +5865,18 @@
         <v>100</v>
       </c>
       <c r="M3" t="s" s="5">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="D4" s="5">
         <v>4</v>
@@ -5846,18 +5897,18 @@
         <v>101</v>
       </c>
       <c r="M4" t="s" s="5">
-        <v>267</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="D5" s="5">
         <v>6</v>
@@ -5878,18 +5929,18 @@
         <v>102</v>
       </c>
       <c r="M5" t="s" s="5">
-        <v>270</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="D6" s="5">
         <v>10</v>
@@ -5910,18 +5961,18 @@
         <v>103</v>
       </c>
       <c r="M6" t="s" s="5">
-        <v>273</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="B7" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C7" t="s" s="5">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="D7" s="5">
         <v>14</v>
@@ -5942,18 +5993,18 @@
         <v>104</v>
       </c>
       <c r="M7" t="s" s="5">
-        <v>276</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C8" t="s" s="5">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="D8" s="5">
         <v>16</v>
@@ -5974,18 +6025,18 @@
         <v>105</v>
       </c>
       <c r="M8" t="s" s="5">
-        <v>279</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="B9" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D9" s="5">
         <v>20</v>
@@ -6006,18 +6057,18 @@
         <v>106</v>
       </c>
       <c r="M9" t="s" s="5">
-        <v>282</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="B10" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C10" t="s" s="5">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="D10" s="5">
         <v>10</v>
@@ -6025,7 +6076,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" t="s" s="5">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="H10" s="6">
         <v>50</v>
@@ -6042,18 +6093,18 @@
         <v>107</v>
       </c>
       <c r="M10" t="s" s="5">
-        <v>286</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="B11" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C11" t="s" s="5">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
@@ -6074,18 +6125,18 @@
         <v>108</v>
       </c>
       <c r="M11" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="B12" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C12" t="s" s="5">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
@@ -6106,18 +6157,18 @@
         <v>109</v>
       </c>
       <c r="M12" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B13" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C13" t="s" s="5">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
@@ -6138,18 +6189,18 @@
         <v>110</v>
       </c>
       <c r="M13" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="B14" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C14" t="s" s="5">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
@@ -6170,18 +6221,18 @@
         <v>111</v>
       </c>
       <c r="M14" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="B15" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C15" t="s" s="5">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
@@ -6202,18 +6253,18 @@
         <v>112</v>
       </c>
       <c r="M15" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="B16" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C16" t="s" s="5">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="D16" s="5">
         <v>1</v>
@@ -6234,18 +6285,18 @@
         <v>113</v>
       </c>
       <c r="M16" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="B17" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C17" t="s" s="5">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="D17" s="5">
         <v>1</v>
@@ -6266,18 +6317,18 @@
         <v>114</v>
       </c>
       <c r="M17" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="B18" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C18" t="s" s="5">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -6298,18 +6349,18 @@
         <v>115</v>
       </c>
       <c r="M18" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="B19" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C19" t="s" s="5">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D19" s="5">
         <v>1</v>
@@ -6330,18 +6381,18 @@
         <v>116</v>
       </c>
       <c r="M19" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="B20" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C20" t="s" s="5">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="D20" s="5">
         <v>1</v>
@@ -6362,18 +6413,18 @@
         <v>117</v>
       </c>
       <c r="M20" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="B21" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C21" t="s" s="5">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="D21" s="5">
         <v>1</v>
@@ -6394,18 +6445,18 @@
         <v>118</v>
       </c>
       <c r="M21" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="B22" t="s" s="5">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C22" t="s" s="5">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
@@ -6426,18 +6477,18 @@
         <v>119</v>
       </c>
       <c r="M22" t="s" s="5">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="B23" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C23" t="s" s="5">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="5">
@@ -6460,18 +6511,18 @@
         <v>120</v>
       </c>
       <c r="M23" t="s" s="5">
-        <v>315</v>
+        <v>322</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="B24" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C24" t="s" s="5">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="5">
@@ -6494,18 +6545,18 @@
         <v>121</v>
       </c>
       <c r="M24" t="s" s="5">
-        <v>318</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="B25" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C25" t="s" s="5">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="5">
@@ -6528,18 +6579,18 @@
         <v>122</v>
       </c>
       <c r="M25" t="s" s="5">
-        <v>321</v>
+        <v>328</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="B26" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C26" t="s" s="5">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="5">
@@ -6562,18 +6613,18 @@
         <v>123</v>
       </c>
       <c r="M26" t="s" s="5">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B27" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C27" t="s" s="5">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="5">
@@ -6596,18 +6647,18 @@
         <v>124</v>
       </c>
       <c r="M27" t="s" s="5">
-        <v>327</v>
+        <v>334</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="B28" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C28" t="s" s="5">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="5">
@@ -6630,18 +6681,18 @@
         <v>125</v>
       </c>
       <c r="M28" t="s" s="5">
-        <v>330</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="B29" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C29" t="s" s="5">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="5">
@@ -6664,18 +6715,18 @@
         <v>126</v>
       </c>
       <c r="M29" t="s" s="5">
-        <v>333</v>
+        <v>340</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="B30" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C30" t="s" s="5">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="5">
@@ -6683,7 +6734,7 @@
       </c>
       <c r="F30" s="6"/>
       <c r="G30" t="s" s="5">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="5">
@@ -6700,18 +6751,18 @@
         <v>127</v>
       </c>
       <c r="M30" t="s" s="5">
-        <v>337</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="B31" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C31" t="s" s="5">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="5">
@@ -6734,18 +6785,18 @@
         <v>128</v>
       </c>
       <c r="M31" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="B32" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C32" t="s" s="5">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="5">
@@ -6768,18 +6819,18 @@
         <v>129</v>
       </c>
       <c r="M32" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="B33" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C33" t="s" s="5">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="5">
@@ -6802,18 +6853,18 @@
         <v>130</v>
       </c>
       <c r="M33" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="B34" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C34" t="s" s="5">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="5">
@@ -6836,18 +6887,18 @@
         <v>131</v>
       </c>
       <c r="M34" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="B35" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C35" t="s" s="5">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="5">
@@ -6870,18 +6921,18 @@
         <v>132</v>
       </c>
       <c r="M35" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="B36" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C36" t="s" s="5">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="5">
@@ -6904,18 +6955,18 @@
         <v>133</v>
       </c>
       <c r="M36" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="B37" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C37" t="s" s="5">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="5">
@@ -6938,18 +6989,18 @@
         <v>134</v>
       </c>
       <c r="M37" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="B38" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C38" t="s" s="5">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="5">
@@ -6972,18 +7023,18 @@
         <v>135</v>
       </c>
       <c r="M38" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="B39" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C39" t="s" s="5">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="5">
@@ -7006,18 +7057,18 @@
         <v>136</v>
       </c>
       <c r="M39" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="B40" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C40" t="s" s="5">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="5">
@@ -7040,18 +7091,18 @@
         <v>137</v>
       </c>
       <c r="M40" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="B41" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C41" t="s" s="5">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="5">
@@ -7074,18 +7125,18 @@
         <v>138</v>
       </c>
       <c r="M41" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="B42" t="s" s="5">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C42" t="s" s="5">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="5">
@@ -7108,18 +7159,18 @@
         <v>139</v>
       </c>
       <c r="M42" t="s" s="5">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="B43" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C43" t="s" s="5">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="D43" s="6">
         <v>1</v>
@@ -7140,18 +7191,18 @@
         <v>140</v>
       </c>
       <c r="M43" t="s" s="5">
-        <v>366</v>
+        <v>373</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="B44" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C44" t="s" s="5">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="5">
@@ -7172,18 +7223,18 @@
         <v>141</v>
       </c>
       <c r="M44" t="s" s="5">
-        <v>369</v>
+        <v>376</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="B45" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C45" t="s" s="5">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="7"/>
@@ -7206,18 +7257,18 @@
         <v>142</v>
       </c>
       <c r="M45" t="s" s="5">
-        <v>372</v>
+        <v>379</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="B46" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C46" t="s" s="5">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="7"/>
@@ -7238,18 +7289,18 @@
         <v>143</v>
       </c>
       <c r="M46" t="s" s="5">
-        <v>375</v>
+        <v>382</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" t="s" s="3">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="B47" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C47" t="s" s="5">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="7"/>
@@ -7270,24 +7321,24 @@
         <v>144</v>
       </c>
       <c r="M47" t="s" s="5">
-        <v>378</v>
+        <v>385</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="B48" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C48" t="s" s="5">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="7"/>
       <c r="F48" s="6"/>
       <c r="G48" t="s" s="5">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="7"/>
@@ -7302,18 +7353,18 @@
         <v>145</v>
       </c>
       <c r="M48" t="s" s="5">
-        <v>382</v>
+        <v>389</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="B49" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C49" t="s" s="5">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="5">
@@ -7334,18 +7385,18 @@
         <v>146</v>
       </c>
       <c r="M49" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="B50" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C50" t="s" s="5">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="5">
@@ -7366,18 +7417,18 @@
         <v>147</v>
       </c>
       <c r="M50" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="B51" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C51" t="s" s="5">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="5">
@@ -7398,18 +7449,18 @@
         <v>148</v>
       </c>
       <c r="M51" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="B52" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C52" t="s" s="5">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="5">
@@ -7430,18 +7481,18 @@
         <v>149</v>
       </c>
       <c r="M52" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="B53" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C53" t="s" s="5">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5">
@@ -7462,18 +7513,18 @@
         <v>150</v>
       </c>
       <c r="M53" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="B54" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C54" t="s" s="5">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5">
@@ -7494,18 +7545,18 @@
         <v>151</v>
       </c>
       <c r="M54" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="B55" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C55" t="s" s="5">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="5">
@@ -7526,18 +7577,18 @@
         <v>152</v>
       </c>
       <c r="M55" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="B56" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C56" t="s" s="5">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="5">
@@ -7558,18 +7609,18 @@
         <v>153</v>
       </c>
       <c r="M56" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="B57" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C57" t="s" s="5">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="5">
@@ -7590,18 +7641,18 @@
         <v>154</v>
       </c>
       <c r="M57" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="B58" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C58" t="s" s="5">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="5">
@@ -7622,18 +7673,18 @@
         <v>155</v>
       </c>
       <c r="M58" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B59" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C59" t="s" s="5">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="5">
@@ -7654,18 +7705,18 @@
         <v>156</v>
       </c>
       <c r="M59" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="B60" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C60" t="s" s="5">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="5">
@@ -7686,18 +7737,18 @@
         <v>157</v>
       </c>
       <c r="M60" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="B61" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C61" t="s" s="5">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5">
@@ -7718,18 +7769,18 @@
         <v>158</v>
       </c>
       <c r="M61" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="B62" t="s" s="5">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C62" t="s" s="5">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="5">
@@ -7750,7 +7801,7 @@
         <v>159</v>
       </c>
       <c r="M62" t="s" s="5">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -7767,7 +7818,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -7787,19 +7838,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>416</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -7913,13 +7964,13 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="5">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="E7" s="5">
         <v>500</v>
       </c>
       <c r="F7" t="s" s="5">
-        <v>263</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -7933,13 +7984,13 @@
         <v>20</v>
       </c>
       <c r="D8" t="s" s="5">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="E8" s="5">
         <v>300</v>
       </c>
       <c r="F8" t="s" s="5">
-        <v>266</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -7953,13 +8004,13 @@
         <v>30</v>
       </c>
       <c r="D9" t="s" s="5">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="E9" s="5">
         <v>200</v>
       </c>
       <c r="F9" t="s" s="5">
-        <v>269</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -7973,13 +8024,13 @@
         <v>40</v>
       </c>
       <c r="D10" t="s" s="5">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="E10" s="5">
         <v>100</v>
       </c>
       <c r="F10" t="s" s="5">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -7993,13 +8044,13 @@
         <v>50</v>
       </c>
       <c r="D11" t="s" s="5">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="E11" s="5">
         <v>50</v>
       </c>
       <c r="F11" t="s" s="5">
-        <v>275</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -8013,13 +8064,13 @@
         <v>50</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="E12" s="5">
         <v>20</v>
       </c>
       <c r="F12" t="s" s="5">
-        <v>278</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -8033,13 +8084,13 @@
         <v>50</v>
       </c>
       <c r="D13" t="s" s="5">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="E13" s="5">
         <v>10</v>
       </c>
       <c r="F13" t="s" s="5">
-        <v>281</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
@@ -8053,13 +8104,13 @@
         <v>999</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="E14" s="5">
         <v>50</v>
       </c>
       <c r="F14" t="s" s="5">
-        <v>284</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
@@ -8073,13 +8124,13 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="5">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="E15" s="5">
         <v>500</v>
       </c>
       <c r="F15" t="s" s="5">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -8093,13 +8144,13 @@
         <v>20</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="E16" s="5">
         <v>300</v>
       </c>
       <c r="F16" t="s" s="5">
-        <v>317</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
@@ -8113,13 +8164,13 @@
         <v>30</v>
       </c>
       <c r="D17" t="s" s="5">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="E17" s="5">
         <v>200</v>
       </c>
       <c r="F17" t="s" s="5">
-        <v>320</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
@@ -8133,13 +8184,13 @@
         <v>40</v>
       </c>
       <c r="D18" t="s" s="5">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="E18" s="5">
         <v>100</v>
       </c>
       <c r="F18" t="s" s="5">
-        <v>323</v>
+        <v>330</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -8153,13 +8204,13 @@
         <v>50</v>
       </c>
       <c r="D19" t="s" s="5">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="E19" s="5">
         <v>50</v>
       </c>
       <c r="F19" t="s" s="5">
-        <v>326</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
@@ -8173,13 +8224,13 @@
         <v>50</v>
       </c>
       <c r="D20" t="s" s="5">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="E20" s="5">
         <v>20</v>
       </c>
       <c r="F20" t="s" s="5">
-        <v>329</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
@@ -8193,13 +8244,13 @@
         <v>50</v>
       </c>
       <c r="D21" t="s" s="5">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="E21" s="5">
         <v>10</v>
       </c>
       <c r="F21" t="s" s="5">
-        <v>332</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
@@ -8213,13 +8264,13 @@
         <v>50</v>
       </c>
       <c r="D22" t="s" s="10">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="E22" s="5">
         <v>50</v>
       </c>
       <c r="F22" t="s" s="5">
-        <v>335</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
@@ -8636,7 +8687,7 @@
         <v>163</v>
       </c>
       <c r="E43" s="5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F43" t="s" s="5">
         <v>164</v>
@@ -8656,7 +8707,7 @@
         <v>167</v>
       </c>
       <c r="E44" s="5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F44" t="s" s="5">
         <v>168</v>
@@ -8669,17 +8720,17 @@
       <c r="B45" s="5">
         <v>1</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="10">
         <v>50</v>
       </c>
       <c r="D45" t="s" s="5">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="E45" s="5">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F45" t="s" s="5">
-        <v>192</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
@@ -8689,17 +8740,17 @@
       <c r="B46" s="5">
         <v>1</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="12">
         <v>50</v>
       </c>
       <c r="D46" t="s" s="5">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="E46" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F46" t="s" s="5">
-        <v>195</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
@@ -8709,17 +8760,17 @@
       <c r="B47" s="5">
         <v>1</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="12">
         <v>50</v>
       </c>
       <c r="D47" t="s" s="5">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="E47" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F47" t="s" s="5">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
@@ -8729,17 +8780,17 @@
       <c r="B48" s="5">
         <v>1</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="12">
         <v>50</v>
       </c>
       <c r="D48" t="s" s="5">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="E48" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F48" t="s" s="5">
-        <v>201</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
@@ -8749,17 +8800,17 @@
       <c r="B49" s="5">
         <v>1</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="12">
         <v>50</v>
       </c>
       <c r="D49" t="s" s="5">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="E49" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F49" t="s" s="5">
-        <v>204</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
@@ -8769,17 +8820,17 @@
       <c r="B50" s="5">
         <v>1</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="11">
         <v>50</v>
       </c>
-      <c r="D50" t="s" s="10">
-        <v>206</v>
+      <c r="D50" t="s" s="5">
+        <v>197</v>
       </c>
       <c r="E50" s="5">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F50" t="s" s="5">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
@@ -8787,19 +8838,19 @@
         <v>49</v>
       </c>
       <c r="B51" s="5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C51" s="5">
         <v>50</v>
       </c>
-      <c r="D51" t="s" s="11">
-        <v>209</v>
+      <c r="D51" t="s" s="5">
+        <v>201</v>
       </c>
       <c r="E51" s="5">
         <v>100</v>
       </c>
       <c r="F51" t="s" s="5">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
@@ -8813,13 +8864,13 @@
         <v>50</v>
       </c>
       <c r="D52" t="s" s="5">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E52" s="5">
         <v>100</v>
       </c>
       <c r="F52" t="s" s="5">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
@@ -8833,13 +8884,13 @@
         <v>50</v>
       </c>
       <c r="D53" t="s" s="5">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="E53" s="5">
         <v>100</v>
       </c>
       <c r="F53" t="s" s="5">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
@@ -8847,19 +8898,19 @@
         <v>52</v>
       </c>
       <c r="B54" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C54" s="5">
         <v>50</v>
       </c>
       <c r="D54" t="s" s="5">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E54" s="5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F54" t="s" s="5">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
@@ -8870,16 +8921,16 @@
         <v>1</v>
       </c>
       <c r="C55" s="5">
-        <v>10</v>
-      </c>
-      <c r="D55" t="s" s="5">
-        <v>363</v>
+        <v>50</v>
+      </c>
+      <c r="D55" t="s" s="10">
+        <v>213</v>
       </c>
       <c r="E55" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F55" t="s" s="5">
-        <v>365</v>
+        <v>214</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
@@ -8887,19 +8938,19 @@
         <v>54</v>
       </c>
       <c r="B56" s="5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C56" s="5">
-        <v>10</v>
-      </c>
-      <c r="D56" t="s" s="5">
-        <v>367</v>
+        <v>50</v>
+      </c>
+      <c r="D56" t="s" s="11">
+        <v>216</v>
       </c>
       <c r="E56" s="5">
         <v>100</v>
       </c>
       <c r="F56" t="s" s="5">
-        <v>368</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
@@ -8910,16 +8961,16 @@
         <v>1</v>
       </c>
       <c r="C57" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D57" t="s" s="5">
-        <v>370</v>
+        <v>219</v>
       </c>
       <c r="E57" s="5">
         <v>100</v>
       </c>
       <c r="F57" t="s" s="5">
-        <v>371</v>
+        <v>220</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
@@ -8927,19 +8978,19 @@
         <v>56</v>
       </c>
       <c r="B58" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C58" s="5">
         <v>50</v>
       </c>
       <c r="D58" t="s" s="5">
-        <v>373</v>
+        <v>222</v>
       </c>
       <c r="E58" s="5">
         <v>100</v>
       </c>
       <c r="F58" t="s" s="5">
-        <v>374</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
@@ -8953,13 +9004,113 @@
         <v>50</v>
       </c>
       <c r="D59" t="s" s="5">
-        <v>376</v>
+        <v>226</v>
       </c>
       <c r="E59" s="5">
+        <v>50</v>
+      </c>
+      <c r="F59" t="s" s="5">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="60" ht="20" customHeight="1">
+      <c r="A60" s="3">
+        <v>58</v>
+      </c>
+      <c r="B60" s="5">
+        <v>1</v>
+      </c>
+      <c r="C60" s="5">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s" s="5">
+        <v>370</v>
+      </c>
+      <c r="E60" s="5">
         <v>100</v>
       </c>
-      <c r="F59" t="s" s="5">
+      <c r="F60" t="s" s="5">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="61" ht="20" customHeight="1">
+      <c r="A61" s="3">
+        <v>59</v>
+      </c>
+      <c r="B61" s="5">
+        <v>1</v>
+      </c>
+      <c r="C61" s="5">
+        <v>10</v>
+      </c>
+      <c r="D61" t="s" s="5">
+        <v>374</v>
+      </c>
+      <c r="E61" s="5">
+        <v>100</v>
+      </c>
+      <c r="F61" t="s" s="5">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="62" ht="20" customHeight="1">
+      <c r="A62" s="3">
+        <v>60</v>
+      </c>
+      <c r="B62" s="5">
+        <v>1</v>
+      </c>
+      <c r="C62" s="5">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s" s="5">
         <v>377</v>
+      </c>
+      <c r="E62" s="5">
+        <v>100</v>
+      </c>
+      <c r="F62" t="s" s="5">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="63" ht="20" customHeight="1">
+      <c r="A63" s="3">
+        <v>61</v>
+      </c>
+      <c r="B63" s="5">
+        <v>20</v>
+      </c>
+      <c r="C63" s="5">
+        <v>50</v>
+      </c>
+      <c r="D63" t="s" s="5">
+        <v>380</v>
+      </c>
+      <c r="E63" s="5">
+        <v>100</v>
+      </c>
+      <c r="F63" t="s" s="5">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="64" ht="20" customHeight="1">
+      <c r="A64" s="3">
+        <v>62</v>
+      </c>
+      <c r="B64" s="5">
+        <v>20</v>
+      </c>
+      <c r="C64" s="5">
+        <v>50</v>
+      </c>
+      <c r="D64" t="s" s="5">
+        <v>383</v>
+      </c>
+      <c r="E64" s="5">
+        <v>100</v>
+      </c>
+      <c r="F64" t="s" s="5">
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #563 FlixelRL-563 指輪の種類を増やす
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="433">
   <si>
     <t>id</t>
   </si>
@@ -1144,7 +1144,7 @@
     <t>守りの指輪</t>
   </si>
   <si>
-    <t>耐久力が1ポイント上昇します</t>
+    <t>敵からのダメージを少し減らします</t>
   </si>
   <si>
     <t>RING3</t>
@@ -1189,88 +1189,112 @@
     <t>RING7</t>
   </si>
   <si>
-    <t>指輪ダミー7</t>
-  </si>
-  <si>
-    <t>指輪の説明文</t>
+    <t>力の指輪+1</t>
+  </si>
+  <si>
+    <t>力が2ポイント上昇します</t>
   </si>
   <si>
     <t>RING8</t>
   </si>
   <si>
-    <t>指輪ダミー8</t>
+    <t>力の指輪+2</t>
+  </si>
+  <si>
+    <t>力が3ポイント上昇します</t>
   </si>
   <si>
     <t>RING9</t>
   </si>
   <si>
-    <t>指輪ダミー9</t>
+    <t>力の指輪+3</t>
+  </si>
+  <si>
+    <t>力が4ポイント上昇します</t>
   </si>
   <si>
     <t>RING10</t>
   </si>
   <si>
-    <t>指輪ダミー10</t>
+    <t>力の指輪+4</t>
+  </si>
+  <si>
+    <t>力が5ポイント上昇します</t>
   </si>
   <si>
     <t>RING11</t>
   </si>
   <si>
-    <t>指輪ダミー11</t>
+    <t>守りの指輪+1</t>
   </si>
   <si>
     <t>RING12</t>
   </si>
   <si>
-    <t>指輪ダミー12</t>
+    <t>守りの指輪+2</t>
   </si>
   <si>
     <t>RING13</t>
   </si>
   <si>
-    <t>指輪ダミー13</t>
+    <t>守りの指輪+3</t>
   </si>
   <si>
     <t>RING14</t>
   </si>
   <si>
-    <t>指輪ダミー14</t>
+    <t>守りの指輪+4</t>
   </si>
   <si>
     <t>RING15</t>
   </si>
   <si>
-    <t>指輪ダミー15</t>
+    <t>HP増加の指輪+1</t>
   </si>
   <si>
     <t>RING16</t>
   </si>
   <si>
-    <t>指輪ダミー16</t>
+    <t>HP増加の指輪+2</t>
+  </si>
+  <si>
+    <t>最大HPが20上昇します</t>
   </si>
   <si>
     <t>RING17</t>
   </si>
   <si>
-    <t>指輪ダミー17</t>
+    <t>HP増加の指輪+3</t>
+  </si>
+  <si>
+    <t>最大HPが30上昇します</t>
   </si>
   <si>
     <t>RING18</t>
   </si>
   <si>
-    <t>指輪ダミー18</t>
+    <t>HP増加の指輪+4</t>
+  </si>
+  <si>
+    <t>最大HPが40上昇します</t>
   </si>
   <si>
     <t>RING19</t>
   </si>
   <si>
-    <t>指輪ダミー19</t>
+    <t>プラチナリング</t>
+  </si>
+  <si>
+    <t>力+1 / ダメージ減少 / HP+10</t>
   </si>
   <si>
     <t>RING20</t>
   </si>
   <si>
-    <t>指輪ダミー20</t>
+    <t>ドラゴンの指輪</t>
+  </si>
+  <si>
+    <t>力+3 / HP+30</t>
   </si>
   <si>
     <t>start</t>
@@ -1283,6 +1307,9 @@
   </si>
   <si>
     <t>ratio</t>
+  </si>
+  <si>
+    <t>shop_only</t>
   </si>
   <si>
     <t>comment</t>
@@ -5744,7 +5771,7 @@
     <col min="4" max="4" width="3.125" style="8" customWidth="1"/>
     <col min="5" max="5" width="3.125" style="8" customWidth="1"/>
     <col min="6" max="6" width="3.125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="6.39844" style="8" customWidth="1"/>
+    <col min="7" max="7" width="6.75" style="8" customWidth="1"/>
     <col min="8" max="8" width="6" style="8" customWidth="1"/>
     <col min="9" max="9" width="3.875" style="8" customWidth="1"/>
     <col min="10" max="10" width="4" style="8" customWidth="1"/>
@@ -7181,11 +7208,11 @@
       <c r="H43" s="6"/>
       <c r="I43" s="7"/>
       <c r="J43" s="6">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="K43" s="6">
         <f>J43*0.35</f>
-        <v>175</v>
+        <v>105</v>
       </c>
       <c r="L43" s="6">
         <v>140</v>
@@ -7213,11 +7240,11 @@
       <c r="H44" s="6"/>
       <c r="I44" s="7"/>
       <c r="J44" s="6">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="K44" s="6">
         <f>J44*0.35</f>
-        <v>175</v>
+        <v>105</v>
       </c>
       <c r="L44" s="6">
         <v>141</v>
@@ -7247,11 +7274,11 @@
       </c>
       <c r="I45" s="7"/>
       <c r="J45" s="6">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="K45" s="6">
         <f>J45*0.35</f>
-        <v>175</v>
+        <v>105</v>
       </c>
       <c r="L45" s="6">
         <v>142</v>
@@ -7366,20 +7393,20 @@
       <c r="C49" t="s" s="5">
         <v>391</v>
       </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="5">
-        <v>1</v>
-      </c>
+      <c r="D49" s="6">
+        <v>2</v>
+      </c>
+      <c r="E49" s="7"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="7"/>
       <c r="J49" s="6">
-        <v>3</v>
+        <v>500</v>
       </c>
       <c r="K49" s="6">
         <f>J49*0.35</f>
-        <v>1.05</v>
+        <v>175</v>
       </c>
       <c r="L49" s="6">
         <v>146</v>
@@ -7398,410 +7425,428 @@
       <c r="C50" t="s" s="5">
         <v>394</v>
       </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="5">
-        <v>1</v>
-      </c>
+      <c r="D50" s="6">
+        <v>3</v>
+      </c>
+      <c r="E50" s="7"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="7"/>
       <c r="J50" s="6">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="K50" s="6">
         <f>J50*0.35</f>
-        <v>1.05</v>
+        <v>350</v>
       </c>
       <c r="L50" s="6">
         <v>147</v>
       </c>
       <c r="M50" t="s" s="5">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B51" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C51" t="s" s="5">
-        <v>396</v>
-      </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="5">
-        <v>1</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="D51" s="6">
+        <v>4</v>
+      </c>
+      <c r="E51" s="7"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
       <c r="I51" s="7"/>
       <c r="J51" s="6">
-        <v>3</v>
+        <v>2500</v>
       </c>
       <c r="K51" s="6">
         <f>J51*0.35</f>
-        <v>1.05</v>
+        <v>875</v>
       </c>
       <c r="L51" s="6">
         <v>148</v>
       </c>
       <c r="M51" t="s" s="5">
-        <v>392</v>
+        <v>398</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B52" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C52" t="s" s="5">
-        <v>398</v>
-      </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="5">
-        <v>1</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="D52" s="6">
+        <v>5</v>
+      </c>
+      <c r="E52" s="7"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
       <c r="I52" s="7"/>
       <c r="J52" s="6">
-        <v>3</v>
+        <v>5000</v>
       </c>
       <c r="K52" s="6">
         <f>J52*0.35</f>
-        <v>1.05</v>
+        <v>1750</v>
       </c>
       <c r="L52" s="6">
         <v>149</v>
       </c>
       <c r="M52" t="s" s="5">
-        <v>392</v>
+        <v>401</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" t="s" s="3">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B53" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C53" t="s" s="5">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="7"/>
       <c r="J53" s="6">
-        <v>3</v>
+        <v>500</v>
       </c>
       <c r="K53" s="6">
         <f>J53*0.35</f>
-        <v>1.05</v>
+        <v>175</v>
       </c>
       <c r="L53" s="6">
         <v>150</v>
       </c>
       <c r="M53" t="s" s="5">
-        <v>392</v>
+        <v>376</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" t="s" s="3">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B54" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C54" t="s" s="5">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
       <c r="I54" s="7"/>
       <c r="J54" s="6">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="K54" s="6">
         <f>J54*0.35</f>
-        <v>1.05</v>
+        <v>350</v>
       </c>
       <c r="L54" s="6">
         <v>151</v>
       </c>
       <c r="M54" t="s" s="5">
-        <v>392</v>
+        <v>376</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B55" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C55" t="s" s="5">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
       <c r="I55" s="7"/>
       <c r="J55" s="6">
-        <v>3</v>
+        <v>2500</v>
       </c>
       <c r="K55" s="6">
         <f>J55*0.35</f>
-        <v>1.05</v>
+        <v>875</v>
       </c>
       <c r="L55" s="6">
         <v>152</v>
       </c>
       <c r="M55" t="s" s="5">
-        <v>392</v>
+        <v>376</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B56" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C56" t="s" s="5">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
       <c r="I56" s="7"/>
       <c r="J56" s="6">
-        <v>3</v>
+        <v>5000</v>
       </c>
       <c r="K56" s="6">
         <f>J56*0.35</f>
-        <v>1.05</v>
+        <v>1750</v>
       </c>
       <c r="L56" s="6">
         <v>153</v>
       </c>
       <c r="M56" t="s" s="5">
-        <v>392</v>
+        <v>376</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="B57" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C57" t="s" s="5">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="D57" s="6"/>
-      <c r="E57" s="5">
-        <v>1</v>
-      </c>
+      <c r="E57" s="7"/>
       <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
+      <c r="G57" t="s" s="5">
+        <v>93</v>
+      </c>
+      <c r="H57" s="6">
+        <v>20</v>
+      </c>
       <c r="I57" s="7"/>
       <c r="J57" s="6">
-        <v>3</v>
+        <v>500</v>
       </c>
       <c r="K57" s="6">
         <f>J57*0.35</f>
-        <v>1.05</v>
+        <v>175</v>
       </c>
       <c r="L57" s="6">
         <v>154</v>
       </c>
       <c r="M57" t="s" s="5">
-        <v>392</v>
+        <v>379</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="B58" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C58" t="s" s="5">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="D58" s="6"/>
-      <c r="E58" s="5">
-        <v>1</v>
-      </c>
+      <c r="E58" s="7"/>
       <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
+      <c r="G58" t="s" s="5">
+        <v>93</v>
+      </c>
+      <c r="H58" s="6">
+        <v>30</v>
+      </c>
       <c r="I58" s="7"/>
       <c r="J58" s="6">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="K58" s="6">
         <f>J58*0.35</f>
-        <v>1.05</v>
+        <v>350</v>
       </c>
       <c r="L58" s="6">
         <v>155</v>
       </c>
       <c r="M58" t="s" s="5">
-        <v>392</v>
+        <v>414</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B59" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C59" t="s" s="5">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="D59" s="6"/>
-      <c r="E59" s="5">
-        <v>1</v>
-      </c>
+      <c r="E59" s="7"/>
       <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
+      <c r="G59" t="s" s="5">
+        <v>93</v>
+      </c>
+      <c r="H59" s="6">
+        <v>40</v>
+      </c>
       <c r="I59" s="7"/>
       <c r="J59" s="6">
-        <v>3</v>
+        <v>2500</v>
       </c>
       <c r="K59" s="6">
         <f>J59*0.35</f>
-        <v>1.05</v>
+        <v>875</v>
       </c>
       <c r="L59" s="6">
         <v>156</v>
       </c>
       <c r="M59" t="s" s="5">
-        <v>392</v>
+        <v>417</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="B60" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C60" t="s" s="5">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D60" s="6"/>
-      <c r="E60" s="5">
-        <v>1</v>
-      </c>
+      <c r="E60" s="7"/>
       <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
+      <c r="G60" t="s" s="5">
+        <v>93</v>
+      </c>
+      <c r="H60" s="6">
+        <v>50</v>
+      </c>
       <c r="I60" s="7"/>
       <c r="J60" s="6">
-        <v>3</v>
+        <v>5000</v>
       </c>
       <c r="K60" s="6">
         <f>J60*0.35</f>
-        <v>1.05</v>
+        <v>1750</v>
       </c>
       <c r="L60" s="6">
         <v>157</v>
       </c>
       <c r="M60" t="s" s="5">
-        <v>392</v>
+        <v>420</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="B61" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C61" t="s" s="5">
-        <v>416</v>
-      </c>
-      <c r="D61" s="6"/>
+        <v>422</v>
+      </c>
+      <c r="D61" s="6">
+        <v>1</v>
+      </c>
       <c r="E61" s="5">
         <v>1</v>
       </c>
       <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
+      <c r="G61" t="s" s="5">
+        <v>93</v>
+      </c>
+      <c r="H61" s="6">
+        <v>10</v>
+      </c>
       <c r="I61" s="7"/>
       <c r="J61" s="6">
-        <v>3</v>
+        <v>1500</v>
       </c>
       <c r="K61" s="6">
         <f>J61*0.35</f>
-        <v>1.05</v>
+        <v>525</v>
       </c>
       <c r="L61" s="6">
         <v>158</v>
       </c>
       <c r="M61" t="s" s="5">
-        <v>392</v>
+        <v>423</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="B62" t="s" s="5">
         <v>371</v>
       </c>
       <c r="C62" t="s" s="5">
-        <v>418</v>
-      </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="5">
-        <v>1</v>
-      </c>
+        <v>425</v>
+      </c>
+      <c r="D62" s="6">
+        <v>3</v>
+      </c>
+      <c r="E62" s="7"/>
       <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-      <c r="H62" s="6"/>
+      <c r="G62" t="s" s="5">
+        <v>93</v>
+      </c>
+      <c r="H62" s="6">
+        <v>30</v>
+      </c>
       <c r="I62" s="7"/>
       <c r="J62" s="6">
-        <v>3</v>
+        <v>5000</v>
       </c>
       <c r="K62" s="6">
         <f>J62*0.35</f>
-        <v>1.05</v>
+        <v>1750</v>
       </c>
       <c r="L62" s="6">
         <v>159</v>
       </c>
       <c r="M62" t="s" s="5">
-        <v>392</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -7818,7 +7863,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -7829,8 +7874,9 @@
     <col min="3" max="3" width="5.90625" style="9" customWidth="1"/>
     <col min="4" max="4" width="9.19531" style="9" customWidth="1"/>
     <col min="5" max="5" width="9.375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="9" customWidth="1"/>
-    <col min="7" max="256" width="12.25" style="9" customWidth="1"/>
+    <col min="6" max="6" width="7.375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="10.375" style="9" customWidth="1"/>
+    <col min="8" max="256" width="12.25" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -7838,19 +7884,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>422</v>
+        <v>430</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>423</v>
+        <v>431</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>432</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -7870,6 +7919,9 @@
         <v>13</v>
       </c>
       <c r="F2" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="5">
         <v>14</v>
       </c>
     </row>
@@ -7889,7 +7941,10 @@
       <c r="E3" s="5">
         <v>500</v>
       </c>
-      <c r="F3" t="s" s="5">
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s" s="5">
         <v>17</v>
       </c>
     </row>
@@ -7909,7 +7964,10 @@
       <c r="E4" s="5">
         <v>120</v>
       </c>
-      <c r="F4" t="s" s="5">
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s" s="5">
         <v>20</v>
       </c>
     </row>
@@ -7929,7 +7987,10 @@
       <c r="E5" s="5">
         <v>120</v>
       </c>
-      <c r="F5" t="s" s="5">
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s" s="5">
         <v>23</v>
       </c>
     </row>
@@ -7949,7 +8010,10 @@
       <c r="E6" s="5">
         <v>50</v>
       </c>
-      <c r="F6" t="s" s="5">
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s" s="5">
         <v>26</v>
       </c>
     </row>
@@ -7969,7 +8033,10 @@
       <c r="E7" s="5">
         <v>500</v>
       </c>
-      <c r="F7" t="s" s="5">
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s" s="5">
         <v>270</v>
       </c>
     </row>
@@ -7989,7 +8056,10 @@
       <c r="E8" s="5">
         <v>300</v>
       </c>
-      <c r="F8" t="s" s="5">
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s" s="5">
         <v>273</v>
       </c>
     </row>
@@ -8009,7 +8079,10 @@
       <c r="E9" s="5">
         <v>200</v>
       </c>
-      <c r="F9" t="s" s="5">
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s" s="5">
         <v>276</v>
       </c>
     </row>
@@ -8029,7 +8102,10 @@
       <c r="E10" s="5">
         <v>100</v>
       </c>
-      <c r="F10" t="s" s="5">
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s" s="5">
         <v>279</v>
       </c>
     </row>
@@ -8049,7 +8125,10 @@
       <c r="E11" s="5">
         <v>50</v>
       </c>
-      <c r="F11" t="s" s="5">
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s" s="5">
         <v>282</v>
       </c>
     </row>
@@ -8069,7 +8148,10 @@
       <c r="E12" s="5">
         <v>20</v>
       </c>
-      <c r="F12" t="s" s="5">
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s" s="5">
         <v>285</v>
       </c>
     </row>
@@ -8089,7 +8171,10 @@
       <c r="E13" s="5">
         <v>10</v>
       </c>
-      <c r="F13" t="s" s="5">
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s" s="5">
         <v>288</v>
       </c>
     </row>
@@ -8109,7 +8194,10 @@
       <c r="E14" s="5">
         <v>50</v>
       </c>
-      <c r="F14" t="s" s="5">
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s" s="5">
         <v>291</v>
       </c>
     </row>
@@ -8129,7 +8217,10 @@
       <c r="E15" s="5">
         <v>500</v>
       </c>
-      <c r="F15" t="s" s="5">
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s" s="5">
         <v>321</v>
       </c>
     </row>
@@ -8149,7 +8240,10 @@
       <c r="E16" s="5">
         <v>300</v>
       </c>
-      <c r="F16" t="s" s="5">
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s" s="5">
         <v>324</v>
       </c>
     </row>
@@ -8169,7 +8263,10 @@
       <c r="E17" s="5">
         <v>200</v>
       </c>
-      <c r="F17" t="s" s="5">
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s" s="5">
         <v>327</v>
       </c>
     </row>
@@ -8189,7 +8286,10 @@
       <c r="E18" s="5">
         <v>100</v>
       </c>
-      <c r="F18" t="s" s="5">
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s" s="5">
         <v>330</v>
       </c>
     </row>
@@ -8209,7 +8309,10 @@
       <c r="E19" s="5">
         <v>50</v>
       </c>
-      <c r="F19" t="s" s="5">
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s" s="5">
         <v>333</v>
       </c>
     </row>
@@ -8229,7 +8332,10 @@
       <c r="E20" s="5">
         <v>20</v>
       </c>
-      <c r="F20" t="s" s="5">
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s" s="5">
         <v>336</v>
       </c>
     </row>
@@ -8249,7 +8355,10 @@
       <c r="E21" s="5">
         <v>10</v>
       </c>
-      <c r="F21" t="s" s="5">
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s" s="5">
         <v>339</v>
       </c>
     </row>
@@ -8269,7 +8378,10 @@
       <c r="E22" s="5">
         <v>50</v>
       </c>
-      <c r="F22" t="s" s="5">
+      <c r="F22" s="5">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s" s="5">
         <v>342</v>
       </c>
     </row>
@@ -8289,7 +8401,10 @@
       <c r="E23" s="5">
         <v>1000</v>
       </c>
-      <c r="F23" t="s" s="5">
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s" s="5">
         <v>44</v>
       </c>
     </row>
@@ -8309,7 +8424,10 @@
       <c r="E24" s="5">
         <v>500</v>
       </c>
-      <c r="F24" t="s" s="5">
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s" s="5">
         <v>47</v>
       </c>
     </row>
@@ -8329,7 +8447,10 @@
       <c r="E25" s="5">
         <v>250</v>
       </c>
-      <c r="F25" t="s" s="5">
+      <c r="F25" s="5">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s" s="5">
         <v>50</v>
       </c>
     </row>
@@ -8349,7 +8470,10 @@
       <c r="E26" s="5">
         <v>120</v>
       </c>
-      <c r="F26" t="s" s="5">
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s" s="5">
         <v>53</v>
       </c>
     </row>
@@ -8369,7 +8493,10 @@
       <c r="E27" s="5">
         <v>60</v>
       </c>
-      <c r="F27" t="s" s="5">
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s" s="5">
         <v>56</v>
       </c>
     </row>
@@ -8389,7 +8516,10 @@
       <c r="E28" s="5">
         <v>30</v>
       </c>
-      <c r="F28" t="s" s="5">
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s" s="5">
         <v>59</v>
       </c>
     </row>
@@ -8409,7 +8539,10 @@
       <c r="E29" s="5">
         <v>500</v>
       </c>
-      <c r="F29" t="s" s="5">
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s" s="5">
         <v>92</v>
       </c>
     </row>
@@ -8429,7 +8562,10 @@
       <c r="E30" s="5">
         <v>500</v>
       </c>
-      <c r="F30" t="s" s="5">
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s" s="5">
         <v>96</v>
       </c>
     </row>
@@ -8449,7 +8585,10 @@
       <c r="E31" s="5">
         <v>500</v>
       </c>
-      <c r="F31" t="s" s="5">
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s" s="5">
         <v>99</v>
       </c>
     </row>
@@ -8469,7 +8608,10 @@
       <c r="E32" s="5">
         <v>100</v>
       </c>
-      <c r="F32" t="s" s="5">
+      <c r="F32" s="5">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s" s="5">
         <v>102</v>
       </c>
     </row>
@@ -8489,7 +8631,10 @@
       <c r="E33" s="5">
         <v>100</v>
       </c>
-      <c r="F33" t="s" s="5">
+      <c r="F33" s="5">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s" s="5">
         <v>105</v>
       </c>
     </row>
@@ -8509,7 +8654,10 @@
       <c r="E34" s="5">
         <v>100</v>
       </c>
-      <c r="F34" t="s" s="5">
+      <c r="F34" s="5">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s" s="5">
         <v>109</v>
       </c>
     </row>
@@ -8529,7 +8677,10 @@
       <c r="E35" s="5">
         <v>100</v>
       </c>
-      <c r="F35" t="s" s="5">
+      <c r="F35" s="5">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s" s="5">
         <v>113</v>
       </c>
     </row>
@@ -8549,7 +8700,10 @@
       <c r="E36" s="5">
         <v>100</v>
       </c>
-      <c r="F36" t="s" s="5">
+      <c r="F36" s="5">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s" s="5">
         <v>117</v>
       </c>
     </row>
@@ -8569,7 +8723,10 @@
       <c r="E37" s="5">
         <v>100</v>
       </c>
-      <c r="F37" t="s" s="5">
+      <c r="F37" s="5">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s" s="5">
         <v>121</v>
       </c>
     </row>
@@ -8589,7 +8746,10 @@
       <c r="E38" s="5">
         <v>100</v>
       </c>
-      <c r="F38" t="s" s="5">
+      <c r="F38" s="5">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s" s="5">
         <v>125</v>
       </c>
     </row>
@@ -8609,7 +8769,10 @@
       <c r="E39" s="5">
         <v>100</v>
       </c>
-      <c r="F39" t="s" s="5">
+      <c r="F39" s="5">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s" s="5">
         <v>129</v>
       </c>
     </row>
@@ -8629,7 +8792,10 @@
       <c r="E40" s="5">
         <v>100</v>
       </c>
-      <c r="F40" t="s" s="5">
+      <c r="F40" s="5">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s" s="5">
         <v>133</v>
       </c>
     </row>
@@ -8649,7 +8815,10 @@
       <c r="E41" s="5">
         <v>20</v>
       </c>
-      <c r="F41" t="s" s="5">
+      <c r="F41" s="5">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s" s="5">
         <v>147</v>
       </c>
     </row>
@@ -8669,7 +8838,10 @@
       <c r="E42" s="5">
         <v>10</v>
       </c>
-      <c r="F42" t="s" s="5">
+      <c r="F42" s="5">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s" s="5">
         <v>151</v>
       </c>
     </row>
@@ -8689,7 +8861,10 @@
       <c r="E43" s="5">
         <v>30</v>
       </c>
-      <c r="F43" t="s" s="5">
+      <c r="F43" s="5">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s" s="5">
         <v>164</v>
       </c>
     </row>
@@ -8709,7 +8884,10 @@
       <c r="E44" s="5">
         <v>30</v>
       </c>
-      <c r="F44" t="s" s="5">
+      <c r="F44" s="5">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s" s="5">
         <v>168</v>
       </c>
     </row>
@@ -8729,7 +8907,10 @@
       <c r="E45" s="5">
         <v>50</v>
       </c>
-      <c r="F45" t="s" s="5">
+      <c r="F45" s="5">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s" s="5">
         <v>172</v>
       </c>
     </row>
@@ -8749,7 +8930,10 @@
       <c r="E46" s="5">
         <v>50</v>
       </c>
-      <c r="F46" t="s" s="5">
+      <c r="F46" s="5">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s" s="5">
         <v>175</v>
       </c>
     </row>
@@ -8769,7 +8953,10 @@
       <c r="E47" s="5">
         <v>50</v>
       </c>
-      <c r="F47" t="s" s="5">
+      <c r="F47" s="5">
+        <v>0</v>
+      </c>
+      <c r="G47" t="s" s="5">
         <v>178</v>
       </c>
     </row>
@@ -8789,7 +8976,10 @@
       <c r="E48" s="5">
         <v>10</v>
       </c>
-      <c r="F48" t="s" s="5">
+      <c r="F48" s="5">
+        <v>0</v>
+      </c>
+      <c r="G48" t="s" s="5">
         <v>181</v>
       </c>
     </row>
@@ -8809,7 +8999,10 @@
       <c r="E49" s="5">
         <v>10</v>
       </c>
-      <c r="F49" t="s" s="5">
+      <c r="F49" s="5">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s" s="5">
         <v>185</v>
       </c>
     </row>
@@ -8829,7 +9022,10 @@
       <c r="E50" s="5">
         <v>80</v>
       </c>
-      <c r="F50" t="s" s="5">
+      <c r="F50" s="5">
+        <v>0</v>
+      </c>
+      <c r="G50" t="s" s="5">
         <v>199</v>
       </c>
     </row>
@@ -8849,7 +9045,10 @@
       <c r="E51" s="5">
         <v>100</v>
       </c>
-      <c r="F51" t="s" s="5">
+      <c r="F51" s="5">
+        <v>0</v>
+      </c>
+      <c r="G51" t="s" s="5">
         <v>202</v>
       </c>
     </row>
@@ -8869,7 +9068,10 @@
       <c r="E52" s="5">
         <v>100</v>
       </c>
-      <c r="F52" t="s" s="5">
+      <c r="F52" s="5">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s" s="5">
         <v>205</v>
       </c>
     </row>
@@ -8889,7 +9091,10 @@
       <c r="E53" s="5">
         <v>100</v>
       </c>
-      <c r="F53" t="s" s="5">
+      <c r="F53" s="5">
+        <v>0</v>
+      </c>
+      <c r="G53" t="s" s="5">
         <v>208</v>
       </c>
     </row>
@@ -8909,7 +9114,10 @@
       <c r="E54" s="5">
         <v>0</v>
       </c>
-      <c r="F54" t="s" s="5">
+      <c r="F54" s="5">
+        <v>0</v>
+      </c>
+      <c r="G54" t="s" s="5">
         <v>211</v>
       </c>
     </row>
@@ -8929,7 +9137,10 @@
       <c r="E55" s="5">
         <v>0</v>
       </c>
-      <c r="F55" t="s" s="5">
+      <c r="F55" s="5">
+        <v>0</v>
+      </c>
+      <c r="G55" t="s" s="5">
         <v>214</v>
       </c>
     </row>
@@ -8949,7 +9160,10 @@
       <c r="E56" s="5">
         <v>100</v>
       </c>
-      <c r="F56" t="s" s="5">
+      <c r="F56" s="5">
+        <v>0</v>
+      </c>
+      <c r="G56" t="s" s="5">
         <v>217</v>
       </c>
     </row>
@@ -8969,7 +9183,10 @@
       <c r="E57" s="5">
         <v>100</v>
       </c>
-      <c r="F57" t="s" s="5">
+      <c r="F57" s="5">
+        <v>0</v>
+      </c>
+      <c r="G57" t="s" s="5">
         <v>220</v>
       </c>
     </row>
@@ -8989,7 +9206,10 @@
       <c r="E58" s="5">
         <v>100</v>
       </c>
-      <c r="F58" t="s" s="5">
+      <c r="F58" s="5">
+        <v>0</v>
+      </c>
+      <c r="G58" t="s" s="5">
         <v>223</v>
       </c>
     </row>
@@ -9009,7 +9229,10 @@
       <c r="E59" s="5">
         <v>50</v>
       </c>
-      <c r="F59" t="s" s="5">
+      <c r="F59" s="5">
+        <v>0</v>
+      </c>
+      <c r="G59" t="s" s="5">
         <v>227</v>
       </c>
     </row>
@@ -9029,7 +9252,10 @@
       <c r="E60" s="5">
         <v>100</v>
       </c>
-      <c r="F60" t="s" s="5">
+      <c r="F60" s="5">
+        <v>0</v>
+      </c>
+      <c r="G60" t="s" s="5">
         <v>372</v>
       </c>
     </row>
@@ -9049,7 +9275,10 @@
       <c r="E61" s="5">
         <v>100</v>
       </c>
-      <c r="F61" t="s" s="5">
+      <c r="F61" s="5">
+        <v>0</v>
+      </c>
+      <c r="G61" t="s" s="5">
         <v>375</v>
       </c>
     </row>
@@ -9069,7 +9298,10 @@
       <c r="E62" s="5">
         <v>100</v>
       </c>
-      <c r="F62" t="s" s="5">
+      <c r="F62" s="5">
+        <v>0</v>
+      </c>
+      <c r="G62" t="s" s="5">
         <v>378</v>
       </c>
     </row>
@@ -9089,7 +9321,10 @@
       <c r="E63" s="5">
         <v>100</v>
       </c>
-      <c r="F63" t="s" s="5">
+      <c r="F63" s="5">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s" s="5">
         <v>381</v>
       </c>
     </row>
@@ -9109,8 +9344,356 @@
       <c r="E64" s="5">
         <v>100</v>
       </c>
-      <c r="F64" t="s" s="5">
+      <c r="F64" s="5">
+        <v>1</v>
+      </c>
+      <c r="G64" t="s" s="5">
         <v>384</v>
+      </c>
+    </row>
+    <row r="65" ht="20" customHeight="1">
+      <c r="A65" s="3">
+        <v>63</v>
+      </c>
+      <c r="B65" s="5">
+        <v>30</v>
+      </c>
+      <c r="C65" s="5">
+        <v>50</v>
+      </c>
+      <c r="D65" t="s" s="5">
+        <v>386</v>
+      </c>
+      <c r="E65" s="5">
+        <v>0</v>
+      </c>
+      <c r="F65" s="5">
+        <v>1</v>
+      </c>
+      <c r="G65" t="s" s="5">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="66" ht="20" customHeight="1">
+      <c r="A66" s="3">
+        <v>64</v>
+      </c>
+      <c r="B66" s="5">
+        <v>5</v>
+      </c>
+      <c r="C66" s="5">
+        <v>15</v>
+      </c>
+      <c r="D66" t="s" s="5">
+        <v>390</v>
+      </c>
+      <c r="E66" s="5">
+        <v>50</v>
+      </c>
+      <c r="F66" s="5">
+        <v>0</v>
+      </c>
+      <c r="G66" t="s" s="5">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="67" ht="20" customHeight="1">
+      <c r="A67" s="3">
+        <v>65</v>
+      </c>
+      <c r="B67" s="5">
+        <v>10</v>
+      </c>
+      <c r="C67" s="5">
+        <v>30</v>
+      </c>
+      <c r="D67" t="s" s="5">
+        <v>393</v>
+      </c>
+      <c r="E67" s="5">
+        <v>30</v>
+      </c>
+      <c r="F67" s="5">
+        <v>0</v>
+      </c>
+      <c r="G67" t="s" s="5">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="68" ht="20" customHeight="1">
+      <c r="A68" s="3">
+        <v>66</v>
+      </c>
+      <c r="B68" s="5">
+        <v>15</v>
+      </c>
+      <c r="C68" s="5">
+        <v>40</v>
+      </c>
+      <c r="D68" t="s" s="5">
+        <v>396</v>
+      </c>
+      <c r="E68" s="5">
+        <v>20</v>
+      </c>
+      <c r="F68" s="5">
+        <v>1</v>
+      </c>
+      <c r="G68" t="s" s="5">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="69" ht="20" customHeight="1">
+      <c r="A69" s="3">
+        <v>67</v>
+      </c>
+      <c r="B69" s="5">
+        <v>20</v>
+      </c>
+      <c r="C69" s="5">
+        <v>50</v>
+      </c>
+      <c r="D69" t="s" s="5">
+        <v>399</v>
+      </c>
+      <c r="E69" s="5">
+        <v>10</v>
+      </c>
+      <c r="F69" s="5">
+        <v>1</v>
+      </c>
+      <c r="G69" t="s" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="70" ht="20" customHeight="1">
+      <c r="A70" s="3">
+        <v>68</v>
+      </c>
+      <c r="B70" s="5">
+        <v>5</v>
+      </c>
+      <c r="C70" s="5">
+        <v>15</v>
+      </c>
+      <c r="D70" t="s" s="5">
+        <v>402</v>
+      </c>
+      <c r="E70" s="5">
+        <v>50</v>
+      </c>
+      <c r="F70" s="5">
+        <v>0</v>
+      </c>
+      <c r="G70" t="s" s="5">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="71" ht="20" customHeight="1">
+      <c r="A71" s="3">
+        <v>69</v>
+      </c>
+      <c r="B71" s="5">
+        <v>10</v>
+      </c>
+      <c r="C71" s="5">
+        <v>30</v>
+      </c>
+      <c r="D71" t="s" s="5">
+        <v>404</v>
+      </c>
+      <c r="E71" s="5">
+        <v>30</v>
+      </c>
+      <c r="F71" s="5">
+        <v>0</v>
+      </c>
+      <c r="G71" t="s" s="5">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="72" ht="20" customHeight="1">
+      <c r="A72" s="3">
+        <v>70</v>
+      </c>
+      <c r="B72" s="5">
+        <v>15</v>
+      </c>
+      <c r="C72" s="5">
+        <v>40</v>
+      </c>
+      <c r="D72" t="s" s="5">
+        <v>406</v>
+      </c>
+      <c r="E72" s="5">
+        <v>20</v>
+      </c>
+      <c r="F72" s="5">
+        <v>1</v>
+      </c>
+      <c r="G72" t="s" s="5">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="73" ht="20" customHeight="1">
+      <c r="A73" s="3">
+        <v>71</v>
+      </c>
+      <c r="B73" s="5">
+        <v>20</v>
+      </c>
+      <c r="C73" s="5">
+        <v>50</v>
+      </c>
+      <c r="D73" t="s" s="5">
+        <v>408</v>
+      </c>
+      <c r="E73" s="5">
+        <v>10</v>
+      </c>
+      <c r="F73" s="5">
+        <v>1</v>
+      </c>
+      <c r="G73" t="s" s="5">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="74" ht="20" customHeight="1">
+      <c r="A74" s="3">
+        <v>72</v>
+      </c>
+      <c r="B74" s="5">
+        <v>5</v>
+      </c>
+      <c r="C74" s="5">
+        <v>15</v>
+      </c>
+      <c r="D74" t="s" s="5">
+        <v>410</v>
+      </c>
+      <c r="E74" s="5">
+        <v>50</v>
+      </c>
+      <c r="F74" s="5">
+        <v>0</v>
+      </c>
+      <c r="G74" t="s" s="5">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="75" ht="20" customHeight="1">
+      <c r="A75" s="3">
+        <v>73</v>
+      </c>
+      <c r="B75" s="5">
+        <v>10</v>
+      </c>
+      <c r="C75" s="5">
+        <v>30</v>
+      </c>
+      <c r="D75" t="s" s="5">
+        <v>412</v>
+      </c>
+      <c r="E75" s="5">
+        <v>30</v>
+      </c>
+      <c r="F75" s="5">
+        <v>0</v>
+      </c>
+      <c r="G75" t="s" s="5">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="76" ht="20" customHeight="1">
+      <c r="A76" s="3">
+        <v>74</v>
+      </c>
+      <c r="B76" s="5">
+        <v>15</v>
+      </c>
+      <c r="C76" s="5">
+        <v>40</v>
+      </c>
+      <c r="D76" t="s" s="5">
+        <v>415</v>
+      </c>
+      <c r="E76" s="5">
+        <v>20</v>
+      </c>
+      <c r="F76" s="5">
+        <v>1</v>
+      </c>
+      <c r="G76" t="s" s="5">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="77" ht="20" customHeight="1">
+      <c r="A77" s="3">
+        <v>75</v>
+      </c>
+      <c r="B77" s="5">
+        <v>20</v>
+      </c>
+      <c r="C77" s="5">
+        <v>50</v>
+      </c>
+      <c r="D77" t="s" s="5">
+        <v>418</v>
+      </c>
+      <c r="E77" s="5">
+        <v>10</v>
+      </c>
+      <c r="F77" s="5">
+        <v>1</v>
+      </c>
+      <c r="G77" t="s" s="5">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="78" ht="20" customHeight="1">
+      <c r="A78" s="3">
+        <v>76</v>
+      </c>
+      <c r="B78" s="5">
+        <v>10</v>
+      </c>
+      <c r="C78" s="5">
+        <v>50</v>
+      </c>
+      <c r="D78" t="s" s="5">
+        <v>421</v>
+      </c>
+      <c r="E78" s="5">
+        <v>20</v>
+      </c>
+      <c r="F78" s="5">
+        <v>1</v>
+      </c>
+      <c r="G78" t="s" s="5">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="79" ht="20" customHeight="1">
+      <c r="A79" s="3">
+        <v>77</v>
+      </c>
+      <c r="B79" s="5">
+        <v>20</v>
+      </c>
+      <c r="C79" s="5">
+        <v>50</v>
+      </c>
+      <c r="D79" t="s" s="5">
+        <v>424</v>
+      </c>
+      <c r="E79" s="5">
+        <v>20</v>
+      </c>
+      <c r="F79" s="5">
+        <v>1</v>
+      </c>
+      <c r="G79" t="s" s="5">
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #553 FlixelRL-553 武器合成の巻物
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -7868,7 +7868,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -8096,7 +8096,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="5">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C10" s="5">
         <v>40</v>
@@ -8119,7 +8119,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="5">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C11" s="5">
         <v>50</v>
@@ -8142,7 +8142,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="5">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C12" s="5">
         <v>50</v>
@@ -8165,7 +8165,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="5">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C13" s="5">
         <v>50</v>
@@ -8280,7 +8280,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C18" s="5">
         <v>40</v>
@@ -8303,7 +8303,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="5">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C19" s="5">
         <v>50</v>
@@ -8326,7 +8326,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="5">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C20" s="5">
         <v>50</v>
@@ -8349,7 +8349,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="5">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C21" s="5">
         <v>50</v>
@@ -8372,7 +8372,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="5">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C22" s="5">
         <v>50</v>
@@ -8487,16 +8487,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C27" s="5">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s" s="5">
         <v>55</v>
       </c>
       <c r="E27" s="5">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F27" s="5">
         <v>0</v>
@@ -8510,7 +8510,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="5">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C28" s="5">
         <v>30</v>
@@ -8519,7 +8519,7 @@
         <v>58</v>
       </c>
       <c r="E28" s="5">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="F28" s="5">
         <v>0</v>
@@ -8533,22 +8533,22 @@
         <v>27</v>
       </c>
       <c r="B29" s="5">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C29" s="5">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s" s="5">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="E29" s="5">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="F29" s="5">
         <v>0</v>
       </c>
       <c r="G29" t="s" s="5">
-        <v>92</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
@@ -8556,22 +8556,22 @@
         <v>28</v>
       </c>
       <c r="B30" s="5">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C30" s="5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s" s="5">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="E30" s="5">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="F30" s="5">
         <v>0</v>
       </c>
       <c r="G30" t="s" s="5">
-        <v>96</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
@@ -8579,22 +8579,22 @@
         <v>29</v>
       </c>
       <c r="B31" s="5">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C31" s="5">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s" s="5">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="E31" s="5">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="F31" s="5">
         <v>0</v>
       </c>
       <c r="G31" t="s" s="5">
-        <v>99</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
@@ -8602,22 +8602,22 @@
         <v>30</v>
       </c>
       <c r="B32" s="5">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C32" s="5">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s" s="5">
+        <v>70</v>
+      </c>
+      <c r="E32" s="5">
         <v>50</v>
-      </c>
-      <c r="D32" t="s" s="5">
-        <v>101</v>
-      </c>
-      <c r="E32" s="5">
-        <v>100</v>
       </c>
       <c r="F32" s="5">
         <v>0</v>
       </c>
       <c r="G32" t="s" s="5">
-        <v>102</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
@@ -8625,22 +8625,22 @@
         <v>31</v>
       </c>
       <c r="B33" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C33" s="5">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s" s="5">
+        <v>73</v>
+      </c>
+      <c r="E33" s="5">
         <v>50</v>
-      </c>
-      <c r="D33" t="s" s="5">
-        <v>104</v>
-      </c>
-      <c r="E33" s="5">
-        <v>100</v>
       </c>
       <c r="F33" s="5">
         <v>0</v>
       </c>
       <c r="G33" t="s" s="5">
-        <v>105</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -8648,22 +8648,22 @@
         <v>32</v>
       </c>
       <c r="B34" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C34" s="5">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s" s="5">
+        <v>76</v>
+      </c>
+      <c r="E34" s="5">
         <v>50</v>
-      </c>
-      <c r="D34" t="s" s="5">
-        <v>108</v>
-      </c>
-      <c r="E34" s="5">
-        <v>100</v>
       </c>
       <c r="F34" s="5">
         <v>0</v>
       </c>
       <c r="G34" t="s" s="5">
-        <v>109</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
@@ -8671,22 +8671,22 @@
         <v>33</v>
       </c>
       <c r="B35" s="5">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C35" s="5">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s" s="5">
+        <v>79</v>
+      </c>
+      <c r="E35" s="5">
         <v>50</v>
-      </c>
-      <c r="D35" t="s" s="5">
-        <v>112</v>
-      </c>
-      <c r="E35" s="5">
-        <v>100</v>
       </c>
       <c r="F35" s="5">
         <v>0</v>
       </c>
       <c r="G35" t="s" s="5">
-        <v>113</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
@@ -8694,22 +8694,22 @@
         <v>34</v>
       </c>
       <c r="B36" s="5">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C36" s="5">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s" s="5">
+        <v>82</v>
+      </c>
+      <c r="E36" s="5">
         <v>50</v>
-      </c>
-      <c r="D36" t="s" s="5">
-        <v>116</v>
-      </c>
-      <c r="E36" s="5">
-        <v>100</v>
       </c>
       <c r="F36" s="5">
         <v>0</v>
       </c>
       <c r="G36" t="s" s="5">
-        <v>117</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
@@ -8717,22 +8717,22 @@
         <v>35</v>
       </c>
       <c r="B37" s="5">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C37" s="5">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s" s="5">
+        <v>85</v>
+      </c>
+      <c r="E37" s="5">
         <v>50</v>
-      </c>
-      <c r="D37" t="s" s="5">
-        <v>120</v>
-      </c>
-      <c r="E37" s="5">
-        <v>100</v>
       </c>
       <c r="F37" s="5">
         <v>0</v>
       </c>
       <c r="G37" t="s" s="5">
-        <v>121</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
@@ -8740,119 +8740,119 @@
         <v>36</v>
       </c>
       <c r="B38" s="5">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C38" s="5">
+        <v>30</v>
+      </c>
+      <c r="D38" t="s" s="5">
+        <v>88</v>
+      </c>
+      <c r="E38" s="5">
         <v>50</v>
-      </c>
-      <c r="D38" t="s" s="5">
-        <v>124</v>
-      </c>
-      <c r="E38" s="5">
-        <v>100</v>
       </c>
       <c r="F38" s="5">
         <v>0</v>
       </c>
       <c r="G38" t="s" s="5">
-        <v>125</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="3">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B39" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C39" s="5">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="D39" t="s" s="5">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="E39" s="5">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="F39" s="5">
         <v>0</v>
       </c>
       <c r="G39" t="s" s="5">
-        <v>129</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="3">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B40" s="5">
         <v>1</v>
       </c>
       <c r="C40" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s" s="5">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="E40" s="5">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="F40" s="5">
         <v>0</v>
       </c>
       <c r="G40" t="s" s="5">
-        <v>133</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="3">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B41" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C41" s="5">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="D41" t="s" s="5">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="E41" s="5">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="F41" s="5">
         <v>0</v>
       </c>
       <c r="G41" t="s" s="5">
-        <v>147</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B42" s="5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C42" s="5">
         <v>50</v>
       </c>
       <c r="D42" t="s" s="5">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="E42" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F42" s="5">
         <v>0</v>
       </c>
       <c r="G42" t="s" s="5">
-        <v>151</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="3">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B43" s="5">
         <v>1</v>
@@ -8861,21 +8861,21 @@
         <v>50</v>
       </c>
       <c r="D43" t="s" s="5">
-        <v>163</v>
+        <v>104</v>
       </c>
       <c r="E43" s="5">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="F43" s="5">
         <v>0</v>
       </c>
       <c r="G43" t="s" s="5">
-        <v>164</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="3">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
@@ -8884,205 +8884,205 @@
         <v>50</v>
       </c>
       <c r="D44" t="s" s="5">
-        <v>167</v>
+        <v>108</v>
       </c>
       <c r="E44" s="5">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="F44" s="5">
         <v>0</v>
       </c>
       <c r="G44" t="s" s="5">
-        <v>168</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="3">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B45" s="5">
         <v>1</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="5">
         <v>50</v>
       </c>
       <c r="D45" t="s" s="5">
-        <v>171</v>
+        <v>112</v>
       </c>
       <c r="E45" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F45" s="5">
         <v>0</v>
       </c>
       <c r="G45" t="s" s="5">
-        <v>172</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="3">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B46" s="5">
         <v>1</v>
       </c>
-      <c r="C46" s="12">
+      <c r="C46" s="5">
         <v>50</v>
       </c>
       <c r="D46" t="s" s="5">
-        <v>174</v>
+        <v>116</v>
       </c>
       <c r="E46" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F46" s="5">
         <v>0</v>
       </c>
       <c r="G46" t="s" s="5">
-        <v>175</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="3">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B47" s="5">
         <v>1</v>
       </c>
-      <c r="C47" s="12">
+      <c r="C47" s="5">
         <v>50</v>
       </c>
       <c r="D47" t="s" s="5">
-        <v>177</v>
+        <v>120</v>
       </c>
       <c r="E47" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F47" s="5">
         <v>0</v>
       </c>
       <c r="G47" t="s" s="5">
-        <v>178</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="3">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B48" s="5">
         <v>1</v>
       </c>
-      <c r="C48" s="12">
+      <c r="C48" s="5">
         <v>50</v>
       </c>
       <c r="D48" t="s" s="5">
-        <v>180</v>
+        <v>124</v>
       </c>
       <c r="E48" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F48" s="5">
         <v>0</v>
       </c>
       <c r="G48" t="s" s="5">
-        <v>181</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="3">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B49" s="5">
-        <v>1</v>
-      </c>
-      <c r="C49" s="12">
+        <v>20</v>
+      </c>
+      <c r="C49" s="5">
         <v>50</v>
       </c>
       <c r="D49" t="s" s="5">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="E49" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F49" s="5">
         <v>0</v>
       </c>
       <c r="G49" t="s" s="5">
-        <v>185</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="3">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B50" s="5">
         <v>1</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="5">
         <v>50</v>
       </c>
       <c r="D50" t="s" s="5">
-        <v>197</v>
+        <v>132</v>
       </c>
       <c r="E50" s="5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F50" s="5">
         <v>0</v>
       </c>
       <c r="G50" t="s" s="5">
-        <v>199</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="3">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B51" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C51" s="5">
         <v>50</v>
       </c>
       <c r="D51" t="s" s="5">
-        <v>201</v>
+        <v>145</v>
       </c>
       <c r="E51" s="5">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F51" s="5">
         <v>0</v>
       </c>
       <c r="G51" t="s" s="5">
-        <v>202</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B52" s="5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C52" s="5">
         <v>50</v>
       </c>
       <c r="D52" t="s" s="5">
-        <v>204</v>
+        <v>150</v>
       </c>
       <c r="E52" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F52" s="5">
         <v>0</v>
       </c>
       <c r="G52" t="s" s="5">
-        <v>205</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="3">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B53" s="5">
         <v>1</v>
@@ -9091,21 +9091,21 @@
         <v>50</v>
       </c>
       <c r="D53" t="s" s="5">
-        <v>207</v>
+        <v>163</v>
       </c>
       <c r="E53" s="5">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="F53" s="5">
         <v>0</v>
       </c>
       <c r="G53" t="s" s="5">
-        <v>208</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
       <c r="A54" s="3">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B54" s="5">
         <v>1</v>
@@ -9114,168 +9114,168 @@
         <v>50</v>
       </c>
       <c r="D54" t="s" s="5">
-        <v>210</v>
+        <v>167</v>
       </c>
       <c r="E54" s="5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F54" s="5">
         <v>0</v>
       </c>
       <c r="G54" t="s" s="5">
-        <v>211</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" s="3">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B55" s="5">
         <v>1</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C55" s="10">
         <v>50</v>
       </c>
-      <c r="D55" t="s" s="10">
-        <v>213</v>
+      <c r="D55" t="s" s="5">
+        <v>171</v>
       </c>
       <c r="E55" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F55" s="5">
         <v>0</v>
       </c>
       <c r="G55" t="s" s="5">
-        <v>214</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" s="3">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B56" s="5">
-        <v>30</v>
-      </c>
-      <c r="C56" s="5">
+        <v>1</v>
+      </c>
+      <c r="C56" s="12">
         <v>50</v>
       </c>
-      <c r="D56" t="s" s="11">
-        <v>216</v>
+      <c r="D56" t="s" s="5">
+        <v>174</v>
       </c>
       <c r="E56" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F56" s="5">
         <v>0</v>
       </c>
       <c r="G56" t="s" s="5">
-        <v>217</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" s="3">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B57" s="5">
         <v>1</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C57" s="12">
         <v>50</v>
       </c>
       <c r="D57" t="s" s="5">
-        <v>219</v>
+        <v>177</v>
       </c>
       <c r="E57" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F57" s="5">
         <v>0</v>
       </c>
       <c r="G57" t="s" s="5">
-        <v>220</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" s="3">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B58" s="5">
         <v>1</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C58" s="12">
         <v>50</v>
       </c>
       <c r="D58" t="s" s="5">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="E58" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F58" s="5">
         <v>0</v>
       </c>
       <c r="G58" t="s" s="5">
-        <v>223</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" s="3">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B59" s="5">
-        <v>20</v>
-      </c>
-      <c r="C59" s="5">
+        <v>1</v>
+      </c>
+      <c r="C59" s="12">
         <v>50</v>
       </c>
       <c r="D59" t="s" s="5">
-        <v>226</v>
+        <v>184</v>
       </c>
       <c r="E59" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F59" s="5">
         <v>0</v>
       </c>
       <c r="G59" t="s" s="5">
-        <v>227</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" s="3">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B60" s="5">
         <v>1</v>
       </c>
-      <c r="C60" s="5">
-        <v>10</v>
+      <c r="C60" s="11">
+        <v>50</v>
       </c>
       <c r="D60" t="s" s="5">
-        <v>371</v>
+        <v>197</v>
       </c>
       <c r="E60" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F60" s="5">
         <v>0</v>
       </c>
       <c r="G60" t="s" s="5">
-        <v>373</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" s="3">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B61" s="5">
         <v>1</v>
       </c>
       <c r="C61" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D61" t="s" s="5">
-        <v>375</v>
+        <v>201</v>
       </c>
       <c r="E61" s="5">
         <v>100</v>
@@ -9284,21 +9284,21 @@
         <v>0</v>
       </c>
       <c r="G61" t="s" s="5">
-        <v>376</v>
+        <v>202</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" s="3">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B62" s="5">
         <v>1</v>
       </c>
       <c r="C62" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D62" t="s" s="5">
-        <v>378</v>
+        <v>204</v>
       </c>
       <c r="E62" s="5">
         <v>100</v>
@@ -9307,150 +9307,150 @@
         <v>0</v>
       </c>
       <c r="G62" t="s" s="5">
-        <v>379</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" s="3">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B63" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C63" s="5">
         <v>50</v>
       </c>
       <c r="D63" t="s" s="5">
-        <v>381</v>
+        <v>207</v>
       </c>
       <c r="E63" s="5">
         <v>100</v>
       </c>
       <c r="F63" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63" t="s" s="5">
-        <v>382</v>
+        <v>208</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
       <c r="A64" s="3">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B64" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C64" s="5">
         <v>50</v>
       </c>
       <c r="D64" t="s" s="5">
-        <v>384</v>
+        <v>210</v>
       </c>
       <c r="E64" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F64" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" t="s" s="5">
-        <v>385</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" s="3">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B65" s="5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C65" s="5">
         <v>50</v>
       </c>
-      <c r="D65" t="s" s="5">
-        <v>387</v>
+      <c r="D65" t="s" s="10">
+        <v>213</v>
       </c>
       <c r="E65" s="5">
         <v>0</v>
       </c>
       <c r="F65" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" t="s" s="5">
-        <v>388</v>
+        <v>214</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" s="3">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B66" s="5">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C66" s="5">
-        <v>15</v>
-      </c>
-      <c r="D66" t="s" s="5">
-        <v>391</v>
+        <v>50</v>
+      </c>
+      <c r="D66" t="s" s="11">
+        <v>216</v>
       </c>
       <c r="E66" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F66" s="5">
         <v>0</v>
       </c>
       <c r="G66" t="s" s="5">
-        <v>392</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
       <c r="A67" s="3">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B67" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C67" s="5">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D67" t="s" s="5">
-        <v>394</v>
+        <v>219</v>
       </c>
       <c r="E67" s="5">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="F67" s="5">
         <v>0</v>
       </c>
       <c r="G67" t="s" s="5">
-        <v>395</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" ht="20" customHeight="1">
       <c r="A68" s="3">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B68" s="5">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C68" s="5">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D68" t="s" s="5">
-        <v>397</v>
+        <v>222</v>
       </c>
       <c r="E68" s="5">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F68" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" t="s" s="5">
-        <v>398</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
       <c r="A69" s="3">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B69" s="5">
         <v>20</v>
@@ -9459,90 +9459,90 @@
         <v>50</v>
       </c>
       <c r="D69" t="s" s="5">
-        <v>400</v>
+        <v>226</v>
       </c>
       <c r="E69" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" t="s" s="5">
-        <v>401</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
       <c r="A70" s="3">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B70" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C70" s="5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D70" t="s" s="5">
-        <v>403</v>
+        <v>371</v>
       </c>
       <c r="E70" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F70" s="5">
         <v>0</v>
       </c>
       <c r="G70" t="s" s="5">
-        <v>404</v>
+        <v>373</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
       <c r="A71" s="3">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B71" s="5">
+        <v>1</v>
+      </c>
+      <c r="C71" s="5">
         <v>10</v>
       </c>
-      <c r="C71" s="5">
-        <v>30</v>
-      </c>
       <c r="D71" t="s" s="5">
-        <v>405</v>
+        <v>375</v>
       </c>
       <c r="E71" s="5">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="F71" s="5">
         <v>0</v>
       </c>
       <c r="G71" t="s" s="5">
-        <v>406</v>
+        <v>376</v>
       </c>
     </row>
     <row r="72" ht="20" customHeight="1">
       <c r="A72" s="3">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B72" s="5">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C72" s="5">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D72" t="s" s="5">
-        <v>407</v>
+        <v>378</v>
       </c>
       <c r="E72" s="5">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F72" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72" t="s" s="5">
-        <v>408</v>
+        <v>379</v>
       </c>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" s="3">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B73" s="5">
         <v>20</v>
@@ -9551,122 +9551,122 @@
         <v>50</v>
       </c>
       <c r="D73" t="s" s="5">
-        <v>409</v>
+        <v>381</v>
       </c>
       <c r="E73" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F73" s="5">
         <v>1</v>
       </c>
       <c r="G73" t="s" s="5">
-        <v>410</v>
+        <v>382</v>
       </c>
     </row>
     <row r="74" ht="20" customHeight="1">
       <c r="A74" s="3">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B74" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C74" s="5">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D74" t="s" s="5">
-        <v>411</v>
+        <v>384</v>
       </c>
       <c r="E74" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F74" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G74" t="s" s="5">
-        <v>412</v>
+        <v>385</v>
       </c>
     </row>
     <row r="75" ht="20" customHeight="1">
       <c r="A75" s="3">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B75" s="5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C75" s="5">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D75" t="s" s="5">
-        <v>413</v>
+        <v>387</v>
       </c>
       <c r="E75" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F75" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G75" t="s" s="5">
-        <v>414</v>
+        <v>388</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
       <c r="A76" s="3">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B76" s="5">
+        <v>5</v>
+      </c>
+      <c r="C76" s="5">
         <v>15</v>
       </c>
-      <c r="C76" s="5">
-        <v>40</v>
-      </c>
       <c r="D76" t="s" s="5">
-        <v>416</v>
+        <v>391</v>
       </c>
       <c r="E76" s="5">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F76" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G76" t="s" s="5">
-        <v>417</v>
+        <v>392</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
       <c r="A77" s="3">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B77" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C77" s="5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D77" t="s" s="5">
-        <v>419</v>
+        <v>394</v>
       </c>
       <c r="E77" s="5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F77" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G77" t="s" s="5">
-        <v>420</v>
+        <v>395</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" s="3">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B78" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C78" s="5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D78" t="s" s="5">
-        <v>422</v>
+        <v>397</v>
       </c>
       <c r="E78" s="5">
         <v>20</v>
@@ -9675,12 +9675,12 @@
         <v>1</v>
       </c>
       <c r="G78" t="s" s="5">
-        <v>423</v>
+        <v>398</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
       <c r="A79" s="3">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B79" s="5">
         <v>20</v>
@@ -9689,15 +9689,245 @@
         <v>50</v>
       </c>
       <c r="D79" t="s" s="5">
+        <v>400</v>
+      </c>
+      <c r="E79" s="5">
+        <v>10</v>
+      </c>
+      <c r="F79" s="5">
+        <v>1</v>
+      </c>
+      <c r="G79" t="s" s="5">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="80" ht="20" customHeight="1">
+      <c r="A80" s="3">
+        <v>68</v>
+      </c>
+      <c r="B80" s="5">
+        <v>5</v>
+      </c>
+      <c r="C80" s="5">
+        <v>15</v>
+      </c>
+      <c r="D80" t="s" s="5">
+        <v>403</v>
+      </c>
+      <c r="E80" s="5">
+        <v>50</v>
+      </c>
+      <c r="F80" s="5">
+        <v>0</v>
+      </c>
+      <c r="G80" t="s" s="5">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="81" ht="20" customHeight="1">
+      <c r="A81" s="3">
+        <v>69</v>
+      </c>
+      <c r="B81" s="5">
+        <v>10</v>
+      </c>
+      <c r="C81" s="5">
+        <v>30</v>
+      </c>
+      <c r="D81" t="s" s="5">
+        <v>405</v>
+      </c>
+      <c r="E81" s="5">
+        <v>30</v>
+      </c>
+      <c r="F81" s="5">
+        <v>0</v>
+      </c>
+      <c r="G81" t="s" s="5">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="82" ht="20" customHeight="1">
+      <c r="A82" s="3">
+        <v>70</v>
+      </c>
+      <c r="B82" s="5">
+        <v>15</v>
+      </c>
+      <c r="C82" s="5">
+        <v>40</v>
+      </c>
+      <c r="D82" t="s" s="5">
+        <v>407</v>
+      </c>
+      <c r="E82" s="5">
+        <v>20</v>
+      </c>
+      <c r="F82" s="5">
+        <v>1</v>
+      </c>
+      <c r="G82" t="s" s="5">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="83" ht="20" customHeight="1">
+      <c r="A83" s="3">
+        <v>71</v>
+      </c>
+      <c r="B83" s="5">
+        <v>20</v>
+      </c>
+      <c r="C83" s="5">
+        <v>50</v>
+      </c>
+      <c r="D83" t="s" s="5">
+        <v>409</v>
+      </c>
+      <c r="E83" s="5">
+        <v>10</v>
+      </c>
+      <c r="F83" s="5">
+        <v>1</v>
+      </c>
+      <c r="G83" t="s" s="5">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="84" ht="20" customHeight="1">
+      <c r="A84" s="3">
+        <v>72</v>
+      </c>
+      <c r="B84" s="5">
+        <v>5</v>
+      </c>
+      <c r="C84" s="5">
+        <v>15</v>
+      </c>
+      <c r="D84" t="s" s="5">
+        <v>411</v>
+      </c>
+      <c r="E84" s="5">
+        <v>50</v>
+      </c>
+      <c r="F84" s="5">
+        <v>0</v>
+      </c>
+      <c r="G84" t="s" s="5">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="85" ht="20" customHeight="1">
+      <c r="A85" s="3">
+        <v>73</v>
+      </c>
+      <c r="B85" s="5">
+        <v>10</v>
+      </c>
+      <c r="C85" s="5">
+        <v>30</v>
+      </c>
+      <c r="D85" t="s" s="5">
+        <v>413</v>
+      </c>
+      <c r="E85" s="5">
+        <v>30</v>
+      </c>
+      <c r="F85" s="5">
+        <v>0</v>
+      </c>
+      <c r="G85" t="s" s="5">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="86" ht="20" customHeight="1">
+      <c r="A86" s="3">
+        <v>74</v>
+      </c>
+      <c r="B86" s="5">
+        <v>15</v>
+      </c>
+      <c r="C86" s="5">
+        <v>40</v>
+      </c>
+      <c r="D86" t="s" s="5">
+        <v>416</v>
+      </c>
+      <c r="E86" s="5">
+        <v>20</v>
+      </c>
+      <c r="F86" s="5">
+        <v>1</v>
+      </c>
+      <c r="G86" t="s" s="5">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="87" ht="20" customHeight="1">
+      <c r="A87" s="3">
+        <v>75</v>
+      </c>
+      <c r="B87" s="5">
+        <v>20</v>
+      </c>
+      <c r="C87" s="5">
+        <v>50</v>
+      </c>
+      <c r="D87" t="s" s="5">
+        <v>419</v>
+      </c>
+      <c r="E87" s="5">
+        <v>10</v>
+      </c>
+      <c r="F87" s="5">
+        <v>1</v>
+      </c>
+      <c r="G87" t="s" s="5">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="88" ht="20" customHeight="1">
+      <c r="A88" s="3">
+        <v>76</v>
+      </c>
+      <c r="B88" s="5">
+        <v>10</v>
+      </c>
+      <c r="C88" s="5">
+        <v>50</v>
+      </c>
+      <c r="D88" t="s" s="5">
+        <v>422</v>
+      </c>
+      <c r="E88" s="5">
+        <v>20</v>
+      </c>
+      <c r="F88" s="5">
+        <v>1</v>
+      </c>
+      <c r="G88" t="s" s="5">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="89" ht="20" customHeight="1">
+      <c r="A89" s="3">
+        <v>77</v>
+      </c>
+      <c r="B89" s="5">
+        <v>20</v>
+      </c>
+      <c r="C89" s="5">
+        <v>50</v>
+      </c>
+      <c r="D89" t="s" s="5">
         <v>425</v>
       </c>
-      <c r="E79" s="5">
+      <c r="E89" s="5">
         <v>20</v>
       </c>
-      <c r="F79" s="5">
-        <v>1</v>
-      </c>
-      <c r="G79" t="s" s="5">
+      <c r="F89" s="5">
+        <v>1</v>
+      </c>
+      <c r="G89" t="s" s="5">
         <v>426</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed #637 FlixelRL-637 毒の杖が強すぎる
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="435">
   <si>
     <t>id</t>
   </si>
@@ -1255,13 +1255,16 @@
     <t>HP増加の指輪+1</t>
   </si>
   <si>
+    <t>最大HPが20上昇します</t>
+  </si>
+  <si>
     <t>RING16</t>
   </si>
   <si>
     <t>HP増加の指輪+2</t>
   </si>
   <si>
-    <t>最大HPが20上昇します</t>
+    <t>最大HPが30上昇します</t>
   </si>
   <si>
     <t>RING17</t>
@@ -1270,7 +1273,7 @@
     <t>HP増加の指輪+3</t>
   </si>
   <si>
-    <t>最大HPが30上昇します</t>
+    <t>最大HPが40上昇します</t>
   </si>
   <si>
     <t>RING18</t>
@@ -1279,7 +1282,7 @@
     <t>HP増加の指輪+4</t>
   </si>
   <si>
-    <t>最大HPが40上昇します</t>
+    <t>最大HPが50上昇します</t>
   </si>
   <si>
     <t>RING19</t>
@@ -3445,11 +3448,11 @@
       <c r="H20" s="6"/>
       <c r="I20" s="7"/>
       <c r="J20" s="6">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="K20" s="6">
         <f>J20*0.35</f>
-        <v>10.5</v>
+        <v>17.5</v>
       </c>
       <c r="L20" s="6">
         <v>201</v>
@@ -3479,11 +3482,11 @@
       <c r="H21" s="6"/>
       <c r="I21" s="7"/>
       <c r="J21" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="K21" s="6">
         <f>J21*0.35</f>
-        <v>17.5</v>
+        <v>35</v>
       </c>
       <c r="L21" s="6">
         <v>202</v>
@@ -3513,11 +3516,11 @@
       <c r="H22" s="6"/>
       <c r="I22" s="7"/>
       <c r="J22" s="6">
-        <v>70</v>
+        <v>250</v>
       </c>
       <c r="K22" s="6">
         <f>J22*0.35</f>
-        <v>24.5</v>
+        <v>87.5</v>
       </c>
       <c r="L22" s="6">
         <v>203</v>
@@ -3547,11 +3550,11 @@
       <c r="H23" s="6"/>
       <c r="I23" s="7"/>
       <c r="J23" s="6">
-        <v>90</v>
+        <v>500</v>
       </c>
       <c r="K23" s="6">
         <f>J23*0.35</f>
-        <v>31.5</v>
+        <v>175</v>
       </c>
       <c r="L23" s="6">
         <v>204</v>
@@ -3581,11 +3584,11 @@
       <c r="H24" s="6"/>
       <c r="I24" s="7"/>
       <c r="J24" s="6">
-        <v>110</v>
+        <v>750</v>
       </c>
       <c r="K24" s="6">
         <f>J24*0.35</f>
-        <v>38.5</v>
+        <v>262.5</v>
       </c>
       <c r="L24" s="6">
         <v>205</v>
@@ -3615,11 +3618,11 @@
       <c r="H25" s="6"/>
       <c r="I25" s="7"/>
       <c r="J25" s="6">
-        <v>130</v>
+        <v>1000</v>
       </c>
       <c r="K25" s="6">
         <f>J25*0.35</f>
-        <v>45.5</v>
+        <v>350</v>
       </c>
       <c r="L25" s="6">
         <v>206</v>
@@ -3649,11 +3652,11 @@
       <c r="H26" s="6"/>
       <c r="I26" s="7"/>
       <c r="J26" s="6">
-        <v>150</v>
+        <v>1200</v>
       </c>
       <c r="K26" s="6">
         <f>J26*0.35</f>
-        <v>52.5</v>
+        <v>420</v>
       </c>
       <c r="L26" s="6">
         <v>207</v>
@@ -3683,11 +3686,11 @@
       <c r="H27" s="6"/>
       <c r="I27" s="7"/>
       <c r="J27" s="6">
-        <v>170</v>
+        <v>1400</v>
       </c>
       <c r="K27" s="6">
         <f>J27*0.35</f>
-        <v>59.49999999999999</v>
+        <v>489.9999999999999</v>
       </c>
       <c r="L27" s="6">
         <v>208</v>
@@ -3717,11 +3720,11 @@
       <c r="H28" s="6"/>
       <c r="I28" s="7"/>
       <c r="J28" s="6">
-        <v>200</v>
+        <v>1600</v>
       </c>
       <c r="K28" s="6">
         <f>J28*0.35</f>
-        <v>70</v>
+        <v>560</v>
       </c>
       <c r="L28" s="6">
         <v>209</v>
@@ -3751,11 +3754,11 @@
       <c r="H29" s="6"/>
       <c r="I29" s="7"/>
       <c r="J29" s="6">
-        <v>250</v>
+        <v>1800</v>
       </c>
       <c r="K29" s="6">
         <f>J29*0.35</f>
-        <v>87.5</v>
+        <v>630</v>
       </c>
       <c r="L29" s="6">
         <v>210</v>
@@ -3785,11 +3788,11 @@
       <c r="H30" s="6"/>
       <c r="I30" s="7"/>
       <c r="J30" s="6">
-        <v>300</v>
+        <v>2000</v>
       </c>
       <c r="K30" s="6">
         <f>J30*0.35</f>
-        <v>105</v>
+        <v>700</v>
       </c>
       <c r="L30" s="6">
         <v>211</v>
@@ -3819,11 +3822,11 @@
       <c r="H31" s="6"/>
       <c r="I31" s="7"/>
       <c r="J31" s="6">
-        <v>350</v>
+        <v>2200</v>
       </c>
       <c r="K31" s="6">
         <f>J31*0.35</f>
-        <v>122.5</v>
+        <v>770</v>
       </c>
       <c r="L31" s="6">
         <v>212</v>
@@ -3853,11 +3856,11 @@
       <c r="H32" s="6"/>
       <c r="I32" s="7"/>
       <c r="J32" s="6">
-        <v>500</v>
+        <v>2400</v>
       </c>
       <c r="K32" s="6">
         <f>J32*0.35</f>
-        <v>175</v>
+        <v>840</v>
       </c>
       <c r="L32" s="6">
         <v>213</v>
@@ -3887,11 +3890,11 @@
       <c r="H33" s="6"/>
       <c r="I33" s="7"/>
       <c r="J33" s="6">
-        <v>600</v>
+        <v>2600</v>
       </c>
       <c r="K33" s="6">
         <f>J33*0.35</f>
-        <v>210</v>
+        <v>909.9999999999999</v>
       </c>
       <c r="L33" s="6">
         <v>214</v>
@@ -3921,11 +3924,11 @@
       <c r="H34" s="6"/>
       <c r="I34" s="7"/>
       <c r="J34" s="6">
-        <v>700</v>
+        <v>2800</v>
       </c>
       <c r="K34" s="6">
         <f>J34*0.35</f>
-        <v>245</v>
+        <v>979.9999999999999</v>
       </c>
       <c r="L34" s="6">
         <v>215</v>
@@ -5027,11 +5030,11 @@
       </c>
       <c r="I67" s="7"/>
       <c r="J67" s="6">
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="K67" s="6">
         <f>J67*0.35</f>
-        <v>315</v>
+        <v>1050</v>
       </c>
       <c r="L67" s="6">
         <v>248</v>
@@ -5091,11 +5094,11 @@
       </c>
       <c r="I69" s="7"/>
       <c r="J69" s="6">
-        <v>900</v>
+        <v>2000</v>
       </c>
       <c r="K69" s="6">
         <f>J69*0.35</f>
-        <v>315</v>
+        <v>700</v>
       </c>
       <c r="L69" s="6">
         <v>250</v>
@@ -5251,11 +5254,11 @@
       </c>
       <c r="I74" s="7"/>
       <c r="J74" s="6">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="K74" s="6">
         <f>J74*0.35</f>
-        <v>315</v>
+        <v>525</v>
       </c>
       <c r="L74" s="6">
         <v>255</v>
@@ -7675,18 +7678,18 @@
         <v>154</v>
       </c>
       <c r="M57" t="s" s="5">
-        <v>380</v>
+        <v>413</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
       <c r="A58" t="s" s="3">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B58" t="s" s="5">
         <v>372</v>
       </c>
       <c r="C58" t="s" s="5">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="7"/>
@@ -7709,18 +7712,18 @@
         <v>155</v>
       </c>
       <c r="M58" t="s" s="5">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B59" t="s" s="5">
         <v>372</v>
       </c>
       <c r="C59" t="s" s="5">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="7"/>
@@ -7743,18 +7746,18 @@
         <v>156</v>
       </c>
       <c r="M59" t="s" s="5">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B60" t="s" s="5">
         <v>372</v>
       </c>
       <c r="C60" t="s" s="5">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="7"/>
@@ -7777,18 +7780,18 @@
         <v>157</v>
       </c>
       <c r="M60" t="s" s="5">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
       <c r="A61" t="s" s="3">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B61" t="s" s="5">
         <v>372</v>
       </c>
       <c r="C61" t="s" s="5">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D61" s="6">
         <v>1</v>
@@ -7815,18 +7818,18 @@
         <v>158</v>
       </c>
       <c r="M61" t="s" s="5">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
       <c r="A62" t="s" s="3">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B62" t="s" s="5">
         <v>372</v>
       </c>
       <c r="C62" t="s" s="5">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D62" s="6">
         <v>3</v>
@@ -7851,7 +7854,7 @@
         <v>159</v>
       </c>
       <c r="M62" t="s" s="5">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -7889,22 +7892,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -8841,7 +8844,7 @@
         <v>101</v>
       </c>
       <c r="E42" s="5">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="F42" s="5">
         <v>0</v>
@@ -8887,7 +8890,7 @@
         <v>108</v>
       </c>
       <c r="E44" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F44" s="5">
         <v>0</v>
@@ -8933,7 +8936,7 @@
         <v>116</v>
       </c>
       <c r="E46" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F46" s="5">
         <v>0</v>
@@ -8993,7 +8996,7 @@
         <v>37</v>
       </c>
       <c r="B49" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C49" s="5">
         <v>50</v>
@@ -9002,7 +9005,7 @@
         <v>128</v>
       </c>
       <c r="E49" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F49" s="5">
         <v>0</v>
@@ -9025,7 +9028,7 @@
         <v>132</v>
       </c>
       <c r="E50" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F50" s="5">
         <v>0</v>
@@ -9039,7 +9042,7 @@
         <v>39</v>
       </c>
       <c r="B51" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C51" s="5">
         <v>50</v>
@@ -9062,7 +9065,7 @@
         <v>40</v>
       </c>
       <c r="B52" s="5">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C52" s="5">
         <v>50</v>
@@ -9209,7 +9212,7 @@
         <v>180</v>
       </c>
       <c r="E58" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F58" s="5">
         <v>0</v>
@@ -9232,7 +9235,7 @@
         <v>184</v>
       </c>
       <c r="E59" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F59" s="5">
         <v>0</v>
@@ -9255,7 +9258,7 @@
         <v>197</v>
       </c>
       <c r="E60" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="F60" s="5">
         <v>0</v>
@@ -9301,7 +9304,7 @@
         <v>204</v>
       </c>
       <c r="E62" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F62" s="5">
         <v>0</v>
@@ -9384,7 +9387,7 @@
         <v>54</v>
       </c>
       <c r="B66" s="5">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C66" s="5">
         <v>50</v>
@@ -9416,7 +9419,7 @@
         <v>219</v>
       </c>
       <c r="E67" s="5">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="F67" s="5">
         <v>0</v>
@@ -9453,7 +9456,7 @@
         <v>57</v>
       </c>
       <c r="B69" s="5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C69" s="5">
         <v>50</v>
@@ -9545,7 +9548,7 @@
         <v>61</v>
       </c>
       <c r="B73" s="5">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C73" s="5">
         <v>50</v>
@@ -9568,7 +9571,7 @@
         <v>62</v>
       </c>
       <c r="B74" s="5">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C74" s="5">
         <v>50</v>
@@ -9591,7 +9594,7 @@
         <v>63</v>
       </c>
       <c r="B75" s="5">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C75" s="5">
         <v>50</v>
@@ -9827,7 +9830,7 @@
         <v>30</v>
       </c>
       <c r="D85" t="s" s="5">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E85" s="5">
         <v>30</v>
@@ -9836,7 +9839,7 @@
         <v>0</v>
       </c>
       <c r="G85" t="s" s="5">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="86" ht="20" customHeight="1">
@@ -9850,7 +9853,7 @@
         <v>40</v>
       </c>
       <c r="D86" t="s" s="5">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E86" s="5">
         <v>20</v>
@@ -9859,7 +9862,7 @@
         <v>1</v>
       </c>
       <c r="G86" t="s" s="5">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="87" ht="20" customHeight="1">
@@ -9873,7 +9876,7 @@
         <v>50</v>
       </c>
       <c r="D87" t="s" s="5">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E87" s="5">
         <v>10</v>
@@ -9882,7 +9885,7 @@
         <v>1</v>
       </c>
       <c r="G87" t="s" s="5">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="88" ht="20" customHeight="1">
@@ -9896,7 +9899,7 @@
         <v>50</v>
       </c>
       <c r="D88" t="s" s="5">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E88" s="5">
         <v>20</v>
@@ -9905,7 +9908,7 @@
         <v>1</v>
       </c>
       <c r="G88" t="s" s="5">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="89" ht="20" customHeight="1">
@@ -9919,7 +9922,7 @@
         <v>50</v>
       </c>
       <c r="D89" t="s" s="5">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E89" s="5">
         <v>20</v>
@@ -9928,7 +9931,7 @@
         <v>1</v>
       </c>
       <c r="G89" t="s" s="5">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #601 FlixelRL-601 強化の巻物のSEがない
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -4542,11 +4542,11 @@
       <c r="H52" s="6"/>
       <c r="I52" s="7"/>
       <c r="J52" s="6">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="K52" s="6">
         <f>J52*0.35</f>
-        <v>350</v>
+        <v>525</v>
       </c>
       <c r="L52" s="6">
         <v>233</v>
@@ -4568,7 +4568,7 @@
       <c r="D53" s="7"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G53" t="s" s="5">
         <v>148</v>

</xml_diff>